<commit_message>
AE-365 add template for swedish energiatodistus with with api support for generating it
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,23 +19,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'1) etusivu'!$A$1:$Q$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$J$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$H$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$A$1:$Q$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$66</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$I$62</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="214">
   <si>
     <t xml:space="preserve">ENERGIATODISTUS 2018</t>
   </si>
@@ -83,7 +83,7 @@
     <t xml:space="preserve">☐ Olemassa olevalle rakennukselle, havainnointikäynnin päivämäärä:</t>
   </si>
   <si>
-    <t xml:space="preserve">Energiatehokkuusluokka </t>
+    <t xml:space="preserve">    Energiatehokkuusluokka </t>
   </si>
   <si>
     <t xml:space="preserve">Rakennuksen laskennallinen
@@ -881,9 +881,6 @@
   </si>
   <si>
     <t xml:space="preserve">kpl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kWh</t>
   </si>
   <si>
     <t xml:space="preserve">Varaava tulisija</t>
@@ -2412,7 +2409,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -6444,9 +6441,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>240120</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>254520</xdr:rowOff>
+      <xdr:rowOff>254160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6460,7 +6457,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4656960"/>
-          <a:ext cx="750240" cy="207000"/>
+          <a:ext cx="749880" cy="206640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6481,9 +6478,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>140040</xdr:colOff>
+      <xdr:colOff>139680</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>254520</xdr:rowOff>
+      <xdr:rowOff>254160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6497,7 +6494,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4971240"/>
-          <a:ext cx="1093680" cy="207000"/>
+          <a:ext cx="1093320" cy="206640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6518,9 +6515,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>13320</xdr:colOff>
+      <xdr:colOff>12960</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>254520</xdr:rowOff>
+      <xdr:rowOff>254160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6534,7 +6531,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5285520"/>
-          <a:ext cx="1400400" cy="207000"/>
+          <a:ext cx="1400040" cy="206640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6555,9 +6552,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>337320</xdr:colOff>
+      <xdr:colOff>336960</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>254520</xdr:rowOff>
+      <xdr:rowOff>254160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6571,7 +6568,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5599800"/>
-          <a:ext cx="1724400" cy="207000"/>
+          <a:ext cx="1724040" cy="206640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6592,9 +6589,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>210600</xdr:colOff>
+      <xdr:colOff>210240</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>267480</xdr:rowOff>
+      <xdr:rowOff>267120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6608,7 +6605,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5909760"/>
-          <a:ext cx="2031480" cy="219960"/>
+          <a:ext cx="2031120" cy="219600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6629,9 +6626,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>153720</xdr:colOff>
+      <xdr:colOff>153360</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>254520</xdr:rowOff>
+      <xdr:rowOff>254160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6645,7 +6642,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6219720"/>
-          <a:ext cx="2367720" cy="207000"/>
+          <a:ext cx="2367360" cy="206640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6666,9 +6663,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>93960</xdr:colOff>
+      <xdr:colOff>93600</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>254520</xdr:rowOff>
+      <xdr:rowOff>254160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6678,7 +6675,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6530400"/>
-          <a:ext cx="2680560" cy="205920"/>
+          <a:ext cx="2680200" cy="205560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7047,9 +7044,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>293400</xdr:colOff>
+      <xdr:colOff>293040</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7059,7 +7056,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="149400" y="78480"/>
-          <a:ext cx="6979680" cy="10549440"/>
+          <a:ext cx="6979320" cy="10549080"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7188,8 +7185,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R31" activeCellId="0" sqref="R31"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O25" activeCellId="0" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7958,10 +7955,10 @@
       <c r="H24" s="44"/>
       <c r="I24" s="44"/>
       <c r="J24" s="44"/>
-      <c r="K24" s="45" t="s">
+      <c r="K24" s="0"/>
+      <c r="L24" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="L24" s="0"/>
       <c r="M24" s="44"/>
       <c r="N24" s="46"/>
       <c r="O24" s="47"/>
@@ -8631,7 +8628,7 @@
     <mergeCell ref="B50:I50"/>
     <mergeCell ref="K50:M50"/>
   </mergeCells>
-  <conditionalFormatting sqref="F24:K24 B25:H31 B24 E32:H32 B32 B4:J4 B5:K5 B33:H34 B6:J6 I14 B23:H23 B37:G37 B15 H12 Q52:Q1048576 P14:P15 B38:C40 D52:H65223 B52:C1048576 L52:P65223 I53:K1048576 B50 J49:K50 L35 B35:D35 B36:C36 Q4 B2:K2 M2:HQ2 L4:P6 R3:HN3 B48:C49 D48:K48 L48:M49 B3 Q3 P8:P11 B7:B11 Q5:Q9 R4:HQ9 D39:P40 I23:P23 R52:HQ1048576 O38:P38 N37:P37 O35:P36 B21:B22 H16:H18 B17:B18 B42:P42 B43:B44 N48:P51 Q13:HQ51 I52 B51:M51 I25:P34 M24:P24">
+  <conditionalFormatting sqref="F24:J24 B25:H31 B24 E32:H32 B32 B4:J4 B5:K5 B33:H34 B6:J6 I14 B23:H23 B37:G37 B15 H12 Q52:Q1048576 P14:P15 B38:C40 D52:H65223 B52:C1048576 L52:P65223 I53:K1048576 B50 J49:K50 L35 B35:D35 B36:C36 Q4 B2:K2 M2:HQ2 L4:P6 R3:HN3 B48:C49 D48:K48 L48:M49 B3 Q3 P8:P11 B7:B11 Q5:Q9 R4:HQ9 D39:P40 I23:P23 R52:HQ1048576 O38:P38 N37:P37 O35:P36 B21:B22 H16:H18 B17:B18 B42:P42 B43:B44 N48:P51 Q13:HQ51 I52 B51:M51 I25:P34 L24:P24">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"*"</formula>
     </cfRule>
@@ -10689,8 +10686,8 @@
   </sheetPr>
   <dimension ref="B2:AMJ67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B66" activeCellId="0" sqref="B66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I60" activeCellId="0" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11332,7 +11329,7 @@
         <v>109</v>
       </c>
       <c r="E49" s="185" t="s">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="F49" s="231"/>
       <c r="G49" s="200"/>
@@ -11340,7 +11337,7 @@
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="167"/>
       <c r="C50" s="168" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D50" s="207"/>
       <c r="E50" s="207"/>
@@ -11350,7 +11347,7 @@
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="167"/>
       <c r="C51" s="168" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D51" s="207"/>
       <c r="E51" s="207"/>
@@ -11360,7 +11357,7 @@
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="164"/>
       <c r="C52" s="165" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D52" s="166"/>
       <c r="E52" s="166"/>
@@ -11371,7 +11368,7 @@
       <c r="B53" s="167"/>
       <c r="C53" s="182"/>
       <c r="D53" s="232" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E53" s="203"/>
       <c r="F53" s="203"/>
@@ -11390,7 +11387,7 @@
     <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="167"/>
       <c r="C55" s="168" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D55" s="196"/>
       <c r="E55" s="234"/>
@@ -11400,7 +11397,7 @@
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="164"/>
       <c r="C56" s="165" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D56" s="166"/>
       <c r="E56" s="166"/>
@@ -11411,10 +11408,10 @@
       <c r="B57" s="167"/>
       <c r="C57" s="199"/>
       <c r="D57" s="235" t="s">
+        <v>115</v>
+      </c>
+      <c r="E57" s="236" t="s">
         <v>116</v>
-      </c>
-      <c r="E57" s="236" t="s">
-        <v>117</v>
       </c>
       <c r="F57" s="199"/>
       <c r="G57" s="200"/>
@@ -11423,7 +11420,7 @@
       <c r="B58" s="167"/>
       <c r="C58" s="182"/>
       <c r="D58" s="237" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E58" s="185" t="s">
         <v>31</v>
@@ -11434,7 +11431,7 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="167"/>
       <c r="C59" s="168" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D59" s="238"/>
       <c r="E59" s="239"/>
@@ -11444,7 +11441,7 @@
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="164"/>
       <c r="C60" s="165" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D60" s="166"/>
       <c r="E60" s="166"/>
@@ -11455,16 +11452,16 @@
       <c r="B61" s="167"/>
       <c r="C61" s="182"/>
       <c r="D61" s="192" t="s">
+        <v>119</v>
+      </c>
+      <c r="E61" s="192" t="s">
         <v>120</v>
       </c>
-      <c r="E61" s="192" t="s">
+      <c r="F61" s="231" t="s">
         <v>121</v>
       </c>
-      <c r="F61" s="231" t="s">
+      <c r="G61" s="192" t="s">
         <v>122</v>
-      </c>
-      <c r="G61" s="192" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11474,13 +11471,13 @@
         <v>32</v>
       </c>
       <c r="E62" s="185" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F62" s="237" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G62" s="185" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11509,7 +11506,7 @@
     </row>
     <row r="66" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="246" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C66" s="246"/>
       <c r="D66" s="246"/>
@@ -12046,7 +12043,7 @@
     <row r="2" s="51" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="248"/>
       <c r="C2" s="249" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D2" s="250"/>
       <c r="E2" s="249"/>
@@ -12139,7 +12136,7 @@
     <row r="8" customFormat="false" ht="18.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="167"/>
       <c r="C8" s="260" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D8" s="170"/>
       <c r="E8" s="262"/>
@@ -12149,7 +12146,7 @@
     <row r="9" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="167"/>
       <c r="C9" s="232" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D9" s="263"/>
       <c r="E9" s="135"/>
@@ -12171,7 +12168,7 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="252"/>
       <c r="C11" s="253" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="254"/>
       <c r="E11" s="254"/>
@@ -12189,16 +12186,16 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="167"/>
       <c r="C13" s="262" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="192" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="192" t="s">
+      <c r="E13" s="192" t="s">
         <v>131</v>
       </c>
-      <c r="E13" s="192" t="s">
+      <c r="F13" s="193" t="s">
         <v>132</v>
-      </c>
-      <c r="F13" s="193" t="s">
-        <v>133</v>
       </c>
       <c r="G13" s="193"/>
     </row>
@@ -12206,13 +12203,13 @@
       <c r="B14" s="167"/>
       <c r="C14" s="182"/>
       <c r="D14" s="192" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="192" t="s">
         <v>134</v>
       </c>
-      <c r="E14" s="192" t="s">
+      <c r="F14" s="193" t="s">
         <v>135</v>
-      </c>
-      <c r="F14" s="193" t="s">
-        <v>136</v>
       </c>
       <c r="G14" s="193"/>
     </row>
@@ -12226,7 +12223,7 @@
         <v>32</v>
       </c>
       <c r="F15" s="237" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G15" s="195" t="s">
         <v>33</v>
@@ -12293,7 +12290,7 @@
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="167"/>
       <c r="C22" s="262" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D22" s="271"/>
       <c r="E22" s="272"/>
@@ -12311,7 +12308,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="252"/>
       <c r="C24" s="253" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D24" s="166"/>
       <c r="E24" s="254"/>
@@ -12349,7 +12346,7 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="167"/>
       <c r="C28" s="275" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D28" s="275"/>
       <c r="E28" s="239"/>
@@ -12359,7 +12356,7 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="167"/>
       <c r="C29" s="275" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D29" s="275"/>
       <c r="E29" s="239"/>
@@ -12369,7 +12366,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="167"/>
       <c r="C30" s="277" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D30" s="277"/>
       <c r="E30" s="239"/>
@@ -12379,7 +12376,7 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="167"/>
       <c r="C31" s="277" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D31" s="277"/>
       <c r="E31" s="239"/>
@@ -12389,7 +12386,7 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="167"/>
       <c r="C32" s="277" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D32" s="277"/>
       <c r="E32" s="239"/>
@@ -12399,7 +12396,7 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="167"/>
       <c r="C33" s="277" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D33" s="277"/>
       <c r="E33" s="239"/>
@@ -12417,7 +12414,7 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="252"/>
       <c r="C35" s="253" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D35" s="254"/>
       <c r="E35" s="254"/>
@@ -12437,13 +12434,13 @@
       <c r="C37" s="182"/>
       <c r="D37" s="182"/>
       <c r="E37" s="192" t="s">
+        <v>146</v>
+      </c>
+      <c r="F37" s="192" t="s">
         <v>147</v>
       </c>
-      <c r="F37" s="192" t="s">
+      <c r="G37" s="192" t="s">
         <v>148</v>
-      </c>
-      <c r="G37" s="192" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12481,7 +12478,7 @@
     <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="167"/>
       <c r="C41" s="168" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D41" s="168"/>
       <c r="E41" s="239"/>
@@ -12493,7 +12490,7 @@
     <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="167"/>
       <c r="C42" s="168" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D42" s="168"/>
       <c r="E42" s="239"/>
@@ -12505,7 +12502,7 @@
     <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="167"/>
       <c r="C43" s="168" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D43" s="168"/>
       <c r="E43" s="239"/>
@@ -12517,7 +12514,7 @@
     <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="167"/>
       <c r="C44" s="168" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D44" s="168"/>
       <c r="E44" s="239"/>
@@ -12531,7 +12528,7 @@
     <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="167"/>
       <c r="C45" s="168" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D45" s="168"/>
       <c r="E45" s="239"/>
@@ -12541,7 +12538,7 @@
     <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="167"/>
       <c r="C46" s="168" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D46" s="168"/>
       <c r="E46" s="239"/>
@@ -12555,7 +12552,7 @@
     <row r="47" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="167"/>
       <c r="C47" s="262" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D47" s="262"/>
       <c r="E47" s="209"/>
@@ -12565,7 +12562,7 @@
     <row r="48" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="167"/>
       <c r="C48" s="226" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D48" s="262"/>
       <c r="E48" s="233"/>
@@ -12583,7 +12580,7 @@
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="252"/>
       <c r="C50" s="253" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D50" s="254"/>
       <c r="E50" s="254"/>
@@ -12621,7 +12618,7 @@
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="167"/>
       <c r="C54" s="168" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D54" s="168"/>
       <c r="E54" s="239"/>
@@ -12631,7 +12628,7 @@
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="167"/>
       <c r="C55" s="168" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D55" s="168"/>
       <c r="E55" s="239"/>
@@ -12651,7 +12648,7 @@
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="167"/>
       <c r="C57" s="168" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D57" s="168"/>
       <c r="E57" s="239"/>
@@ -12669,7 +12666,7 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="167"/>
       <c r="C59" s="226" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D59" s="282"/>
       <c r="E59" s="283"/>
@@ -12679,7 +12676,7 @@
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="167"/>
       <c r="C60" s="226" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D60" s="282"/>
       <c r="E60" s="284"/>
@@ -12697,7 +12694,7 @@
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="252"/>
       <c r="C62" s="253" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D62" s="254"/>
       <c r="E62" s="254"/>
@@ -12735,7 +12732,7 @@
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="167"/>
       <c r="C66" s="168" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D66" s="168"/>
       <c r="E66" s="239"/>
@@ -12745,7 +12742,7 @@
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="167"/>
       <c r="C67" s="168" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D67" s="168"/>
       <c r="E67" s="239"/>
@@ -12755,7 +12752,7 @@
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="167"/>
       <c r="C68" s="168" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D68" s="168"/>
       <c r="E68" s="239"/>
@@ -12765,7 +12762,7 @@
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="167"/>
       <c r="C69" s="168" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D69" s="168"/>
       <c r="E69" s="239"/>
@@ -12775,7 +12772,7 @@
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="167"/>
       <c r="C70" s="168" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D70" s="168"/>
       <c r="E70" s="239"/>
@@ -12793,7 +12790,7 @@
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="252"/>
       <c r="C72" s="253" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D72" s="254"/>
       <c r="E72" s="254"/>
@@ -12811,7 +12808,7 @@
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="167"/>
       <c r="C74" s="168" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D74" s="168"/>
       <c r="E74" s="286"/>
@@ -12829,7 +12826,7 @@
     <row r="76" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="246" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C77" s="246"/>
       <c r="D77" s="246"/>
@@ -13334,7 +13331,7 @@
   </sheetPr>
   <dimension ref="B2:AMJ55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
@@ -13355,7 +13352,7 @@
     <row r="2" s="288" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="289"/>
       <c r="C2" s="290" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D2" s="290"/>
       <c r="E2" s="291"/>
@@ -13415,7 +13412,7 @@
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="102"/>
       <c r="C3" s="293" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D3" s="293"/>
       <c r="E3" s="293"/>
@@ -13439,7 +13436,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="98"/>
       <c r="C5" s="99" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5" s="99"/>
       <c r="E5" s="100"/>
@@ -13498,7 +13495,7 @@
     <row r="10" s="288" customFormat="true" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="296"/>
       <c r="C10" s="297" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D10" s="298"/>
       <c r="E10" s="299"/>
@@ -13573,7 +13570,7 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="102"/>
       <c r="C12" s="105" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D12" s="105"/>
       <c r="E12" s="306"/>
@@ -13597,7 +13594,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="102"/>
       <c r="C14" s="105" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D14" s="105"/>
       <c r="E14" s="306"/>
@@ -13621,7 +13618,7 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="102"/>
       <c r="C16" s="310" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D16" s="105"/>
       <c r="E16" s="306"/>
@@ -13634,7 +13631,7 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="102"/>
       <c r="C17" s="310" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D17" s="105"/>
       <c r="E17" s="306"/>
@@ -13658,7 +13655,7 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="102"/>
       <c r="C19" s="105" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D19" s="105"/>
       <c r="E19" s="105"/>
@@ -13682,17 +13679,17 @@
     <row r="21" s="288" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="296"/>
       <c r="C21" s="297" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D21" s="297"/>
       <c r="E21" s="315" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" s="316" t="s">
         <v>176</v>
       </c>
-      <c r="F21" s="316" t="s">
+      <c r="G21" s="315" t="s">
         <v>177</v>
-      </c>
-      <c r="G21" s="315" t="s">
-        <v>178</v>
       </c>
       <c r="H21" s="316" t="s">
         <v>30</v>
@@ -13763,12 +13760,12 @@
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="102"/>
       <c r="C23" s="105" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D23" s="105"/>
       <c r="E23" s="239"/>
       <c r="F23" s="324" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G23" s="325" t="n">
         <v>10</v>
@@ -13780,12 +13777,12 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="102"/>
       <c r="C24" s="105" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D24" s="105"/>
       <c r="E24" s="239"/>
       <c r="F24" s="324" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G24" s="325" t="n">
         <v>1300</v>
@@ -13797,12 +13794,12 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="102"/>
       <c r="C25" s="105" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D25" s="105"/>
       <c r="E25" s="239"/>
       <c r="F25" s="324" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G25" s="325" t="n">
         <v>1700</v>
@@ -13814,12 +13811,12 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="102"/>
       <c r="C26" s="105" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D26" s="105"/>
       <c r="E26" s="239"/>
       <c r="F26" s="324" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G26" s="325" t="n">
         <v>4.7</v>
@@ -13853,7 +13850,7 @@
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="102"/>
       <c r="C29" s="329" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D29" s="329"/>
       <c r="E29" s="239"/>
@@ -13921,7 +13918,7 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="102"/>
       <c r="C35" s="297" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D35" s="297"/>
       <c r="E35" s="306"/>
@@ -13960,7 +13957,7 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="102"/>
       <c r="C38" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="346"/>
@@ -13984,7 +13981,7 @@
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="102"/>
       <c r="C40" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="346"/>
@@ -14008,7 +14005,7 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="102"/>
       <c r="C42" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="346"/>
@@ -14032,7 +14029,7 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="102"/>
       <c r="C44" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="346"/>
@@ -14056,7 +14053,7 @@
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="102"/>
       <c r="C46" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="4"/>
@@ -14080,7 +14077,7 @@
     <row r="48" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="96"/>
       <c r="C48" s="353" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D48" s="353"/>
       <c r="E48" s="353"/>
@@ -14148,7 +14145,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="355" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C54" s="355"/>
       <c r="D54" s="355"/>
@@ -14671,7 +14668,7 @@
     <row r="1" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" s="356" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="357" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2" s="357"/>
       <c r="D2" s="357"/>
@@ -14710,7 +14707,7 @@
     </row>
     <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="358" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" s="358"/>
       <c r="D3" s="358"/>
@@ -14719,7 +14716,7 @@
     </row>
     <row r="4" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="359" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C4" s="99"/>
       <c r="D4" s="360"/>
@@ -14771,7 +14768,7 @@
     </row>
     <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="363" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C11" s="363"/>
       <c r="D11" s="363"/>
@@ -14808,16 +14805,16 @@
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="366"/>
       <c r="C15" s="367" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="367" t="s">
         <v>197</v>
       </c>
-      <c r="D15" s="367" t="s">
+      <c r="E15" s="367" t="s">
         <v>198</v>
       </c>
-      <c r="E15" s="367" t="s">
+      <c r="F15" s="368" t="s">
         <v>199</v>
-      </c>
-      <c r="F15" s="368" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14864,7 +14861,7 @@
     </row>
     <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="371" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C20" s="99"/>
       <c r="D20" s="360"/>
@@ -14917,7 +14914,7 @@
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="363" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C27" s="363"/>
       <c r="D27" s="363"/>
@@ -14954,16 +14951,16 @@
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="373"/>
       <c r="C31" s="367" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D31" s="367" t="s">
+        <v>201</v>
+      </c>
+      <c r="E31" s="367" t="s">
         <v>202</v>
       </c>
-      <c r="E31" s="367" t="s">
-        <v>203</v>
-      </c>
       <c r="F31" s="368" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15010,7 +15007,7 @@
     </row>
     <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="371" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C36" s="374"/>
       <c r="D36" s="13"/>
@@ -15061,7 +15058,7 @@
     </row>
     <row r="43" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="363" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C43" s="363"/>
       <c r="D43" s="363"/>
@@ -15098,16 +15095,16 @@
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="373"/>
       <c r="C47" s="367" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D47" s="367" t="s">
+        <v>201</v>
+      </c>
+      <c r="E47" s="367" t="s">
         <v>202</v>
       </c>
-      <c r="E47" s="367" t="s">
-        <v>203</v>
-      </c>
       <c r="F47" s="368" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15154,7 +15151,7 @@
     </row>
     <row r="52" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="246" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C52" s="246"/>
       <c r="D52" s="246"/>
@@ -15367,7 +15364,7 @@
     <row r="1" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="359" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" s="99"/>
       <c r="D2" s="360"/>
@@ -15427,7 +15424,7 @@
     </row>
     <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="376" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C10" s="376"/>
       <c r="D10" s="376"/>
@@ -15464,16 +15461,16 @@
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="373"/>
       <c r="C14" s="367" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D14" s="367" t="s">
+        <v>201</v>
+      </c>
+      <c r="E14" s="367" t="s">
         <v>202</v>
       </c>
-      <c r="E14" s="367" t="s">
-        <v>203</v>
-      </c>
       <c r="F14" s="368" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15520,7 +15517,7 @@
     </row>
     <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="371" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C19" s="374"/>
       <c r="D19" s="13"/>
@@ -15578,7 +15575,7 @@
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="376" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C27" s="376"/>
       <c r="D27" s="376"/>
@@ -15615,16 +15612,16 @@
     <row r="31" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="373"/>
       <c r="C31" s="367" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D31" s="367" t="s">
+        <v>201</v>
+      </c>
+      <c r="E31" s="367" t="s">
         <v>202</v>
       </c>
-      <c r="E31" s="367" t="s">
-        <v>203</v>
-      </c>
       <c r="F31" s="368" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15671,7 +15668,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="378" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C36" s="378"/>
       <c r="D36" s="378"/>
@@ -15785,7 +15782,7 @@
     </row>
     <row r="52" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="359" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C52" s="99"/>
       <c r="D52" s="360"/>
@@ -15801,7 +15798,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="324" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C54" s="324"/>
       <c r="D54" s="324"/>
@@ -15838,7 +15835,7 @@
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="246" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C59" s="246"/>
       <c r="D59" s="246"/>
@@ -15990,7 +15987,7 @@
     <row r="1" customFormat="false" ht="7.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="381" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" s="381"/>
       <c r="D2" s="381"/>
@@ -16534,7 +16531,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="382" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C62" s="382"/>
       <c r="D62" s="382"/>

</xml_diff>

<commit_message>
AE-427-AE-432 add new fields for last page of finnish 2018 xlsx template
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$J$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$H$63</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$N$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$B$1:$R$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
@@ -36,7 +36,7 @@
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$I$62</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$O$62</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="768">
   <si>
     <t xml:space="preserve">[:id]</t>
   </si>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">[:perustiedot :katuosoite-sv]</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29169]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44497]</t>
   </si>
   <si>
     <t xml:space="preserve">[:perustiedot :rakennustunnus]</t>
@@ -83,34 +83,34 @@
     <t xml:space="preserve">[:perustiedot :alakayttotarkoitus-sv]</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29171]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29173]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29175]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44499]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44501]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44503]</t>
   </si>
   <si>
     <t xml:space="preserve">Pysyvä rakennustunnus:</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29177]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44505]</t>
   </si>
   <si>
     <t xml:space="preserve">Rakennuksen valmistumisvuosi:</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29179]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44507]</t>
   </si>
   <si>
     <t xml:space="preserve">Rakennuksen käyttötarkoitusluokka:</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29181]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29183]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44509]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44511]</t>
   </si>
   <si>
     <t xml:space="preserve">Todistustunnus:</t>
@@ -134,10 +134,10 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29186]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29188]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44514]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44516]</t>
   </si>
   <si>
     <t xml:space="preserve">    Energiatehokkuusluokka </t>
@@ -222,7 +222,7 @@
     <t xml:space="preserve">Viimeinen voimassaolopäivä:</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29190]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44518]</t>
   </si>
   <si>
     <t xml:space="preserve">YHTEENVETO RAKENNUKSEN ENERGIATEHOKKUUDESTA</t>
@@ -509,25 +509,25 @@
     <t xml:space="preserve">[:tulokset :e-luokka-info :luokittelu :label-sv]</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29192]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29195]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29198]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29201]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29204]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29207]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29210]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44520]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44523]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44526]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44529]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44532]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44535]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44538]</t>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :e-luokka-info :e-luokka]</t>
@@ -1423,40 +1423,40 @@
     <t xml:space="preserve">[:lahtotiedot :lkvn-kaytto :lammitysenergian-nettotarve]</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29213]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29215]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29217]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29219]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29221]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29223]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29225]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29227]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29229]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29231]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29233]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29235]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44541]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44543]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44545]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44547]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44549]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44551]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44553]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44555]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44557]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44559]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44561]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44563]</t>
   </si>
   <si>
     <t xml:space="preserve">E-LUVUN LASKENNAN TULOKSET</t>
@@ -2066,13 +2066,13 @@
     <t xml:space="preserve">[:tulokset :laskentatyokalu]</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29237]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44565]</t>
   </si>
   <si>
     <t xml:space="preserve">TOTEUTUNUT ENERGIANKULUTUS</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29239]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--44567]</t>
   </si>
   <si>
     <t xml:space="preserve">Saatavilla olevat ostoenergian määrät ilmoitetaan sellaisenaan ilman lämmitystarvelukukorjausta.
@@ -2800,6 +2800,472 @@
   <si>
     <t xml:space="preserve">[:lisamerkintoja-sv]</t>
   </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :rakennusvaippa :lampokapasiteetti]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :rakennusvaippa :ilmatilavuus]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :ilmanvaihto :tuloilma-lampotila]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :tilat-ja-iv :lampopumppu-tuotto-osuus]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :lammin-kayttovesi :lampopumppu-tuotto-osuus]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :tilat-ja-iv :lampohavio-lammittamaton-tila]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :lammin-kayttovesi :lampohavio-lammittamaton-tila]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuukausitason erittely ympäristöstä olevasta energiasta otetun energian määrästä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kulutus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyöty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aurinko-sähkö</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muusähkö</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aurinko-lämpö</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muu lämpö</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lämpö-pumppu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tammi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helmi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huhti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Touko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kesä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heinä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joulu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energiatodistuksen laatimisessa käytettyjä lähtötietoja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lämpökapasiteetti Crak omin
+(Wh/m²K)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rakennuksen ilmatilavuus V
+(m³)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuloilman sisäänpuhalluslämpötila Tsp
+(°C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lämpöpumpun tuotto-osuus tilojen lämpöenergian tarpeesta QLP/Qlämmitys, tilat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lämpöpumpun tuotto-osuus käyttöveden lämpöenergian tarpeesta QLP/Qlämmitys, lkv </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lämmönjakelujärjestelmän lämpöhäviöt lämmittämättömään tilaan Qjakelu, ulos
+(kWh/a)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :hyoty :lampo]</t>
+  </si>
 </sst>
 </file>
 
@@ -2818,7 +3284,7 @@
     <numFmt numFmtId="173" formatCode="0%"/>
     <numFmt numFmtId="174" formatCode="0"/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="45">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3142,6 +3608,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF009EE0"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -3205,7 +3678,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="30">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -3406,6 +3879,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF009EE0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF009EE0"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF009EE0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF009EE0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -3434,7 +4087,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="394">
+  <cellXfs count="423">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5006,6 +5659,122 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="44" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="35" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -7657,9 +8426,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>234720</xdr:colOff>
+      <xdr:colOff>234000</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>249120</xdr:rowOff>
+      <xdr:rowOff>248400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7673,7 +8442,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4656960"/>
-          <a:ext cx="744840" cy="201600"/>
+          <a:ext cx="744120" cy="200880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7694,9 +8463,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>134640</xdr:colOff>
+      <xdr:colOff>133920</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>249120</xdr:rowOff>
+      <xdr:rowOff>248400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7710,7 +8479,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4971240"/>
-          <a:ext cx="1088280" cy="201600"/>
+          <a:ext cx="1087560" cy="200880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7731,9 +8500,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
+      <xdr:colOff>7200</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>249120</xdr:rowOff>
+      <xdr:rowOff>248400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7747,7 +8516,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5285520"/>
-          <a:ext cx="1395000" cy="201600"/>
+          <a:ext cx="1394280" cy="200880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7768,9 +8537,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>331920</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>249120</xdr:rowOff>
+      <xdr:rowOff>248400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7784,7 +8553,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5599800"/>
-          <a:ext cx="1719000" cy="201600"/>
+          <a:ext cx="1718280" cy="200880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7805,9 +8574,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>205200</xdr:colOff>
+      <xdr:colOff>204480</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7821,7 +8590,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5909760"/>
-          <a:ext cx="2026080" cy="214560"/>
+          <a:ext cx="2025360" cy="213840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7842,9 +8611,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>148320</xdr:colOff>
+      <xdr:colOff>147600</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>249120</xdr:rowOff>
+      <xdr:rowOff>248400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7858,7 +8627,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6219720"/>
-          <a:ext cx="2362320" cy="201600"/>
+          <a:ext cx="2361600" cy="200880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7879,9 +8648,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>88560</xdr:colOff>
+      <xdr:colOff>87840</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>250200</xdr:rowOff>
+      <xdr:rowOff>249480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7891,7 +8660,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6531480"/>
-          <a:ext cx="2675160" cy="200520"/>
+          <a:ext cx="2674440" cy="199800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8260,9 +9029,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287280</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8272,7 +9041,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1978200" y="78480"/>
-          <a:ext cx="6974280" cy="10495800"/>
+          <a:ext cx="6973560" cy="10495080"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8697,7 +9466,7 @@
       <c r="J9" s="0"/>
       <c r="K9" s="20" t="str">
         <f aca="false">A5</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29169]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44497]</v>
       </c>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
@@ -9134,7 +9903,7 @@
       <c r="D19" s="18"/>
       <c r="E19" s="38" t="str">
         <f aca="false">A10</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29171]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44499]</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
@@ -9161,7 +9930,7 @@
       <c r="D20" s="18"/>
       <c r="E20" s="38" t="str">
         <f aca="false">A12</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29175]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44503]</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
@@ -9186,7 +9955,7 @@
       <c r="D21" s="16"/>
       <c r="E21" s="16" t="str">
         <f aca="false">A14</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29179]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44507]</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
@@ -9874,7 +10643,7 @@
     <row r="50" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C50" s="92" t="str">
         <f aca="false">A21</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29186]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44514]</v>
       </c>
       <c r="D50" s="92"/>
       <c r="E50" s="92"/>
@@ -9886,7 +10655,7 @@
       <c r="K50" s="87"/>
       <c r="L50" s="94" t="str">
         <f aca="false">A22</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29188]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44516]</v>
       </c>
       <c r="M50" s="94"/>
       <c r="N50" s="94"/>
@@ -10187,7 +10956,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="107" t="str">
         <f aca="false">A2</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29190]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44518]</v>
       </c>
       <c r="G5" s="108"/>
       <c r="H5" s="5"/>
@@ -10904,15 +11673,15 @@
       <c r="F25" s="5"/>
       <c r="G25" s="139" t="str">
         <f aca="false">A45</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29192]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44520]</v>
       </c>
       <c r="H25" s="140" t="str">
         <f aca="false">A46</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29195]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44523]</v>
       </c>
       <c r="I25" s="141" t="str">
         <f aca="false">A47</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29198]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44526]</v>
       </c>
       <c r="J25" s="136"/>
       <c r="L25" s="0"/>
@@ -10943,15 +11712,15 @@
       <c r="F26" s="5"/>
       <c r="G26" s="142" t="str">
         <f aca="false">A48</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29201]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44529]</v>
       </c>
       <c r="H26" s="143" t="str">
         <f aca="false">A49</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29204]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44532]</v>
       </c>
       <c r="I26" s="144" t="str">
         <f aca="false">A50</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29207]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44535]</v>
       </c>
       <c r="J26" s="136"/>
       <c r="L26" s="0"/>
@@ -10982,7 +11751,7 @@
       <c r="F27" s="5"/>
       <c r="G27" s="145" t="str">
         <f aca="false">A51</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29210]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44538]</v>
       </c>
       <c r="H27" s="146"/>
       <c r="I27" s="146"/>
@@ -13468,19 +14237,19 @@
       <c r="C63" s="20"/>
       <c r="D63" s="211" t="str">
         <f aca="false">A81</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29213]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44541]</v>
       </c>
       <c r="E63" s="210" t="str">
         <f aca="false">A82</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29215]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44543]</v>
       </c>
       <c r="F63" s="244" t="str">
         <f aca="false">A83</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29217]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44545]</v>
       </c>
       <c r="G63" s="210" t="str">
         <f aca="false">A84</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29219]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44547]</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13491,19 +14260,19 @@
       <c r="C64" s="20"/>
       <c r="D64" s="211" t="str">
         <f aca="false">A85</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29221]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44549]</v>
       </c>
       <c r="E64" s="244" t="str">
         <f aca="false">A86</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29223]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44551]</v>
       </c>
       <c r="F64" s="244" t="str">
         <f aca="false">A87</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29225]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44553]</v>
       </c>
       <c r="G64" s="210" t="str">
         <f aca="false">A88</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29227]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44555]</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13514,19 +14283,19 @@
       <c r="C65" s="183"/>
       <c r="D65" s="246" t="str">
         <f aca="false">A89</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29229]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44557]</v>
       </c>
       <c r="E65" s="215" t="str">
         <f aca="false">A90</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29231]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44559]</v>
       </c>
       <c r="F65" s="247" t="str">
         <f aca="false">A91</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29233]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44561]</v>
       </c>
       <c r="G65" s="215" t="str">
         <f aca="false">A92</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29235]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44563]</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14137,59 +14906,59 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E10" type="none">
-      <formula1>OR(ISNUMBER(E12),E12="*")</formula1>
+      <formula1>OR(ISNUMBER(F12),F12="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E11 E13:E14" type="none">
-      <formula1>OR(ISNUMBER(E13),E13="*")</formula1>
+      <formula1>OR(ISNUMBER(F13),F13="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F15" type="none">
-      <formula1>OR(ISNUMBER(F17),F17="*")</formula1>
+      <formula1>OR(ISNUMBER(G17),G17="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G15" type="none">
-      <formula1>OR(ISNUMBER(G17),G17="*")</formula1>
+      <formula1>OR(ISNUMBER(H17),H17="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D19:D21 E20 D22:D26" type="none">
-      <formula1>OR(ISNUMBER(D21),D21="*")</formula1>
+      <formula1>OR(ISNUMBER(E21),E21="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E19:F19 F20:F26 E21:E26" type="none">
-      <formula1>OR(ISNUMBER(E21),E21="*")</formula1>
+      <formula1>OR(ISNUMBER(F21),F21="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D33:F33" type="none">
-      <formula1>OR(ISNUMBER(E35),E35="*")</formula1>
+      <formula1>OR(ISNUMBER(F35),F35="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D34:E34" type="none">
-      <formula1>OR(ISNUMBER(E36),E36="*")</formula1>
+      <formula1>OR(ISNUMBER(F36),F36="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D35:E35" type="none">
-      <formula1>OR(ISNUMBER(E37),E37="*")</formula1>
+      <formula1>OR(ISNUMBER(F37),F37="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G33" type="none">
-      <formula1>OR(ISNUMBER(G35),G35="*")</formula1>
+      <formula1>OR(ISNUMBER(H35),H35="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E36" type="none">
-      <formula1>OR(ISNUMBER(E38),E38="*")</formula1>
+      <formula1>OR(ISNUMBER(F38),F38="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D43:G44" type="none">
-      <formula1>OR(ISNUMBER(D7),D7="*")</formula1>
+      <formula1>OR(ISNUMBER(E7),E7="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D50:E51" type="none">
-      <formula1>OR(ISNUMBER(D14),D14="*")</formula1>
+      <formula1>OR(ISNUMBER(E14),E14="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D55:E55 D59:E59 D63:G65" type="none">
-      <formula1>OR(ISNUMBER(D27),D27="*")</formula1>
+      <formula1>OR(ISNUMBER(E27),E27="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -16136,7 +16905,7 @@
   <dimension ref="A1:AMJ67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I46" activeCellId="0" sqref="I46"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16289,7 +17058,7 @@
       <c r="B7" s="105"/>
       <c r="C7" s="300" t="str">
         <f aca="false">A2</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29237]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--44565]</v>
       </c>
       <c r="D7" s="111"/>
       <c r="E7" s="111"/>
@@ -18851,8 +19620,8 @@
   </sheetPr>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19714,20 +20483,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:O130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T41" activeCellId="0" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="366" width="25.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="3" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="1.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="994" min="10" style="3" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="995" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="2.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="3" width="10.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="2.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="1.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1000" min="16" style="3" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1001" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="7.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19748,6 +20519,12 @@
       <c r="F2" s="392"/>
       <c r="G2" s="392"/>
       <c r="H2" s="392"/>
+      <c r="I2" s="392"/>
+      <c r="J2" s="392"/>
+      <c r="K2" s="392"/>
+      <c r="L2" s="392"/>
+      <c r="M2" s="392"/>
+      <c r="N2" s="392"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="366" t="s">
@@ -19763,8 +20540,17 @@
       <c r="F3" s="373"/>
       <c r="G3" s="373"/>
       <c r="H3" s="373"/>
+      <c r="I3" s="373"/>
+      <c r="J3" s="373"/>
+      <c r="K3" s="373"/>
+      <c r="L3" s="373"/>
+      <c r="M3" s="373"/>
+      <c r="N3" s="373"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="366" t="s">
+        <v>614</v>
+      </c>
       <c r="B4" s="373"/>
       <c r="C4" s="373"/>
       <c r="D4" s="373"/>
@@ -19772,8 +20558,17 @@
       <c r="F4" s="373"/>
       <c r="G4" s="373"/>
       <c r="H4" s="373"/>
+      <c r="I4" s="373"/>
+      <c r="J4" s="373"/>
+      <c r="K4" s="373"/>
+      <c r="L4" s="373"/>
+      <c r="M4" s="373"/>
+      <c r="N4" s="373"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="366" t="s">
+        <v>615</v>
+      </c>
       <c r="B5" s="373"/>
       <c r="C5" s="373"/>
       <c r="D5" s="373"/>
@@ -19781,8 +20576,17 @@
       <c r="F5" s="373"/>
       <c r="G5" s="373"/>
       <c r="H5" s="373"/>
+      <c r="I5" s="373"/>
+      <c r="J5" s="373"/>
+      <c r="K5" s="373"/>
+      <c r="L5" s="373"/>
+      <c r="M5" s="373"/>
+      <c r="N5" s="373"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="366" t="s">
+        <v>616</v>
+      </c>
       <c r="B6" s="373"/>
       <c r="C6" s="373"/>
       <c r="D6" s="373"/>
@@ -19790,9 +20594,18 @@
       <c r="F6" s="373"/>
       <c r="G6" s="373"/>
       <c r="H6" s="373"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="373"/>
+      <c r="J6" s="373"/>
+      <c r="K6" s="373"/>
+      <c r="L6" s="373"/>
+      <c r="M6" s="373"/>
+      <c r="N6" s="373"/>
+      <c r="O6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="7.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="366" t="s">
+        <v>617</v>
+      </c>
       <c r="B7" s="373"/>
       <c r="C7" s="373"/>
       <c r="D7" s="373"/>
@@ -19800,9 +20613,18 @@
       <c r="F7" s="373"/>
       <c r="G7" s="373"/>
       <c r="H7" s="373"/>
-      <c r="I7" s="13"/>
+      <c r="I7" s="373"/>
+      <c r="J7" s="373"/>
+      <c r="K7" s="373"/>
+      <c r="L7" s="373"/>
+      <c r="M7" s="373"/>
+      <c r="N7" s="373"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="366" t="s">
+        <v>618</v>
+      </c>
       <c r="B8" s="373"/>
       <c r="C8" s="373"/>
       <c r="D8" s="373"/>
@@ -19810,8 +20632,17 @@
       <c r="F8" s="373"/>
       <c r="G8" s="373"/>
       <c r="H8" s="373"/>
+      <c r="I8" s="373"/>
+      <c r="J8" s="373"/>
+      <c r="K8" s="373"/>
+      <c r="L8" s="373"/>
+      <c r="M8" s="373"/>
+      <c r="N8" s="373"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="366" t="s">
+        <v>619</v>
+      </c>
       <c r="B9" s="373"/>
       <c r="C9" s="373"/>
       <c r="D9" s="373"/>
@@ -19819,8 +20650,17 @@
       <c r="F9" s="373"/>
       <c r="G9" s="373"/>
       <c r="H9" s="373"/>
+      <c r="I9" s="373"/>
+      <c r="J9" s="373"/>
+      <c r="K9" s="373"/>
+      <c r="L9" s="373"/>
+      <c r="M9" s="373"/>
+      <c r="N9" s="373"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="366" t="s">
+        <v>620</v>
+      </c>
       <c r="B10" s="373"/>
       <c r="C10" s="373"/>
       <c r="D10" s="373"/>
@@ -19828,8 +20668,17 @@
       <c r="F10" s="373"/>
       <c r="G10" s="373"/>
       <c r="H10" s="373"/>
+      <c r="I10" s="373"/>
+      <c r="J10" s="373"/>
+      <c r="K10" s="373"/>
+      <c r="L10" s="373"/>
+      <c r="M10" s="373"/>
+      <c r="N10" s="373"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="366" t="s">
+        <v>621</v>
+      </c>
       <c r="B11" s="373"/>
       <c r="C11" s="373"/>
       <c r="D11" s="373"/>
@@ -19837,8 +20686,17 @@
       <c r="F11" s="373"/>
       <c r="G11" s="373"/>
       <c r="H11" s="373"/>
+      <c r="I11" s="373"/>
+      <c r="J11" s="373"/>
+      <c r="K11" s="373"/>
+      <c r="L11" s="373"/>
+      <c r="M11" s="373"/>
+      <c r="N11" s="373"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="366" t="s">
+        <v>622</v>
+      </c>
       <c r="B12" s="373"/>
       <c r="C12" s="373"/>
       <c r="D12" s="373"/>
@@ -19846,8 +20704,17 @@
       <c r="F12" s="373"/>
       <c r="G12" s="373"/>
       <c r="H12" s="373"/>
+      <c r="I12" s="373"/>
+      <c r="J12" s="373"/>
+      <c r="K12" s="373"/>
+      <c r="L12" s="373"/>
+      <c r="M12" s="373"/>
+      <c r="N12" s="373"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="366" t="s">
+        <v>623</v>
+      </c>
       <c r="B13" s="373"/>
       <c r="C13" s="373"/>
       <c r="D13" s="373"/>
@@ -19855,8 +20722,17 @@
       <c r="F13" s="373"/>
       <c r="G13" s="373"/>
       <c r="H13" s="373"/>
+      <c r="I13" s="373"/>
+      <c r="J13" s="373"/>
+      <c r="K13" s="373"/>
+      <c r="L13" s="373"/>
+      <c r="M13" s="373"/>
+      <c r="N13" s="373"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="366" t="s">
+        <v>624</v>
+      </c>
       <c r="B14" s="373"/>
       <c r="C14" s="373"/>
       <c r="D14" s="373"/>
@@ -19864,8 +20740,17 @@
       <c r="F14" s="373"/>
       <c r="G14" s="373"/>
       <c r="H14" s="373"/>
+      <c r="I14" s="373"/>
+      <c r="J14" s="373"/>
+      <c r="K14" s="373"/>
+      <c r="L14" s="373"/>
+      <c r="M14" s="373"/>
+      <c r="N14" s="373"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="366" t="s">
+        <v>625</v>
+      </c>
       <c r="B15" s="373"/>
       <c r="C15" s="373"/>
       <c r="D15" s="373"/>
@@ -19873,8 +20758,17 @@
       <c r="F15" s="373"/>
       <c r="G15" s="373"/>
       <c r="H15" s="373"/>
+      <c r="I15" s="373"/>
+      <c r="J15" s="373"/>
+      <c r="K15" s="373"/>
+      <c r="L15" s="373"/>
+      <c r="M15" s="373"/>
+      <c r="N15" s="373"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="366" t="s">
+        <v>626</v>
+      </c>
       <c r="B16" s="373"/>
       <c r="C16" s="373"/>
       <c r="D16" s="373"/>
@@ -19882,8 +20776,17 @@
       <c r="F16" s="373"/>
       <c r="G16" s="373"/>
       <c r="H16" s="373"/>
+      <c r="I16" s="373"/>
+      <c r="J16" s="373"/>
+      <c r="K16" s="373"/>
+      <c r="L16" s="373"/>
+      <c r="M16" s="373"/>
+      <c r="N16" s="373"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="366" t="s">
+        <v>627</v>
+      </c>
       <c r="B17" s="373"/>
       <c r="C17" s="373"/>
       <c r="D17" s="373"/>
@@ -19891,8 +20794,17 @@
       <c r="F17" s="373"/>
       <c r="G17" s="373"/>
       <c r="H17" s="373"/>
+      <c r="I17" s="373"/>
+      <c r="J17" s="373"/>
+      <c r="K17" s="373"/>
+      <c r="L17" s="373"/>
+      <c r="M17" s="373"/>
+      <c r="N17" s="373"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="366" t="s">
+        <v>628</v>
+      </c>
       <c r="B18" s="373"/>
       <c r="C18" s="373"/>
       <c r="D18" s="373"/>
@@ -19900,8 +20812,17 @@
       <c r="F18" s="373"/>
       <c r="G18" s="373"/>
       <c r="H18" s="373"/>
+      <c r="I18" s="373"/>
+      <c r="J18" s="373"/>
+      <c r="K18" s="373"/>
+      <c r="L18" s="373"/>
+      <c r="M18" s="373"/>
+      <c r="N18" s="373"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="366" t="s">
+        <v>629</v>
+      </c>
       <c r="B19" s="373"/>
       <c r="C19" s="373"/>
       <c r="D19" s="373"/>
@@ -19909,8 +20830,17 @@
       <c r="F19" s="373"/>
       <c r="G19" s="373"/>
       <c r="H19" s="373"/>
+      <c r="I19" s="373"/>
+      <c r="J19" s="373"/>
+      <c r="K19" s="373"/>
+      <c r="L19" s="373"/>
+      <c r="M19" s="373"/>
+      <c r="N19" s="373"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="366" t="s">
+        <v>630</v>
+      </c>
       <c r="B20" s="373"/>
       <c r="C20" s="373"/>
       <c r="D20" s="373"/>
@@ -19918,404 +20848,1590 @@
       <c r="F20" s="373"/>
       <c r="G20" s="373"/>
       <c r="H20" s="373"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="373"/>
-      <c r="C21" s="373"/>
-      <c r="D21" s="373"/>
-      <c r="E21" s="373"/>
-      <c r="F21" s="373"/>
-      <c r="G21" s="373"/>
-      <c r="H21" s="373"/>
+      <c r="I20" s="373"/>
+      <c r="J20" s="373"/>
+      <c r="K20" s="373"/>
+      <c r="L20" s="373"/>
+      <c r="M20" s="373"/>
+      <c r="N20" s="373"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="366" t="s">
+        <v>631</v>
+      </c>
+      <c r="B21" s="393" t="s">
+        <v>632</v>
+      </c>
+      <c r="C21" s="393"/>
+      <c r="D21" s="393"/>
+      <c r="E21" s="393"/>
+      <c r="F21" s="393"/>
+      <c r="G21" s="393"/>
+      <c r="H21" s="393"/>
+      <c r="I21" s="393"/>
+      <c r="J21" s="393"/>
+      <c r="K21" s="393"/>
+      <c r="L21" s="393"/>
+      <c r="M21" s="393"/>
+      <c r="N21" s="393"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="373"/>
-      <c r="C22" s="373"/>
-      <c r="D22" s="373"/>
-      <c r="E22" s="373"/>
-      <c r="F22" s="373"/>
-      <c r="G22" s="373"/>
-      <c r="H22" s="373"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="373"/>
-      <c r="C23" s="373"/>
-      <c r="D23" s="373"/>
-      <c r="E23" s="373"/>
-      <c r="F23" s="373"/>
-      <c r="G23" s="373"/>
-      <c r="H23" s="373"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="373"/>
-      <c r="C24" s="373"/>
-      <c r="D24" s="373"/>
-      <c r="E24" s="373"/>
-      <c r="F24" s="373"/>
-      <c r="G24" s="373"/>
-      <c r="H24" s="373"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="373"/>
-      <c r="C25" s="373"/>
-      <c r="D25" s="373"/>
-      <c r="E25" s="373"/>
-      <c r="F25" s="373"/>
-      <c r="G25" s="373"/>
-      <c r="H25" s="373"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="373"/>
-      <c r="C26" s="373"/>
-      <c r="D26" s="373"/>
-      <c r="E26" s="373"/>
-      <c r="F26" s="373"/>
-      <c r="G26" s="373"/>
-      <c r="H26" s="373"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="373"/>
-      <c r="C27" s="373"/>
-      <c r="D27" s="373"/>
-      <c r="E27" s="373"/>
-      <c r="F27" s="373"/>
-      <c r="G27" s="373"/>
-      <c r="H27" s="373"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="373"/>
-      <c r="C28" s="373"/>
-      <c r="D28" s="373"/>
-      <c r="E28" s="373"/>
-      <c r="F28" s="373"/>
-      <c r="G28" s="373"/>
-      <c r="H28" s="373"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="373"/>
-      <c r="C29" s="373"/>
-      <c r="D29" s="373"/>
-      <c r="E29" s="373"/>
-      <c r="F29" s="373"/>
-      <c r="G29" s="373"/>
-      <c r="H29" s="373"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="373"/>
-      <c r="C30" s="373"/>
-      <c r="D30" s="373"/>
-      <c r="E30" s="373"/>
-      <c r="F30" s="373"/>
-      <c r="G30" s="373"/>
-      <c r="H30" s="373"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="373"/>
-      <c r="C31" s="373"/>
-      <c r="D31" s="373"/>
-      <c r="E31" s="373"/>
-      <c r="F31" s="373"/>
-      <c r="G31" s="373"/>
-      <c r="H31" s="373"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="373"/>
-      <c r="C32" s="373"/>
-      <c r="D32" s="373"/>
-      <c r="E32" s="373"/>
-      <c r="F32" s="373"/>
-      <c r="G32" s="373"/>
-      <c r="H32" s="373"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="373"/>
-      <c r="C33" s="373"/>
-      <c r="D33" s="373"/>
-      <c r="E33" s="373"/>
-      <c r="F33" s="373"/>
-      <c r="G33" s="373"/>
-      <c r="H33" s="373"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="373"/>
-      <c r="C34" s="373"/>
-      <c r="D34" s="373"/>
-      <c r="E34" s="373"/>
-      <c r="F34" s="373"/>
-      <c r="G34" s="373"/>
-      <c r="H34" s="373"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="373"/>
-      <c r="C35" s="373"/>
-      <c r="D35" s="373"/>
-      <c r="E35" s="373"/>
-      <c r="F35" s="373"/>
-      <c r="G35" s="373"/>
-      <c r="H35" s="373"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="373"/>
-      <c r="C36" s="373"/>
-      <c r="D36" s="373"/>
-      <c r="E36" s="373"/>
-      <c r="F36" s="373"/>
-      <c r="G36" s="373"/>
-      <c r="H36" s="373"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="373"/>
-      <c r="C37" s="373"/>
-      <c r="D37" s="373"/>
-      <c r="E37" s="373"/>
-      <c r="F37" s="373"/>
-      <c r="G37" s="373"/>
-      <c r="H37" s="373"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="373"/>
-      <c r="C38" s="373"/>
-      <c r="D38" s="373"/>
-      <c r="E38" s="373"/>
-      <c r="F38" s="373"/>
-      <c r="G38" s="373"/>
-      <c r="H38" s="373"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="373"/>
-      <c r="C39" s="373"/>
-      <c r="D39" s="373"/>
-      <c r="E39" s="373"/>
-      <c r="F39" s="373"/>
-      <c r="G39" s="373"/>
-      <c r="H39" s="373"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="373"/>
-      <c r="C40" s="373"/>
-      <c r="D40" s="373"/>
-      <c r="E40" s="373"/>
-      <c r="F40" s="373"/>
-      <c r="G40" s="373"/>
-      <c r="H40" s="373"/>
-    </row>
-    <row r="41" customFormat="false" ht="6.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="373"/>
-      <c r="C41" s="373"/>
-      <c r="D41" s="373"/>
-      <c r="E41" s="373"/>
-      <c r="F41" s="373"/>
-      <c r="G41" s="373"/>
-      <c r="H41" s="373"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="373"/>
-      <c r="C42" s="373"/>
-      <c r="D42" s="373"/>
-      <c r="E42" s="373"/>
-      <c r="F42" s="373"/>
-      <c r="G42" s="373"/>
-      <c r="H42" s="373"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="373"/>
-      <c r="C43" s="373"/>
-      <c r="D43" s="373"/>
-      <c r="E43" s="373"/>
-      <c r="F43" s="373"/>
-      <c r="G43" s="373"/>
-      <c r="H43" s="373"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="373"/>
-      <c r="C44" s="373"/>
-      <c r="D44" s="373"/>
-      <c r="E44" s="373"/>
-      <c r="F44" s="373"/>
-      <c r="G44" s="373"/>
-      <c r="H44" s="373"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="373"/>
-      <c r="C45" s="373"/>
-      <c r="D45" s="373"/>
-      <c r="E45" s="373"/>
-      <c r="F45" s="373"/>
-      <c r="G45" s="373"/>
-      <c r="H45" s="373"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="373"/>
-      <c r="C46" s="373"/>
-      <c r="D46" s="373"/>
-      <c r="E46" s="373"/>
-      <c r="F46" s="373"/>
-      <c r="G46" s="373"/>
-      <c r="H46" s="373"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="373"/>
-      <c r="C47" s="373"/>
-      <c r="D47" s="373"/>
-      <c r="E47" s="373"/>
-      <c r="F47" s="373"/>
-      <c r="G47" s="373"/>
-      <c r="H47" s="373"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="373"/>
-      <c r="C48" s="373"/>
-      <c r="D48" s="373"/>
-      <c r="E48" s="373"/>
-      <c r="F48" s="373"/>
-      <c r="G48" s="373"/>
-      <c r="H48" s="373"/>
-    </row>
-    <row r="49" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="373"/>
-      <c r="C49" s="373"/>
-      <c r="D49" s="373"/>
-      <c r="E49" s="373"/>
-      <c r="F49" s="373"/>
-      <c r="G49" s="373"/>
-      <c r="H49" s="373"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="373"/>
-      <c r="C50" s="373"/>
-      <c r="D50" s="373"/>
-      <c r="E50" s="373"/>
-      <c r="F50" s="373"/>
-      <c r="G50" s="373"/>
-      <c r="H50" s="373"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="373"/>
-      <c r="C51" s="373"/>
-      <c r="D51" s="373"/>
-      <c r="E51" s="373"/>
-      <c r="F51" s="373"/>
-      <c r="G51" s="373"/>
-      <c r="H51" s="373"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="373"/>
-      <c r="C52" s="373"/>
-      <c r="D52" s="373"/>
-      <c r="E52" s="373"/>
-      <c r="F52" s="373"/>
-      <c r="G52" s="373"/>
-      <c r="H52" s="373"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="373"/>
-      <c r="C53" s="373"/>
-      <c r="D53" s="373"/>
-      <c r="E53" s="373"/>
-      <c r="F53" s="373"/>
-      <c r="G53" s="373"/>
-      <c r="H53" s="373"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="373"/>
-      <c r="C54" s="373"/>
-      <c r="D54" s="373"/>
-      <c r="E54" s="373"/>
-      <c r="F54" s="373"/>
-      <c r="G54" s="373"/>
-      <c r="H54" s="373"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="373"/>
-      <c r="C55" s="373"/>
-      <c r="D55" s="373"/>
-      <c r="E55" s="373"/>
-      <c r="F55" s="373"/>
-      <c r="G55" s="373"/>
-      <c r="H55" s="373"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="373"/>
-      <c r="C56" s="373"/>
-      <c r="D56" s="373"/>
-      <c r="E56" s="373"/>
-      <c r="F56" s="373"/>
-      <c r="G56" s="373"/>
-      <c r="H56" s="373"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="373"/>
-      <c r="C57" s="373"/>
-      <c r="D57" s="373"/>
-      <c r="E57" s="373"/>
-      <c r="F57" s="373"/>
-      <c r="G57" s="373"/>
-      <c r="H57" s="373"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="373"/>
-      <c r="C58" s="373"/>
-      <c r="D58" s="373"/>
-      <c r="E58" s="373"/>
-      <c r="F58" s="373"/>
-      <c r="G58" s="373"/>
-      <c r="H58" s="373"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="373"/>
-      <c r="C59" s="373"/>
-      <c r="D59" s="373"/>
-      <c r="E59" s="373"/>
-      <c r="F59" s="373"/>
-      <c r="G59" s="373"/>
-      <c r="H59" s="373"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="373"/>
-      <c r="C60" s="373"/>
-      <c r="D60" s="373"/>
-      <c r="E60" s="373"/>
-      <c r="F60" s="373"/>
-      <c r="G60" s="373"/>
-      <c r="H60" s="373"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="373"/>
-      <c r="C61" s="373"/>
-      <c r="D61" s="373"/>
-      <c r="E61" s="373"/>
-      <c r="F61" s="373"/>
-      <c r="G61" s="373"/>
-      <c r="H61" s="373"/>
+      <c r="A22" s="366" t="s">
+        <v>633</v>
+      </c>
+      <c r="B22" s="393"/>
+      <c r="C22" s="393"/>
+      <c r="D22" s="393"/>
+      <c r="E22" s="393"/>
+      <c r="F22" s="393"/>
+      <c r="G22" s="393"/>
+      <c r="H22" s="393"/>
+      <c r="I22" s="393"/>
+      <c r="J22" s="393"/>
+      <c r="K22" s="393"/>
+      <c r="L22" s="393"/>
+      <c r="M22" s="393"/>
+      <c r="N22" s="393"/>
+    </row>
+    <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="366" t="s">
+        <v>634</v>
+      </c>
+      <c r="B23" s="394"/>
+      <c r="C23" s="395"/>
+      <c r="D23" s="395"/>
+      <c r="E23" s="395"/>
+      <c r="F23" s="395"/>
+      <c r="G23" s="395"/>
+      <c r="H23" s="395"/>
+      <c r="I23" s="395"/>
+      <c r="J23" s="395"/>
+      <c r="K23" s="395"/>
+      <c r="L23" s="395"/>
+      <c r="M23" s="395"/>
+      <c r="N23" s="396"/>
+    </row>
+    <row r="24" customFormat="false" ht="26.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="366" t="s">
+        <v>635</v>
+      </c>
+      <c r="B24" s="394"/>
+      <c r="C24" s="395"/>
+      <c r="D24" s="397" t="s">
+        <v>222</v>
+      </c>
+      <c r="E24" s="398"/>
+      <c r="F24" s="398"/>
+      <c r="G24" s="398"/>
+      <c r="H24" s="398"/>
+      <c r="I24" s="399"/>
+      <c r="J24" s="397" t="s">
+        <v>636</v>
+      </c>
+      <c r="K24" s="399"/>
+      <c r="L24" s="397" t="s">
+        <v>637</v>
+      </c>
+      <c r="M24" s="399"/>
+      <c r="N24" s="396"/>
+    </row>
+    <row r="25" customFormat="false" ht="27.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="366" t="s">
+        <v>638</v>
+      </c>
+      <c r="B25" s="394"/>
+      <c r="C25" s="395"/>
+      <c r="D25" s="400" t="s">
+        <v>639</v>
+      </c>
+      <c r="E25" s="401" t="s">
+        <v>300</v>
+      </c>
+      <c r="F25" s="401" t="s">
+        <v>640</v>
+      </c>
+      <c r="G25" s="401" t="s">
+        <v>641</v>
+      </c>
+      <c r="H25" s="401" t="s">
+        <v>642</v>
+      </c>
+      <c r="I25" s="402" t="s">
+        <v>643</v>
+      </c>
+      <c r="J25" s="400" t="s">
+        <v>306</v>
+      </c>
+      <c r="K25" s="402" t="s">
+        <v>307</v>
+      </c>
+      <c r="L25" s="400" t="s">
+        <v>306</v>
+      </c>
+      <c r="M25" s="402" t="s">
+        <v>307</v>
+      </c>
+      <c r="N25" s="396"/>
+    </row>
+    <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="366" t="s">
+        <v>644</v>
+      </c>
+      <c r="B26" s="394"/>
+      <c r="C26" s="403" t="s">
+        <v>645</v>
+      </c>
+      <c r="D26" s="404" t="str">
+        <f aca="false">A11</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E26" s="405" t="str">
+        <f aca="false">A12</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F26" s="405" t="str">
+        <f aca="false">A13</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :muusahko]</v>
+      </c>
+      <c r="G26" s="405" t="str">
+        <f aca="false">A14</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H26" s="405" t="str">
+        <f aca="false">A15</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :muulampo]</v>
+      </c>
+      <c r="I26" s="406" t="str">
+        <f aca="false">A16</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J26" s="404" t="str">
+        <f aca="false">A17</f>
+        <v>[:tulokset :kuukausierittely 0 :kulutus :sahko]</v>
+      </c>
+      <c r="K26" s="406" t="str">
+        <f aca="false">A18</f>
+        <v>[:tulokset :kuukausierittely 0 :kulutus :lampo]</v>
+      </c>
+      <c r="L26" s="404" t="str">
+        <f aca="false">A19</f>
+        <v>[:tulokset :kuukausierittely 0 :hyoty :sahko]</v>
+      </c>
+      <c r="M26" s="406" t="str">
+        <f aca="false">A20</f>
+        <v>[:tulokset :kuukausierittely 0 :hyoty :lampo]</v>
+      </c>
+      <c r="N26" s="396"/>
+    </row>
+    <row r="27" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="366" t="s">
+        <v>646</v>
+      </c>
+      <c r="B27" s="394"/>
+      <c r="C27" s="407" t="s">
+        <v>647</v>
+      </c>
+      <c r="D27" s="408" t="str">
+        <f aca="false">A21</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E27" s="409" t="str">
+        <f aca="false">A22</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F27" s="409" t="str">
+        <f aca="false">A23</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :muusahko]</v>
+      </c>
+      <c r="G27" s="409" t="str">
+        <f aca="false">A24</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H27" s="409" t="str">
+        <f aca="false">A25</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :muulampo]</v>
+      </c>
+      <c r="I27" s="410" t="str">
+        <f aca="false">A26</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J27" s="408" t="str">
+        <f aca="false">A27</f>
+        <v>[:tulokset :kuukausierittely 1 :kulutus :sahko]</v>
+      </c>
+      <c r="K27" s="410" t="str">
+        <f aca="false">A28</f>
+        <v>[:tulokset :kuukausierittely 1 :kulutus :lampo]</v>
+      </c>
+      <c r="L27" s="408" t="str">
+        <f aca="false">A29</f>
+        <v>[:tulokset :kuukausierittely 1 :hyoty :sahko]</v>
+      </c>
+      <c r="M27" s="410" t="str">
+        <f aca="false">A30</f>
+        <v>[:tulokset :kuukausierittely 1 :hyoty :lampo]</v>
+      </c>
+      <c r="N27" s="396"/>
+    </row>
+    <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="366" t="s">
+        <v>648</v>
+      </c>
+      <c r="B28" s="394"/>
+      <c r="C28" s="407" t="s">
+        <v>649</v>
+      </c>
+      <c r="D28" s="408" t="str">
+        <f aca="false">A31</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E28" s="409" t="str">
+        <f aca="false">A32</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F28" s="409" t="str">
+        <f aca="false">A33</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :muusahko]</v>
+      </c>
+      <c r="G28" s="409" t="str">
+        <f aca="false">A34</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H28" s="409" t="str">
+        <f aca="false">A35</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :muulampo]</v>
+      </c>
+      <c r="I28" s="410" t="str">
+        <f aca="false">A36</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J28" s="408" t="str">
+        <f aca="false">A37</f>
+        <v>[:tulokset :kuukausierittely 2 :kulutus :sahko]</v>
+      </c>
+      <c r="K28" s="410" t="str">
+        <f aca="false">A38</f>
+        <v>[:tulokset :kuukausierittely 2 :kulutus :lampo]</v>
+      </c>
+      <c r="L28" s="408" t="str">
+        <f aca="false">A39</f>
+        <v>[:tulokset :kuukausierittely 2 :hyoty :sahko]</v>
+      </c>
+      <c r="M28" s="410" t="str">
+        <f aca="false">A40</f>
+        <v>[:tulokset :kuukausierittely 2 :hyoty :lampo]</v>
+      </c>
+      <c r="N28" s="396"/>
+    </row>
+    <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="366" t="s">
+        <v>650</v>
+      </c>
+      <c r="B29" s="394"/>
+      <c r="C29" s="407" t="s">
+        <v>651</v>
+      </c>
+      <c r="D29" s="408" t="str">
+        <f aca="false">A41</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E29" s="409" t="str">
+        <f aca="false">A42</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F29" s="409" t="str">
+        <f aca="false">A43</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :muusahko]</v>
+      </c>
+      <c r="G29" s="409" t="str">
+        <f aca="false">A44</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H29" s="409" t="str">
+        <f aca="false">A45</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :muulampo]</v>
+      </c>
+      <c r="I29" s="410" t="str">
+        <f aca="false">A46</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J29" s="408" t="str">
+        <f aca="false">A47</f>
+        <v>[:tulokset :kuukausierittely 3 :kulutus :sahko]</v>
+      </c>
+      <c r="K29" s="410" t="str">
+        <f aca="false">A48</f>
+        <v>[:tulokset :kuukausierittely 3 :kulutus :lampo]</v>
+      </c>
+      <c r="L29" s="408" t="str">
+        <f aca="false">A49</f>
+        <v>[:tulokset :kuukausierittely 3 :hyoty :sahko]</v>
+      </c>
+      <c r="M29" s="410" t="str">
+        <f aca="false">A50</f>
+        <v>[:tulokset :kuukausierittely 3 :hyoty :lampo]</v>
+      </c>
+      <c r="N29" s="396"/>
+    </row>
+    <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="366" t="s">
+        <v>652</v>
+      </c>
+      <c r="B30" s="394"/>
+      <c r="C30" s="407" t="s">
+        <v>653</v>
+      </c>
+      <c r="D30" s="404" t="str">
+        <f aca="false">A51</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E30" s="409" t="str">
+        <f aca="false">A52</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F30" s="409" t="str">
+        <f aca="false">A53</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :muusahko]</v>
+      </c>
+      <c r="G30" s="409" t="str">
+        <f aca="false">A54</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H30" s="409" t="str">
+        <f aca="false">A55</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :muulampo]</v>
+      </c>
+      <c r="I30" s="410" t="str">
+        <f aca="false">A56</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J30" s="408" t="str">
+        <f aca="false">A57</f>
+        <v>[:tulokset :kuukausierittely 4 :kulutus :sahko]</v>
+      </c>
+      <c r="K30" s="410" t="str">
+        <f aca="false">A58</f>
+        <v>[:tulokset :kuukausierittely 4 :kulutus :lampo]</v>
+      </c>
+      <c r="L30" s="408" t="str">
+        <f aca="false">A59</f>
+        <v>[:tulokset :kuukausierittely 4 :hyoty :sahko]</v>
+      </c>
+      <c r="M30" s="410" t="str">
+        <f aca="false">A60</f>
+        <v>[:tulokset :kuukausierittely 4 :hyoty :lampo]</v>
+      </c>
+      <c r="N30" s="396"/>
+    </row>
+    <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="366" t="s">
+        <v>654</v>
+      </c>
+      <c r="B31" s="394"/>
+      <c r="C31" s="407" t="s">
+        <v>655</v>
+      </c>
+      <c r="D31" s="408" t="str">
+        <f aca="false">A61</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E31" s="409" t="str">
+        <f aca="false">A62</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F31" s="409" t="str">
+        <f aca="false">A63</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :muusahko]</v>
+      </c>
+      <c r="G31" s="409" t="str">
+        <f aca="false">A64</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H31" s="409" t="str">
+        <f aca="false">A65</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :muulampo]</v>
+      </c>
+      <c r="I31" s="410" t="str">
+        <f aca="false">A66</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J31" s="408" t="str">
+        <f aca="false">A67</f>
+        <v>[:tulokset :kuukausierittely 5 :kulutus :sahko]</v>
+      </c>
+      <c r="K31" s="410" t="str">
+        <f aca="false">A68</f>
+        <v>[:tulokset :kuukausierittely 5 :kulutus :lampo]</v>
+      </c>
+      <c r="L31" s="408" t="str">
+        <f aca="false">A69</f>
+        <v>[:tulokset :kuukausierittely 5 :hyoty :sahko]</v>
+      </c>
+      <c r="M31" s="410" t="str">
+        <f aca="false">A70</f>
+        <v>[:tulokset :kuukausierittely 5 :hyoty :lampo]</v>
+      </c>
+      <c r="N31" s="396"/>
+    </row>
+    <row r="32" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="366" t="s">
+        <v>656</v>
+      </c>
+      <c r="B32" s="394"/>
+      <c r="C32" s="407" t="s">
+        <v>657</v>
+      </c>
+      <c r="D32" s="408" t="str">
+        <f aca="false">A71</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E32" s="409" t="str">
+        <f aca="false">A72</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F32" s="409" t="str">
+        <f aca="false">A73</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :muusahko]</v>
+      </c>
+      <c r="G32" s="409" t="str">
+        <f aca="false">A74</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H32" s="409" t="str">
+        <f aca="false">A75</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :muulampo]</v>
+      </c>
+      <c r="I32" s="410" t="str">
+        <f aca="false">A76</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J32" s="408" t="str">
+        <f aca="false">A77</f>
+        <v>[:tulokset :kuukausierittely 6 :kulutus :sahko]</v>
+      </c>
+      <c r="K32" s="410" t="str">
+        <f aca="false">A78</f>
+        <v>[:tulokset :kuukausierittely 6 :kulutus :lampo]</v>
+      </c>
+      <c r="L32" s="408" t="str">
+        <f aca="false">A79</f>
+        <v>[:tulokset :kuukausierittely 6 :hyoty :sahko]</v>
+      </c>
+      <c r="M32" s="410" t="str">
+        <f aca="false">A80</f>
+        <v>[:tulokset :kuukausierittely 6 :hyoty :lampo]</v>
+      </c>
+      <c r="N32" s="396"/>
+    </row>
+    <row r="33" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="366" t="s">
+        <v>658</v>
+      </c>
+      <c r="B33" s="394"/>
+      <c r="C33" s="407" t="s">
+        <v>659</v>
+      </c>
+      <c r="D33" s="408" t="str">
+        <f aca="false">A81</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E33" s="409" t="str">
+        <f aca="false">A82</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F33" s="409" t="str">
+        <f aca="false">A83</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :muusahko]</v>
+      </c>
+      <c r="G33" s="409" t="str">
+        <f aca="false">A84</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H33" s="409" t="str">
+        <f aca="false">A85</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :muulampo]</v>
+      </c>
+      <c r="I33" s="410" t="str">
+        <f aca="false">A86</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J33" s="408" t="str">
+        <f aca="false">A87</f>
+        <v>[:tulokset :kuukausierittely 7 :kulutus :sahko]</v>
+      </c>
+      <c r="K33" s="410" t="str">
+        <f aca="false">A88</f>
+        <v>[:tulokset :kuukausierittely 7 :kulutus :lampo]</v>
+      </c>
+      <c r="L33" s="408" t="str">
+        <f aca="false">A89</f>
+        <v>[:tulokset :kuukausierittely 7 :hyoty :sahko]</v>
+      </c>
+      <c r="M33" s="410" t="str">
+        <f aca="false">A90</f>
+        <v>[:tulokset :kuukausierittely 7 :hyoty :lampo]</v>
+      </c>
+      <c r="N33" s="396"/>
+    </row>
+    <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="366" t="s">
+        <v>660</v>
+      </c>
+      <c r="B34" s="394"/>
+      <c r="C34" s="407" t="s">
+        <v>661</v>
+      </c>
+      <c r="D34" s="408" t="str">
+        <f aca="false">A91</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E34" s="409" t="str">
+        <f aca="false">A92</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F34" s="409" t="str">
+        <f aca="false">A93</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :muusahko]</v>
+      </c>
+      <c r="G34" s="409" t="str">
+        <f aca="false">A94</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H34" s="409" t="str">
+        <f aca="false">A95</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :muulampo]</v>
+      </c>
+      <c r="I34" s="410" t="str">
+        <f aca="false">A96</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J34" s="408" t="str">
+        <f aca="false">A97</f>
+        <v>[:tulokset :kuukausierittely 8 :kulutus :sahko]</v>
+      </c>
+      <c r="K34" s="410" t="str">
+        <f aca="false">A98</f>
+        <v>[:tulokset :kuukausierittely 8 :kulutus :lampo]</v>
+      </c>
+      <c r="L34" s="408" t="str">
+        <f aca="false">A99</f>
+        <v>[:tulokset :kuukausierittely 8 :hyoty :sahko]</v>
+      </c>
+      <c r="M34" s="410" t="str">
+        <f aca="false">A100</f>
+        <v>[:tulokset :kuukausierittely 8 :hyoty :lampo]</v>
+      </c>
+      <c r="N34" s="396"/>
+    </row>
+    <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="366" t="s">
+        <v>662</v>
+      </c>
+      <c r="B35" s="394"/>
+      <c r="C35" s="407" t="s">
+        <v>663</v>
+      </c>
+      <c r="D35" s="408" t="str">
+        <f aca="false">A101</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E35" s="409" t="str">
+        <f aca="false">A102</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F35" s="409" t="str">
+        <f aca="false">A103</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :muusahko]</v>
+      </c>
+      <c r="G35" s="409" t="str">
+        <f aca="false">A104</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H35" s="409" t="str">
+        <f aca="false">A105</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :muulampo]</v>
+      </c>
+      <c r="I35" s="410" t="str">
+        <f aca="false">A106</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J35" s="408" t="str">
+        <f aca="false">A107</f>
+        <v>[:tulokset :kuukausierittely 9 :kulutus :sahko]</v>
+      </c>
+      <c r="K35" s="410" t="str">
+        <f aca="false">A108</f>
+        <v>[:tulokset :kuukausierittely 9 :kulutus :lampo]</v>
+      </c>
+      <c r="L35" s="408" t="str">
+        <f aca="false">A109</f>
+        <v>[:tulokset :kuukausierittely 9 :hyoty :sahko]</v>
+      </c>
+      <c r="M35" s="410" t="str">
+        <f aca="false">A110</f>
+        <v>[:tulokset :kuukausierittely 9 :hyoty :lampo]</v>
+      </c>
+      <c r="N35" s="396"/>
+    </row>
+    <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="366" t="s">
+        <v>664</v>
+      </c>
+      <c r="B36" s="394"/>
+      <c r="C36" s="407" t="s">
+        <v>665</v>
+      </c>
+      <c r="D36" s="408" t="str">
+        <f aca="false">A111</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E36" s="409" t="str">
+        <f aca="false">A112</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F36" s="409" t="str">
+        <f aca="false">A113</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :muusahko]</v>
+      </c>
+      <c r="G36" s="409" t="str">
+        <f aca="false">A114</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H36" s="409" t="str">
+        <f aca="false">A115</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :muulampo]</v>
+      </c>
+      <c r="I36" s="410" t="str">
+        <f aca="false">A116</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J36" s="408" t="str">
+        <f aca="false">A117</f>
+        <v>[:tulokset :kuukausierittely 10 :kulutus :sahko]</v>
+      </c>
+      <c r="K36" s="410" t="str">
+        <f aca="false">A118</f>
+        <v>[:tulokset :kuukausierittely 10 :kulutus :lampo]</v>
+      </c>
+      <c r="L36" s="408" t="str">
+        <f aca="false">A119</f>
+        <v>[:tulokset :kuukausierittely 10 :hyoty :sahko]</v>
+      </c>
+      <c r="M36" s="410" t="str">
+        <f aca="false">A120</f>
+        <v>[:tulokset :kuukausierittely 10 :hyoty :lampo]</v>
+      </c>
+      <c r="N36" s="396"/>
+    </row>
+    <row r="37" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="366" t="s">
+        <v>666</v>
+      </c>
+      <c r="B37" s="394"/>
+      <c r="C37" s="411" t="s">
+        <v>667</v>
+      </c>
+      <c r="D37" s="412" t="str">
+        <f aca="false">A121</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E37" s="413" t="str">
+        <f aca="false">A122</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F37" s="413" t="str">
+        <f aca="false">A123</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :muusahko]</v>
+      </c>
+      <c r="G37" s="413" t="str">
+        <f aca="false">A124</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H37" s="413" t="str">
+        <f aca="false">A125</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :muulampo]</v>
+      </c>
+      <c r="I37" s="414" t="str">
+        <f aca="false">A126</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="J37" s="412" t="str">
+        <f aca="false">A127</f>
+        <v>[:tulokset :kuukausierittely 11 :kulutus :sahko]</v>
+      </c>
+      <c r="K37" s="414" t="str">
+        <f aca="false">A128</f>
+        <v>[:tulokset :kuukausierittely 11 :kulutus :lampo]</v>
+      </c>
+      <c r="L37" s="412" t="str">
+        <f aca="false">A129</f>
+        <v>[:tulokset :kuukausierittely 11 :hyoty :sahko]</v>
+      </c>
+      <c r="M37" s="414" t="str">
+        <f aca="false">A130</f>
+        <v>[:tulokset :kuukausierittely 11 :hyoty :lampo]</v>
+      </c>
+      <c r="N37" s="396"/>
+    </row>
+    <row r="38" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="366" t="s">
+        <v>668</v>
+      </c>
+      <c r="B38" s="394"/>
+      <c r="C38" s="395"/>
+      <c r="D38" s="395"/>
+      <c r="E38" s="395"/>
+      <c r="F38" s="395"/>
+      <c r="G38" s="395"/>
+      <c r="H38" s="395"/>
+      <c r="I38" s="395"/>
+      <c r="J38" s="395"/>
+      <c r="K38" s="395"/>
+      <c r="L38" s="395"/>
+      <c r="M38" s="395"/>
+      <c r="N38" s="396"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="366" t="s">
+        <v>669</v>
+      </c>
+      <c r="B39" s="393" t="s">
+        <v>670</v>
+      </c>
+      <c r="C39" s="393"/>
+      <c r="D39" s="393"/>
+      <c r="E39" s="393"/>
+      <c r="F39" s="393"/>
+      <c r="G39" s="393"/>
+      <c r="H39" s="393"/>
+      <c r="I39" s="393"/>
+      <c r="J39" s="393"/>
+      <c r="K39" s="393"/>
+      <c r="L39" s="393"/>
+      <c r="M39" s="393"/>
+      <c r="N39" s="393"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="366" t="s">
+        <v>671</v>
+      </c>
+      <c r="B40" s="393"/>
+      <c r="C40" s="393"/>
+      <c r="D40" s="393"/>
+      <c r="E40" s="393"/>
+      <c r="F40" s="393"/>
+      <c r="G40" s="393"/>
+      <c r="H40" s="393"/>
+      <c r="I40" s="393"/>
+      <c r="J40" s="393"/>
+      <c r="K40" s="393"/>
+      <c r="L40" s="393"/>
+      <c r="M40" s="393"/>
+      <c r="N40" s="393"/>
+    </row>
+    <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="366" t="s">
+        <v>672</v>
+      </c>
+      <c r="B41" s="394"/>
+      <c r="C41" s="395"/>
+      <c r="D41" s="395"/>
+      <c r="E41" s="395"/>
+      <c r="F41" s="395"/>
+      <c r="G41" s="395"/>
+      <c r="H41" s="395"/>
+      <c r="I41" s="395"/>
+      <c r="J41" s="395"/>
+      <c r="K41" s="395"/>
+      <c r="L41" s="395"/>
+      <c r="M41" s="395"/>
+      <c r="N41" s="396"/>
+    </row>
+    <row r="42" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="366" t="s">
+        <v>673</v>
+      </c>
+      <c r="B42" s="394"/>
+      <c r="C42" s="415" t="s">
+        <v>674</v>
+      </c>
+      <c r="D42" s="415"/>
+      <c r="E42" s="415"/>
+      <c r="F42" s="415"/>
+      <c r="G42" s="416" t="str">
+        <f aca="false">A4</f>
+        <v>[:lahtotiedot :rakennusvaippa :lampokapasiteetti]</v>
+      </c>
+      <c r="H42" s="416"/>
+      <c r="I42" s="417"/>
+      <c r="J42" s="395"/>
+      <c r="K42" s="395"/>
+      <c r="L42" s="395"/>
+      <c r="M42" s="395"/>
+      <c r="N42" s="396"/>
+    </row>
+    <row r="43" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="366" t="s">
+        <v>675</v>
+      </c>
+      <c r="B43" s="394"/>
+      <c r="C43" s="415" t="s">
+        <v>676</v>
+      </c>
+      <c r="D43" s="415"/>
+      <c r="E43" s="415"/>
+      <c r="F43" s="415"/>
+      <c r="G43" s="416" t="str">
+        <f aca="false">A5</f>
+        <v>[:lahtotiedot :rakennusvaippa :ilmatilavuus]</v>
+      </c>
+      <c r="H43" s="416"/>
+      <c r="I43" s="417"/>
+      <c r="J43" s="395"/>
+      <c r="K43" s="395"/>
+      <c r="L43" s="395"/>
+      <c r="M43" s="395"/>
+      <c r="N43" s="396"/>
+    </row>
+    <row r="44" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="366" t="s">
+        <v>677</v>
+      </c>
+      <c r="B44" s="394"/>
+      <c r="C44" s="418" t="s">
+        <v>678</v>
+      </c>
+      <c r="D44" s="418"/>
+      <c r="E44" s="418"/>
+      <c r="F44" s="418"/>
+      <c r="G44" s="416" t="str">
+        <f aca="false">A6</f>
+        <v>[:lahtotiedot :ilmanvaihto :tuloilma-lampotila]</v>
+      </c>
+      <c r="H44" s="416"/>
+      <c r="I44" s="417"/>
+      <c r="J44" s="395"/>
+      <c r="K44" s="395"/>
+      <c r="L44" s="395"/>
+      <c r="M44" s="395"/>
+      <c r="N44" s="396"/>
+    </row>
+    <row r="45" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="366" t="s">
+        <v>679</v>
+      </c>
+      <c r="B45" s="394"/>
+      <c r="C45" s="418" t="s">
+        <v>680</v>
+      </c>
+      <c r="D45" s="418"/>
+      <c r="E45" s="418"/>
+      <c r="F45" s="418"/>
+      <c r="G45" s="416" t="str">
+        <f aca="false">A7</f>
+        <v>[:lahtotiedot :lammitys :tilat-ja-iv :lampopumppu-tuotto-osuus]</v>
+      </c>
+      <c r="H45" s="416"/>
+      <c r="I45" s="417"/>
+      <c r="J45" s="395"/>
+      <c r="K45" s="395"/>
+      <c r="L45" s="395"/>
+      <c r="M45" s="395"/>
+      <c r="N45" s="396"/>
+    </row>
+    <row r="46" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="366" t="s">
+        <v>681</v>
+      </c>
+      <c r="B46" s="394"/>
+      <c r="C46" s="418" t="s">
+        <v>682</v>
+      </c>
+      <c r="D46" s="418"/>
+      <c r="E46" s="418"/>
+      <c r="F46" s="418"/>
+      <c r="G46" s="416" t="str">
+        <f aca="false">A8</f>
+        <v>[:lahtotiedot :lammitys :lammin-kayttovesi :lampopumppu-tuotto-osuus]</v>
+      </c>
+      <c r="H46" s="416"/>
+      <c r="I46" s="417"/>
+      <c r="J46" s="395"/>
+      <c r="K46" s="395"/>
+      <c r="L46" s="395"/>
+      <c r="M46" s="395"/>
+      <c r="N46" s="396"/>
+    </row>
+    <row r="47" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="366" t="s">
+        <v>683</v>
+      </c>
+      <c r="B47" s="394"/>
+      <c r="C47" s="418" t="s">
+        <v>684</v>
+      </c>
+      <c r="D47" s="418"/>
+      <c r="E47" s="418"/>
+      <c r="F47" s="418"/>
+      <c r="G47" s="416" t="str">
+        <f aca="false">A9</f>
+        <v>[:lahtotiedot :lammitys :tilat-ja-iv :lampohavio-lammittamaton-tila]</v>
+      </c>
+      <c r="H47" s="416"/>
+      <c r="I47" s="417"/>
+      <c r="J47" s="395"/>
+      <c r="K47" s="395"/>
+      <c r="L47" s="395"/>
+      <c r="M47" s="395"/>
+      <c r="N47" s="396"/>
+    </row>
+    <row r="48" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="366" t="s">
+        <v>685</v>
+      </c>
+      <c r="B48" s="394"/>
+      <c r="C48" s="0"/>
+      <c r="D48" s="0"/>
+      <c r="E48" s="0"/>
+      <c r="F48" s="0"/>
+      <c r="G48" s="0"/>
+      <c r="H48" s="0"/>
+      <c r="I48" s="417"/>
+      <c r="J48" s="395"/>
+      <c r="K48" s="395"/>
+      <c r="L48" s="395"/>
+      <c r="M48" s="395"/>
+      <c r="N48" s="396"/>
+    </row>
+    <row r="49" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="366" t="s">
+        <v>686</v>
+      </c>
+      <c r="B49" s="394"/>
+      <c r="C49" s="0"/>
+      <c r="D49" s="0"/>
+      <c r="E49" s="0"/>
+      <c r="F49" s="0"/>
+      <c r="G49" s="0"/>
+      <c r="H49" s="0"/>
+      <c r="I49" s="417"/>
+      <c r="J49" s="395"/>
+      <c r="K49" s="395"/>
+      <c r="L49" s="395"/>
+      <c r="M49" s="395"/>
+      <c r="N49" s="396"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="366" t="s">
+        <v>687</v>
+      </c>
+      <c r="B50" s="394"/>
+      <c r="C50" s="395"/>
+      <c r="D50" s="395"/>
+      <c r="E50" s="395"/>
+      <c r="F50" s="395"/>
+      <c r="G50" s="395"/>
+      <c r="H50" s="395"/>
+      <c r="I50" s="395"/>
+      <c r="J50" s="395"/>
+      <c r="K50" s="395"/>
+      <c r="L50" s="395"/>
+      <c r="M50" s="395"/>
+      <c r="N50" s="396"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="366" t="s">
+        <v>688</v>
+      </c>
+      <c r="B51" s="394"/>
+      <c r="C51" s="395"/>
+      <c r="D51" s="395"/>
+      <c r="E51" s="395"/>
+      <c r="F51" s="395"/>
+      <c r="G51" s="395"/>
+      <c r="H51" s="395"/>
+      <c r="I51" s="395"/>
+      <c r="J51" s="395"/>
+      <c r="K51" s="395"/>
+      <c r="L51" s="395"/>
+      <c r="M51" s="395"/>
+      <c r="N51" s="396"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="366" t="s">
+        <v>689</v>
+      </c>
+      <c r="B52" s="394"/>
+      <c r="C52" s="395"/>
+      <c r="D52" s="395"/>
+      <c r="E52" s="395"/>
+      <c r="F52" s="395"/>
+      <c r="G52" s="395"/>
+      <c r="H52" s="395"/>
+      <c r="I52" s="395"/>
+      <c r="J52" s="395"/>
+      <c r="K52" s="395"/>
+      <c r="L52" s="395"/>
+      <c r="M52" s="395"/>
+      <c r="N52" s="396"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="366" t="s">
+        <v>690</v>
+      </c>
+      <c r="B53" s="394"/>
+      <c r="C53" s="395"/>
+      <c r="D53" s="395"/>
+      <c r="E53" s="395"/>
+      <c r="F53" s="395"/>
+      <c r="G53" s="395"/>
+      <c r="H53" s="395"/>
+      <c r="I53" s="395"/>
+      <c r="J53" s="395"/>
+      <c r="K53" s="395"/>
+      <c r="L53" s="395"/>
+      <c r="M53" s="395"/>
+      <c r="N53" s="396"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="366" t="s">
+        <v>691</v>
+      </c>
+      <c r="B54" s="394"/>
+      <c r="C54" s="395"/>
+      <c r="D54" s="395"/>
+      <c r="E54" s="395"/>
+      <c r="F54" s="395"/>
+      <c r="G54" s="395"/>
+      <c r="H54" s="395"/>
+      <c r="I54" s="395"/>
+      <c r="J54" s="395"/>
+      <c r="K54" s="395"/>
+      <c r="L54" s="395"/>
+      <c r="M54" s="395"/>
+      <c r="N54" s="396"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="366" t="s">
+        <v>692</v>
+      </c>
+      <c r="B55" s="394"/>
+      <c r="C55" s="395"/>
+      <c r="D55" s="395"/>
+      <c r="E55" s="395"/>
+      <c r="F55" s="395"/>
+      <c r="G55" s="395"/>
+      <c r="H55" s="395"/>
+      <c r="I55" s="395"/>
+      <c r="J55" s="395"/>
+      <c r="K55" s="395"/>
+      <c r="L55" s="395"/>
+      <c r="M55" s="395"/>
+      <c r="N55" s="396"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="366" t="s">
+        <v>693</v>
+      </c>
+      <c r="B56" s="394"/>
+      <c r="C56" s="395"/>
+      <c r="D56" s="395"/>
+      <c r="E56" s="395"/>
+      <c r="F56" s="395"/>
+      <c r="G56" s="395"/>
+      <c r="H56" s="395"/>
+      <c r="I56" s="395"/>
+      <c r="J56" s="395"/>
+      <c r="K56" s="395"/>
+      <c r="L56" s="395"/>
+      <c r="M56" s="395"/>
+      <c r="N56" s="396"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="366" t="s">
+        <v>694</v>
+      </c>
+      <c r="B57" s="394"/>
+      <c r="C57" s="395"/>
+      <c r="D57" s="395"/>
+      <c r="E57" s="395"/>
+      <c r="F57" s="395"/>
+      <c r="G57" s="395"/>
+      <c r="H57" s="395"/>
+      <c r="I57" s="395"/>
+      <c r="J57" s="395"/>
+      <c r="K57" s="395"/>
+      <c r="L57" s="395"/>
+      <c r="M57" s="395"/>
+      <c r="N57" s="396"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="366" t="s">
+        <v>695</v>
+      </c>
+      <c r="B58" s="394"/>
+      <c r="C58" s="395"/>
+      <c r="D58" s="395"/>
+      <c r="E58" s="395"/>
+      <c r="F58" s="395"/>
+      <c r="G58" s="395"/>
+      <c r="H58" s="395"/>
+      <c r="I58" s="395"/>
+      <c r="J58" s="395"/>
+      <c r="K58" s="395"/>
+      <c r="L58" s="395"/>
+      <c r="M58" s="395"/>
+      <c r="N58" s="396"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="366" t="s">
+        <v>696</v>
+      </c>
+      <c r="B59" s="394"/>
+      <c r="C59" s="395"/>
+      <c r="D59" s="395"/>
+      <c r="E59" s="395"/>
+      <c r="F59" s="395"/>
+      <c r="G59" s="395"/>
+      <c r="H59" s="395"/>
+      <c r="I59" s="395"/>
+      <c r="J59" s="395"/>
+      <c r="K59" s="395"/>
+      <c r="L59" s="395"/>
+      <c r="M59" s="395"/>
+      <c r="N59" s="396"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="366" t="s">
+        <v>697</v>
+      </c>
+      <c r="B60" s="394"/>
+      <c r="C60" s="395"/>
+      <c r="D60" s="395"/>
+      <c r="E60" s="395"/>
+      <c r="F60" s="395"/>
+      <c r="G60" s="395"/>
+      <c r="H60" s="395"/>
+      <c r="I60" s="395"/>
+      <c r="J60" s="395"/>
+      <c r="K60" s="395"/>
+      <c r="L60" s="395"/>
+      <c r="M60" s="395"/>
+      <c r="N60" s="396"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="366" t="s">
+        <v>698</v>
+      </c>
+      <c r="B61" s="419"/>
+      <c r="C61" s="420"/>
+      <c r="D61" s="420"/>
+      <c r="E61" s="420"/>
+      <c r="F61" s="420"/>
+      <c r="G61" s="420"/>
+      <c r="H61" s="420"/>
+      <c r="I61" s="420"/>
+      <c r="J61" s="420"/>
+      <c r="K61" s="420"/>
+      <c r="L61" s="420"/>
+      <c r="M61" s="420"/>
+      <c r="N61" s="421"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="393" t="str">
+      <c r="A62" s="366" t="s">
+        <v>699</v>
+      </c>
+      <c r="B62" s="422" t="str">
         <f aca="false">"Todistustunnus: "&amp;A1&amp;", 8/8"</f>
         <v>Todistustunnus: [:id], 8/8</v>
       </c>
-      <c r="C62" s="393"/>
-      <c r="D62" s="393"/>
-      <c r="E62" s="393"/>
-      <c r="F62" s="393"/>
-      <c r="G62" s="393"/>
-      <c r="H62" s="393"/>
+      <c r="C62" s="422"/>
+      <c r="D62" s="422"/>
+      <c r="E62" s="422"/>
+      <c r="F62" s="422"/>
+      <c r="G62" s="422"/>
+      <c r="H62" s="422"/>
+      <c r="I62" s="422"/>
+      <c r="J62" s="422"/>
+      <c r="K62" s="422"/>
+      <c r="L62" s="422"/>
+      <c r="M62" s="422"/>
+      <c r="N62" s="422"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="393"/>
-      <c r="C63" s="393"/>
-      <c r="D63" s="393"/>
-      <c r="E63" s="393"/>
-      <c r="F63" s="393"/>
-      <c r="G63" s="393"/>
-      <c r="H63" s="393"/>
+      <c r="A63" s="366" t="s">
+        <v>700</v>
+      </c>
+      <c r="B63" s="422"/>
+      <c r="C63" s="422"/>
+      <c r="D63" s="422"/>
+      <c r="E63" s="422"/>
+      <c r="F63" s="422"/>
+      <c r="G63" s="422"/>
+      <c r="H63" s="422"/>
+      <c r="I63" s="422"/>
+      <c r="J63" s="422"/>
+      <c r="K63" s="422"/>
+      <c r="L63" s="422"/>
+      <c r="M63" s="422"/>
+      <c r="N63" s="422"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="366" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="366" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="366" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="366" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="366" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="366" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="366" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="366" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="366" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="366" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="366" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="366" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="366" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="366" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="366" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="366" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="366" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="366" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="366" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="366" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="366" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="366" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="366" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="366" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="366" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="366" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="366" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="366" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="366" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="366" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="366" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="366" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="366" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="366" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="366" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="366" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="366" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="366" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="366" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="366" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="366" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="366" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="366" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="366" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="366" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="366" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="366" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="366" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="366" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="366" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="366" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="366" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="366" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="366" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="366" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="366" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="366" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="366" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="366" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="366" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="366" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="366" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="366" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="366" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="366" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="366" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="366" t="s">
+        <v>767</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H61"/>
-    <mergeCell ref="B62:H63"/>
+  <mergeCells count="17">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N20"/>
+    <mergeCell ref="B21:N22"/>
+    <mergeCell ref="B39:N40"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="B62:N63"/>
   </mergeCells>
-  <conditionalFormatting sqref="I2:AMJ2 B2 A3:AMJ1048576">
+  <conditionalFormatting sqref="O2:AMJ19 B2:C2 A3:N19 A20:AMJ43 A50:AMJ1048576 A44:B49 I44:AMJ45 I46:AMJ49 D44:H47">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="356">
       <formula>"*"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fix typos in cell wrap related issues in energiatodistus templates
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,23 +19,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'1) etusivu'!$B$1:$R$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$N$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$B$1:$R$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$66</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$L$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$O$62</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -204,7 +204,7 @@
     <t xml:space="preserve">Uuden rakennuksen E-luvun vaatimus</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;</t>
+    <t xml:space="preserve">≤</t>
   </si>
   <si>
     <t xml:space="preserve">Todistuksen laatija:</t>
@@ -2101,6 +2101,7 @@
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">m</t>
     </r>
@@ -2112,6 +2113,7 @@
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -3337,7 +3339,7 @@
     <numFmt numFmtId="173" formatCode="0%"/>
     <numFmt numFmtId="174" formatCode="0"/>
   </numFmts>
-  <fonts count="47">
+  <fonts count="45">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3630,21 +3632,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4292,9 +4279,9 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
@@ -5356,11 +5343,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5484,7 +5471,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="42" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5556,11 +5543,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5576,11 +5563,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5596,7 +5583,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="44" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5828,7 +5815,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="46" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="44" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8494,9 +8481,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>232560</xdr:colOff>
+      <xdr:colOff>232200</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>246960</xdr:rowOff>
+      <xdr:rowOff>246600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8510,7 +8497,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4656960"/>
-          <a:ext cx="742680" cy="199440"/>
+          <a:ext cx="742320" cy="199080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8531,9 +8518,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>132480</xdr:colOff>
+      <xdr:colOff>132120</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>246960</xdr:rowOff>
+      <xdr:rowOff>246600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8547,7 +8534,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4971240"/>
-          <a:ext cx="1086120" cy="199440"/>
+          <a:ext cx="1085760" cy="199080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8568,9 +8555,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
+      <xdr:colOff>5400</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>246960</xdr:rowOff>
+      <xdr:rowOff>246600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8584,7 +8571,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5285520"/>
-          <a:ext cx="1392840" cy="199440"/>
+          <a:ext cx="1392480" cy="199080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8605,9 +8592,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>329760</xdr:colOff>
+      <xdr:colOff>329400</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>246960</xdr:rowOff>
+      <xdr:rowOff>246600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8621,7 +8608,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5599800"/>
-          <a:ext cx="1716840" cy="199440"/>
+          <a:ext cx="1716480" cy="199080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8642,9 +8629,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>203040</xdr:colOff>
+      <xdr:colOff>202680</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>259920</xdr:rowOff>
+      <xdr:rowOff>259560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8658,7 +8645,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5909760"/>
-          <a:ext cx="2023920" cy="212400"/>
+          <a:ext cx="2023560" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8679,9 +8666,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>146160</xdr:colOff>
+      <xdr:colOff>145800</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>246960</xdr:rowOff>
+      <xdr:rowOff>246600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8695,7 +8682,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6219720"/>
-          <a:ext cx="2360160" cy="199440"/>
+          <a:ext cx="2359800" cy="199080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8716,9 +8703,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>86400</xdr:colOff>
+      <xdr:colOff>86040</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>248040</xdr:rowOff>
+      <xdr:rowOff>247680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8728,7 +8715,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6531480"/>
-          <a:ext cx="2673000" cy="198360"/>
+          <a:ext cx="2672640" cy="198000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9097,9 +9084,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>285840</xdr:colOff>
+      <xdr:colOff>285480</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9109,7 +9096,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1978200" y="78480"/>
-          <a:ext cx="6972120" cy="10493640"/>
+          <a:ext cx="6971760" cy="10493280"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9238,8 +9225,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9791,7 +9778,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="0"/>
-      <c r="K14" s="27" t="str">
+      <c r="K14" s="34" t="str">
         <f aca="false">A8</f>
         <v>[:perustiedot :alakayttotarkoitus-fi]</v>
       </c>
@@ -9816,7 +9803,7 @@
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
+      <c r="K15" s="34"/>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
@@ -10445,7 +10432,7 @@
       <c r="Q36" s="60"/>
       <c r="R36" s="6"/>
     </row>
-    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="3"/>
       <c r="C37" s="60"/>
       <c r="D37" s="61"/>
@@ -10759,8 +10746,9 @@
       <c r="L52" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
     <mergeCell ref="C3:Q3"/>
+    <mergeCell ref="K14:O15"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="F25:N25"/>
     <mergeCell ref="D26:E26"/>
@@ -16975,7 +16963,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
     </sheetView>
   </sheetViews>
@@ -16983,8 +16971,8 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="97" width="49.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="98" width="1.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="98" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="98" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="98" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="98" width="7.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="98" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="98" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="98" width="2.31"/>

</xml_diff>

<commit_message>
AE-651 / AE-762 fix label and first page layout issue in pdf
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,23 +19,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'1) etusivu'!$B$1:$R$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$M$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$B$1:$R$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$66</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$L$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$N$62</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0" vbProcedure="false">'8) lisämerkintöjä'!$B$1:$M$63</definedName>
   </definedNames>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="782">
   <si>
     <t xml:space="preserve">[:id]</t>
   </si>
@@ -1227,6 +1227,9 @@
   </si>
   <si>
     <t xml:space="preserve">kpl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kWh</t>
   </si>
   <si>
     <t xml:space="preserve">[:lahtotiedot :ikkunat :luode :ala]</t>
@@ -5832,7 +5835,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="44" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="44" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -6074,7 +6077,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF99"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6084,7 +6087,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6114,7 +6117,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF99"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6124,7 +6127,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8634,9 +8637,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>230040</xdr:colOff>
+      <xdr:colOff>229680</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>244440</xdr:rowOff>
+      <xdr:rowOff>244080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8650,7 +8653,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4656960"/>
-          <a:ext cx="740160" cy="196920"/>
+          <a:ext cx="739800" cy="196560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8671,9 +8674,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>129960</xdr:colOff>
+      <xdr:colOff>129600</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>244440</xdr:rowOff>
+      <xdr:rowOff>244080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8687,7 +8690,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4971240"/>
-          <a:ext cx="1083600" cy="196920"/>
+          <a:ext cx="1083240" cy="196560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8708,9 +8711,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>3240</xdr:colOff>
+      <xdr:colOff>2880</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>244440</xdr:rowOff>
+      <xdr:rowOff>244080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8724,7 +8727,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5285520"/>
-          <a:ext cx="1390320" cy="196920"/>
+          <a:ext cx="1389960" cy="196560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8745,9 +8748,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>327240</xdr:colOff>
+      <xdr:colOff>326880</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>244440</xdr:rowOff>
+      <xdr:rowOff>244080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8761,7 +8764,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5599800"/>
-          <a:ext cx="1714320" cy="196920"/>
+          <a:ext cx="1713960" cy="196560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8782,9 +8785,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>200520</xdr:colOff>
+      <xdr:colOff>200160</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8798,7 +8801,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5909760"/>
-          <a:ext cx="2021400" cy="209880"/>
+          <a:ext cx="2021040" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8819,9 +8822,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>143640</xdr:colOff>
+      <xdr:colOff>143280</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>244440</xdr:rowOff>
+      <xdr:rowOff>244080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8835,7 +8838,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6219720"/>
-          <a:ext cx="2357640" cy="196920"/>
+          <a:ext cx="2357280" cy="196560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8856,9 +8859,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>83880</xdr:colOff>
+      <xdr:colOff>83520</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>245520</xdr:rowOff>
+      <xdr:rowOff>245160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8868,7 +8871,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6531480"/>
-          <a:ext cx="2670480" cy="195840"/>
+          <a:ext cx="2670120" cy="195480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9237,9 +9240,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>283320</xdr:colOff>
+      <xdr:colOff>282960</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9249,7 +9252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1978200" y="78480"/>
-          <a:ext cx="6969600" cy="10491120"/>
+          <a:ext cx="6969240" cy="10490760"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9378,8 +9381,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9553,11 +9556,11 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="0"/>
-      <c r="K7" s="5" t="str">
+      <c r="J7" s="5" t="str">
         <f aca="false">A2</f>
         <v>[:perustiedot :nimi]</v>
       </c>
+      <c r="K7" s="0"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -9612,11 +9615,11 @@
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
-      <c r="J8" s="0"/>
-      <c r="K8" s="20" t="str">
+      <c r="J8" s="20" t="str">
         <f aca="false">A3</f>
         <v>[:perustiedot :katuosoite-fi]</v>
       </c>
+      <c r="K8" s="0"/>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="20"/>
@@ -9671,11 +9674,11 @@
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
-      <c r="J9" s="0"/>
-      <c r="K9" s="20" t="str">
+      <c r="J9" s="20" t="str">
         <f aca="false">A5</f>
         <v>#function[solita.etp.service.energiatodistus-pdf/fn--55811]</v>
       </c>
+      <c r="K9" s="0"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="20"/>
@@ -9842,11 +9845,11 @@
       </c>
       <c r="F12" s="24"/>
       <c r="I12" s="26"/>
-      <c r="J12" s="0"/>
-      <c r="K12" s="27" t="str">
+      <c r="J12" s="27" t="str">
         <f aca="false">A6</f>
         <v>[:perustiedot :rakennustunnus]</v>
       </c>
+      <c r="K12" s="0"/>
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
       <c r="N12" s="27"/>
@@ -9903,11 +9906,11 @@
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
       <c r="I13" s="26"/>
-      <c r="J13" s="0"/>
-      <c r="K13" s="27" t="str">
+      <c r="J13" s="27" t="str">
         <f aca="false">A7</f>
         <v>[:perustiedot :valmistumisvuosi]</v>
       </c>
+      <c r="K13" s="0"/>
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
@@ -9930,11 +9933,11 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="0"/>
-      <c r="K14" s="34" t="str">
+      <c r="J14" s="34" t="str">
         <f aca="false">A8</f>
         <v>[:perustiedot :alakayttotarkoitus-fi]</v>
       </c>
+      <c r="K14" s="34"/>
       <c r="L14" s="34"/>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
@@ -9955,7 +9958,7 @@
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
+      <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
@@ -9977,11 +9980,11 @@
       </c>
       <c r="F16" s="24"/>
       <c r="I16" s="26"/>
-      <c r="J16" s="0"/>
-      <c r="K16" s="27" t="str">
+      <c r="J16" s="27" t="str">
         <f aca="false">A1</f>
         <v>[:id]</v>
       </c>
+      <c r="K16" s="0"/>
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
       <c r="N16" s="27"/>
@@ -10901,7 +10904,7 @@
   </sheetData>
   <mergeCells count="24">
     <mergeCell ref="C3:Q3"/>
-    <mergeCell ref="K14:O15"/>
+    <mergeCell ref="J14:O15"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="F25:N25"/>
     <mergeCell ref="D26:E26"/>
@@ -10925,7 +10928,7 @@
     <mergeCell ref="C50:I50"/>
     <mergeCell ref="L50:N50"/>
   </mergeCells>
-  <conditionalFormatting sqref="G24:K24 C25:I31 C24 F32:I32 C32 C4:K4 C5:L5 C33:I34 C6:K6 C23:I23 C37:H37 C15 I12 R52:R1048576 Q14:Q15 C38:D40 E52:I65223 C52:D1048576 M52:Q65223 J53:L1048576 K49:L50 M35 C35:E35 C36:D36 R4 C2:L2 N2:HR2 M4:Q6 S3:HO3 C48:D49 E48:L48 M48:N49 C3 R3 Q8:Q11 C7:C11 R5:R9 S4:HR9 E39:Q40 J23:Q23 S52:HR1048576 P38:Q38 O37:Q37 P35:Q36 C21:C22 I16:I18 C17:C18 C42:Q42 C43:C44 O48:Q51 R13:HR51 J52 C51:N51 J25:Q34 M24:Q24 C50">
+  <conditionalFormatting sqref="G24:K24 C25:I31 C24 F32:I32 C32 C4:K4 C5:L5 C33:I34 C6:K6 C23:I23 C37:H37 C15 I12 R52:R1048576 Q14:Q15 C38:D40 E52:I65223 C52:D1048576 M52:Q65223 J53:L1048576 K49:L50 M35 C35:E35 C36:D36 C2:L2 N2:HR2 M4:R6 S3:HO3 C48:D49 E48:L48 M48:N49 C3 R3 Q8:Q11 C7:C11 R7:R9 S4:HR9 E39:Q40 J23:Q23 S52:HR1048576 P38:Q38 O37:Q37 P35:Q36 C21:C22 I16:I18 C17:C18 C42:Q42 C43:C44 O48:Q51 R13:HR51 J52 C51:N51 J25:Q34 M24:Q24 C50">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"*"</formula>
     </cfRule>
@@ -10950,52 +10953,52 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16 C14:I14">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>$C$12="ei mitään"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M37">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+      <formula>$C$12="ei mitään"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41:Q41">
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Q7">
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16 C14:I14">
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
-      <formula>$C$12="ei mitään"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M37">
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
-      <formula>$C$12="ei mitään"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C41:Q41">
     <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>"*"</formula>
     </cfRule>
@@ -13231,8 +13234,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D43" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14230,18 +14233,18 @@
         <v>224</v>
       </c>
       <c r="E49" s="188" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="F49" s="233"/>
       <c r="G49" s="204"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="166" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B50" s="171"/>
       <c r="C50" s="172" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D50" s="210" t="str">
         <f aca="false">A74</f>
@@ -14256,11 +14259,11 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="166" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B51" s="171"/>
       <c r="C51" s="172" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D51" s="210" t="str">
         <f aca="false">A76</f>
@@ -14275,11 +14278,11 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="166" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B52" s="168"/>
       <c r="C52" s="169" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D52" s="170"/>
       <c r="E52" s="170"/>
@@ -14293,7 +14296,7 @@
       <c r="B53" s="171"/>
       <c r="C53" s="185"/>
       <c r="D53" s="234" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E53" s="207"/>
       <c r="F53" s="207"/>
@@ -14314,11 +14317,11 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="166" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B55" s="171"/>
       <c r="C55" s="172" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D55" s="200" t="str">
         <f aca="false">A78</f>
@@ -14330,11 +14333,11 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="166" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B56" s="168"/>
       <c r="C56" s="169" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D56" s="170"/>
       <c r="E56" s="170"/>
@@ -14343,27 +14346,27 @@
     </row>
     <row r="57" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="166" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B57" s="171"/>
       <c r="C57" s="203"/>
       <c r="D57" s="237" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E57" s="238" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F57" s="203"/>
       <c r="G57" s="204"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="166" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B58" s="171"/>
       <c r="C58" s="185"/>
       <c r="D58" s="239" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E58" s="188" t="s">
         <v>61</v>
@@ -14373,11 +14376,11 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="166" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B59" s="171"/>
       <c r="C59" s="172" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D59" s="240" t="str">
         <f aca="false">A79</f>
@@ -14392,11 +14395,11 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="166" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B60" s="168"/>
       <c r="C60" s="169" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D60" s="170"/>
       <c r="E60" s="170"/>
@@ -14405,26 +14408,26 @@
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="166" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B61" s="171"/>
       <c r="C61" s="185"/>
       <c r="D61" s="196" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E61" s="196" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F61" s="233" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G61" s="196" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="166" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B62" s="171"/>
       <c r="C62" s="185"/>
@@ -14432,18 +14435,18 @@
         <v>62</v>
       </c>
       <c r="E62" s="188" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F62" s="239" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G62" s="188" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="166" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B63" s="171"/>
       <c r="C63" s="20"/>
@@ -14512,7 +14515,7 @@
     </row>
     <row r="66" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="166" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B66" s="162" t="str">
         <f aca="false">"Todistustunnus: "&amp;A1&amp;", 3/8"</f>
@@ -14527,7 +14530,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="166" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B67" s="248"/>
       <c r="C67" s="4"/>
@@ -14538,127 +14541,127 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="166" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="166" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="166" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="166" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="166" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="166" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="166" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="166" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="166" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="166" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="166" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="166" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="166" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="166" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="166" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="166" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="166" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="166" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="166" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="166" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="166" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="166" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="166" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="166" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="166" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -15217,7 +15220,7 @@
       </c>
       <c r="B2" s="250"/>
       <c r="C2" s="251" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D2" s="252"/>
       <c r="E2" s="251"/>
@@ -15334,7 +15337,7 @@
       </c>
       <c r="B8" s="171"/>
       <c r="C8" s="262" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D8" s="263" t="str">
         <f aca="false">A5</f>
@@ -15346,11 +15349,11 @@
     </row>
     <row r="9" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="166" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B9" s="171"/>
       <c r="C9" s="234" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D9" s="266" t="str">
         <f aca="false">A6</f>
@@ -15381,7 +15384,7 @@
       </c>
       <c r="B11" s="254"/>
       <c r="C11" s="255" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D11" s="256"/>
       <c r="E11" s="256"/>
@@ -15401,20 +15404,20 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="166" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B13" s="171"/>
       <c r="C13" s="265" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D13" s="196" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E13" s="196" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F13" s="197" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G13" s="197"/>
     </row>
@@ -15425,13 +15428,13 @@
       <c r="B14" s="171"/>
       <c r="C14" s="185"/>
       <c r="D14" s="196" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E14" s="196" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F14" s="197" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G14" s="197"/>
     </row>
@@ -15448,7 +15451,7 @@
         <v>62</v>
       </c>
       <c r="F15" s="239" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G15" s="199" t="s">
         <v>63</v>
@@ -15467,7 +15470,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="166" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B17" s="171"/>
       <c r="C17" s="270" t="s">
@@ -15567,7 +15570,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="166" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B21" s="171"/>
       <c r="C21" s="273" t="s">
@@ -15596,7 +15599,7 @@
       </c>
       <c r="B22" s="171"/>
       <c r="C22" s="265" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D22" s="274" t="str">
         <f aca="false">A42</f>
@@ -15629,7 +15632,7 @@
       </c>
       <c r="B24" s="254"/>
       <c r="C24" s="255" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D24" s="170"/>
       <c r="E24" s="256"/>
@@ -15638,7 +15641,7 @@
     </row>
     <row r="25" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="166" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B25" s="222"/>
       <c r="C25" s="276"/>
@@ -15679,7 +15682,7 @@
       </c>
       <c r="B28" s="171"/>
       <c r="C28" s="278" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D28" s="278"/>
       <c r="E28" s="241" t="str">
@@ -15698,7 +15701,7 @@
       </c>
       <c r="B29" s="171"/>
       <c r="C29" s="278" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D29" s="278"/>
       <c r="E29" s="241" t="str">
@@ -15713,11 +15716,11 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="166" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B30" s="171"/>
       <c r="C30" s="280" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D30" s="280"/>
       <c r="E30" s="241" t="str">
@@ -15736,7 +15739,7 @@
       </c>
       <c r="B31" s="171"/>
       <c r="C31" s="280" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D31" s="280"/>
       <c r="E31" s="241" t="str">
@@ -15755,7 +15758,7 @@
       </c>
       <c r="B32" s="171"/>
       <c r="C32" s="280" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D32" s="280"/>
       <c r="E32" s="241" t="str">
@@ -15774,7 +15777,7 @@
       </c>
       <c r="B33" s="171"/>
       <c r="C33" s="280" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D33" s="280"/>
       <c r="E33" s="241" t="str">
@@ -15800,11 +15803,11 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="166" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B35" s="254"/>
       <c r="C35" s="255" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D35" s="256"/>
       <c r="E35" s="256"/>
@@ -15830,13 +15833,13 @@
       <c r="C37" s="185"/>
       <c r="D37" s="185"/>
       <c r="E37" s="196" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F37" s="196" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G37" s="196" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15869,7 +15872,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="166" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B40" s="171"/>
       <c r="C40" s="172" t="s">
@@ -15886,7 +15889,7 @@
       </c>
       <c r="B41" s="171"/>
       <c r="C41" s="172" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D41" s="172"/>
       <c r="E41" s="241" t="str">
@@ -15903,11 +15906,11 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="166" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B42" s="171"/>
       <c r="C42" s="172" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D42" s="172"/>
       <c r="E42" s="241" t="str">
@@ -15924,11 +15927,11 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="166" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B43" s="171"/>
       <c r="C43" s="172" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D43" s="172"/>
       <c r="E43" s="241" t="str">
@@ -15949,7 +15952,7 @@
       </c>
       <c r="B44" s="171"/>
       <c r="C44" s="172" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D44" s="172"/>
       <c r="E44" s="241" t="str">
@@ -15965,11 +15968,11 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="166" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B45" s="171"/>
       <c r="C45" s="172" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D45" s="172"/>
       <c r="E45" s="241" t="str">
@@ -15987,11 +15990,11 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="166" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B46" s="171"/>
       <c r="C46" s="172" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D46" s="172"/>
       <c r="E46" s="241" t="str">
@@ -16007,11 +16010,11 @@
     </row>
     <row r="47" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="166" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B47" s="171"/>
       <c r="C47" s="265" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D47" s="265"/>
       <c r="E47" s="283" t="str">
@@ -16029,11 +16032,11 @@
     </row>
     <row r="48" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="166" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B48" s="171"/>
       <c r="C48" s="228" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D48" s="265"/>
       <c r="E48" s="235"/>
@@ -16042,7 +16045,7 @@
     </row>
     <row r="49" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="166" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B49" s="171"/>
       <c r="C49" s="203"/>
@@ -16053,11 +16056,11 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="166" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B50" s="254"/>
       <c r="C50" s="255" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D50" s="256"/>
       <c r="E50" s="256"/>
@@ -16066,7 +16069,7 @@
     </row>
     <row r="51" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="166" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B51" s="171"/>
       <c r="C51" s="203"/>
@@ -16077,7 +16080,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="166" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B52" s="171"/>
       <c r="C52" s="185"/>
@@ -16092,7 +16095,7 @@
     </row>
     <row r="53" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="166" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B53" s="171"/>
       <c r="C53" s="185"/>
@@ -16103,11 +16106,11 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="166" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B54" s="171"/>
       <c r="C54" s="172" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D54" s="172"/>
       <c r="E54" s="241" t="str">
@@ -16122,11 +16125,11 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="166" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B55" s="171"/>
       <c r="C55" s="172" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D55" s="172"/>
       <c r="E55" s="241" t="str">
@@ -16141,7 +16144,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="166" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B56" s="171"/>
       <c r="C56" s="172" t="s">
@@ -16160,11 +16163,11 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="166" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B57" s="171"/>
       <c r="C57" s="172" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D57" s="172"/>
       <c r="E57" s="241" t="str">
@@ -16179,7 +16182,7 @@
     </row>
     <row r="58" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="166" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B58" s="171"/>
       <c r="C58" s="172"/>
@@ -16190,11 +16193,11 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="166" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B59" s="171"/>
       <c r="C59" s="228" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D59" s="286"/>
       <c r="E59" s="287"/>
@@ -16203,11 +16206,11 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="166" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B60" s="171"/>
       <c r="C60" s="228" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D60" s="286"/>
       <c r="E60" s="288"/>
@@ -16216,7 +16219,7 @@
     </row>
     <row r="61" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="166" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B61" s="171"/>
       <c r="C61" s="172"/>
@@ -16227,11 +16230,11 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="166" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B62" s="254"/>
       <c r="C62" s="255" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D62" s="256"/>
       <c r="E62" s="256"/>
@@ -16240,7 +16243,7 @@
     </row>
     <row r="63" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="166" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B63" s="171"/>
       <c r="C63" s="203"/>
@@ -16251,7 +16254,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="166" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B64" s="171"/>
       <c r="C64" s="185"/>
@@ -16266,7 +16269,7 @@
     </row>
     <row r="65" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="166" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B65" s="171"/>
       <c r="C65" s="185"/>
@@ -16277,11 +16280,11 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="166" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B66" s="171"/>
       <c r="C66" s="172" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D66" s="172"/>
       <c r="E66" s="241" t="str">
@@ -16296,11 +16299,11 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="166" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B67" s="171"/>
       <c r="C67" s="172" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D67" s="172"/>
       <c r="E67" s="241" t="str">
@@ -16315,11 +16318,11 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="166" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B68" s="171"/>
       <c r="C68" s="172" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D68" s="172"/>
       <c r="E68" s="241" t="str">
@@ -16334,11 +16337,11 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="166" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B69" s="171"/>
       <c r="C69" s="172" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D69" s="172"/>
       <c r="E69" s="241" t="str">
@@ -16353,11 +16356,11 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="166" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B70" s="171"/>
       <c r="C70" s="172" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D70" s="172"/>
       <c r="E70" s="241" t="str">
@@ -16372,7 +16375,7 @@
     </row>
     <row r="71" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="166" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B71" s="171"/>
       <c r="C71" s="172"/>
@@ -16383,11 +16386,11 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="166" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B72" s="254"/>
       <c r="C72" s="255" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D72" s="256"/>
       <c r="E72" s="256"/>
@@ -16396,7 +16399,7 @@
     </row>
     <row r="73" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="166" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B73" s="171"/>
       <c r="C73" s="203"/>
@@ -16407,11 +16410,11 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="166" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B74" s="171"/>
       <c r="C74" s="172" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D74" s="172"/>
       <c r="E74" s="290" t="str">
@@ -16423,7 +16426,7 @@
     </row>
     <row r="75" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="166" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B75" s="245"/>
       <c r="C75" s="183"/>
@@ -16434,12 +16437,12 @@
     </row>
     <row r="76" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="166" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="166" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B77" s="292" t="str">
         <f aca="false">"Todistustunnus: "&amp;A1&amp;", 4/8"</f>
@@ -16453,182 +16456,182 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="166" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="166" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="166" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="166" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="166" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="166" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="166" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="166" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="166" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="166" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="166" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="166" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="166" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="166" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="166" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="166" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="166" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="166" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="166" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="166" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="166" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="166" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="166" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="166" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="166" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="166" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="166" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="166" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="166" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="166" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="166" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="166" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="166" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="166" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="166" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="166" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -17145,7 +17148,7 @@
       </c>
       <c r="B2" s="294"/>
       <c r="C2" s="295" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D2" s="295"/>
       <c r="E2" s="295"/>
@@ -17208,7 +17211,7 @@
       </c>
       <c r="B3" s="105"/>
       <c r="C3" s="299" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D3" s="299"/>
       <c r="E3" s="299"/>
@@ -17221,7 +17224,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="97" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B4" s="105"/>
       <c r="C4" s="68"/>
@@ -17236,11 +17239,11 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="97" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B5" s="101"/>
       <c r="C5" s="102" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D5" s="102"/>
       <c r="E5" s="102"/>
@@ -17253,7 +17256,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="97" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B6" s="105"/>
       <c r="C6" s="0"/>
@@ -17269,7 +17272,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="97" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B7" s="105"/>
       <c r="C7" s="16" t="s">
@@ -17280,7 +17283,7 @@
         <v>[:lahtotiedot :lammitetty-nettoala]</v>
       </c>
       <c r="E7" s="301" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F7" s="111"/>
       <c r="G7" s="302"/>
@@ -17292,7 +17295,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="97" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B8" s="105"/>
       <c r="C8" s="5"/>
@@ -17307,7 +17310,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="97" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B9" s="114"/>
       <c r="C9" s="115"/>
@@ -17322,11 +17325,11 @@
     </row>
     <row r="10" s="298" customFormat="true" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="293" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B10" s="304"/>
       <c r="C10" s="305" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D10" s="306"/>
       <c r="E10" s="306"/>
@@ -17389,7 +17392,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="97" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B11" s="105"/>
       <c r="C11" s="5"/>
@@ -17404,11 +17407,11 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="97" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B12" s="105"/>
       <c r="C12" s="108" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D12" s="108"/>
       <c r="E12" s="108"/>
@@ -17427,7 +17430,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="97" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B13" s="105"/>
       <c r="C13" s="108"/>
@@ -17442,11 +17445,11 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="97" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B14" s="105"/>
       <c r="C14" s="108" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D14" s="108"/>
       <c r="E14" s="108"/>
@@ -17465,7 +17468,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="97" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B15" s="105"/>
       <c r="C15" s="108"/>
@@ -17480,11 +17483,11 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="97" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B16" s="105"/>
       <c r="C16" s="319" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D16" s="108"/>
       <c r="E16" s="108"/>
@@ -17503,11 +17506,11 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="97" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B17" s="105"/>
       <c r="C17" s="319" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D17" s="108"/>
       <c r="E17" s="108"/>
@@ -17526,7 +17529,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="97" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B18" s="105"/>
       <c r="C18" s="319"/>
@@ -17541,11 +17544,11 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="97" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B19" s="105"/>
       <c r="C19" s="108" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D19" s="108"/>
       <c r="E19" s="108"/>
@@ -17564,7 +17567,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="97" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B20" s="114"/>
       <c r="C20" s="320"/>
@@ -17579,22 +17582,22 @@
     </row>
     <row r="21" s="298" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="293" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B21" s="304"/>
       <c r="C21" s="305" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D21" s="305"/>
       <c r="E21" s="305"/>
       <c r="F21" s="324" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="G21" s="325" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="H21" s="324" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="I21" s="325" t="s">
         <v>60</v>
@@ -17652,7 +17655,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="97" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B22" s="99"/>
       <c r="C22" s="326"/>
@@ -17667,11 +17670,11 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="97" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B23" s="105"/>
       <c r="C23" s="108" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D23" s="108"/>
       <c r="E23" s="108"/>
@@ -17680,7 +17683,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :kevyt-polttooljy]</v>
       </c>
       <c r="G23" s="333" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H23" s="334" t="n">
         <v>10</v>
@@ -17697,11 +17700,11 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="97" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B24" s="105"/>
       <c r="C24" s="108" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D24" s="108"/>
       <c r="E24" s="108"/>
@@ -17710,7 +17713,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :pilkkeet-havu-sekapuu]</v>
       </c>
       <c r="G24" s="333" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H24" s="334" t="n">
         <v>1300</v>
@@ -17727,11 +17730,11 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="97" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B25" s="105"/>
       <c r="C25" s="108" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D25" s="108"/>
       <c r="E25" s="108"/>
@@ -17740,7 +17743,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :pilkkeet-koivu]</v>
       </c>
       <c r="G25" s="333" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H25" s="334" t="n">
         <v>1700</v>
@@ -17757,11 +17760,11 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="97" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B26" s="105"/>
       <c r="C26" s="108" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D26" s="108"/>
       <c r="E26" s="108"/>
@@ -17770,7 +17773,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :puupelletit]</v>
       </c>
       <c r="G26" s="333" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="H26" s="334" t="n">
         <v>4.7</v>
@@ -17787,7 +17790,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="97" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B27" s="105"/>
       <c r="C27" s="335" t="str">
@@ -17820,7 +17823,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="97" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B28" s="105"/>
       <c r="C28" s="335" t="str">
@@ -17853,11 +17856,11 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="97" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B29" s="105"/>
       <c r="C29" s="338" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D29" s="338"/>
       <c r="E29" s="338"/>
@@ -17870,7 +17873,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="97" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B30" s="105"/>
       <c r="C30" s="338"/>
@@ -17885,7 +17888,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="97" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B31" s="105"/>
       <c r="C31" s="338"/>
@@ -17900,7 +17903,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="97" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B32" s="105"/>
       <c r="C32" s="338"/>
@@ -17915,7 +17918,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="97" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B33" s="105"/>
       <c r="C33" s="342"/>
@@ -17930,7 +17933,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="97" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B34" s="114"/>
       <c r="C34" s="343"/>
@@ -17945,11 +17948,11 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="97" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B35" s="105"/>
       <c r="C35" s="305" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D35" s="305"/>
       <c r="E35" s="305"/>
@@ -17962,7 +17965,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="97" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B36" s="105"/>
       <c r="C36" s="305"/>
@@ -17981,7 +17984,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="97" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B37" s="99"/>
       <c r="C37" s="349"/>
@@ -17996,11 +17999,11 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="97" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B38" s="105"/>
       <c r="C38" s="32" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D38" s="32"/>
       <c r="E38" s="32"/>
@@ -18019,7 +18022,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="97" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B39" s="105"/>
       <c r="C39" s="32"/>
@@ -18034,11 +18037,11 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="97" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B40" s="105"/>
       <c r="C40" s="32" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D40" s="32"/>
       <c r="E40" s="32"/>
@@ -18057,7 +18060,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="97" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B41" s="105"/>
       <c r="C41" s="32"/>
@@ -18072,11 +18075,11 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="97" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B42" s="105"/>
       <c r="C42" s="32" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D42" s="32"/>
       <c r="E42" s="32"/>
@@ -18095,7 +18098,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="97" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B43" s="105"/>
       <c r="C43" s="32"/>
@@ -18110,11 +18113,11 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="97" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B44" s="105"/>
       <c r="C44" s="32" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D44" s="32"/>
       <c r="E44" s="32"/>
@@ -18133,7 +18136,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="97" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B45" s="105"/>
       <c r="C45" s="32"/>
@@ -18148,11 +18151,11 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="97" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B46" s="105"/>
       <c r="C46" s="16" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -18171,7 +18174,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="97" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B47" s="114"/>
       <c r="C47" s="361"/>
@@ -18186,11 +18189,11 @@
     </row>
     <row r="48" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="97" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B48" s="99"/>
       <c r="C48" s="364" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D48" s="364"/>
       <c r="E48" s="364"/>
@@ -18203,7 +18206,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="97" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B49" s="105"/>
       <c r="C49" s="364"/>
@@ -18218,7 +18221,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="97" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B50" s="105"/>
       <c r="C50" s="364"/>
@@ -18233,7 +18236,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="97" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B51" s="105"/>
       <c r="C51" s="364"/>
@@ -18248,7 +18251,7 @@
     </row>
     <row r="52" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="97" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B52" s="105"/>
       <c r="C52" s="364"/>
@@ -18263,7 +18266,7 @@
     </row>
     <row r="53" customFormat="false" ht="33.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="97" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B53" s="152"/>
       <c r="C53" s="364"/>
@@ -18279,7 +18282,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="97" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B54" s="366" t="str">
         <f aca="false">"Todistustunnus: "&amp;A1&amp;", 5/8"</f>
@@ -18297,7 +18300,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="97" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B55" s="366"/>
       <c r="C55" s="366"/>
@@ -18312,62 +18315,62 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="97" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="97" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="97" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="97" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="97" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="97" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="97" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="97" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="97" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="97" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="97" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="97" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -18875,10 +18878,10 @@
     </row>
     <row r="2" s="369" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="249" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B2" s="368" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C2" s="368"/>
       <c r="D2" s="368"/>
@@ -18917,10 +18920,10 @@
     </row>
     <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="166" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B3" s="370" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C3" s="370"/>
       <c r="D3" s="370"/>
@@ -18929,10 +18932,10 @@
     </row>
     <row r="4" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="367" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B4" s="371" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C4" s="102"/>
       <c r="D4" s="372"/>
@@ -18941,7 +18944,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="367" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B5" s="374" t="str">
         <f aca="false">A2</f>
@@ -18955,7 +18958,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="367" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B6" s="374"/>
       <c r="C6" s="374"/>
@@ -18965,7 +18968,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="367" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B7" s="374"/>
       <c r="C7" s="374"/>
@@ -18975,7 +18978,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="367" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B8" s="374"/>
       <c r="C8" s="374"/>
@@ -18985,7 +18988,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="367" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B9" s="374"/>
       <c r="C9" s="374"/>
@@ -18995,7 +18998,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="367" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B10" s="374"/>
       <c r="C10" s="374"/>
@@ -19005,10 +19008,10 @@
     </row>
     <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="166" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B11" s="375" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C11" s="375"/>
       <c r="D11" s="375"/>
@@ -19017,7 +19020,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="166" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B12" s="376" t="n">
         <v>1</v>
@@ -19032,7 +19035,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="166" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B13" s="376" t="n">
         <v>2</v>
@@ -19047,7 +19050,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="166" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B14" s="376" t="n">
         <v>3</v>
@@ -19062,25 +19065,25 @@
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="166" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B15" s="378"/>
       <c r="C15" s="379" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D15" s="379" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E15" s="379" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F15" s="380" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="166" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B16" s="381"/>
       <c r="C16" s="120" t="s">
@@ -19098,7 +19101,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="166" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B17" s="376" t="n">
         <v>1</v>
@@ -19122,7 +19125,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="166" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B18" s="376" t="n">
         <v>2</v>
@@ -19146,7 +19149,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="166" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B19" s="376" t="n">
         <v>3</v>
@@ -19170,10 +19173,10 @@
     </row>
     <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="166" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B20" s="383" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C20" s="102"/>
       <c r="D20" s="372"/>
@@ -19182,7 +19185,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="166" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B21" s="374" t="str">
         <f aca="false">A22</f>
@@ -19195,7 +19198,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="166" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B22" s="374"/>
       <c r="C22" s="374"/>
@@ -19205,7 +19208,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="166" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B23" s="374"/>
       <c r="C23" s="374"/>
@@ -19215,7 +19218,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="166" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B24" s="374"/>
       <c r="C24" s="374"/>
@@ -19225,7 +19228,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="166" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B25" s="374"/>
       <c r="C25" s="374"/>
@@ -19235,7 +19238,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="166" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B26" s="374"/>
       <c r="C26" s="374"/>
@@ -19245,10 +19248,10 @@
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="166" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B27" s="375" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C27" s="375"/>
       <c r="D27" s="375"/>
@@ -19257,7 +19260,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="166" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B28" s="376" t="n">
         <v>1</v>
@@ -19272,7 +19275,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="166" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B29" s="376" t="n">
         <v>2</v>
@@ -19287,7 +19290,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="166" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B30" s="376" t="n">
         <v>3</v>
@@ -19302,25 +19305,25 @@
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="166" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B31" s="385"/>
       <c r="C31" s="379" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D31" s="379" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E31" s="379" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F31" s="380" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="166" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B32" s="385"/>
       <c r="C32" s="120" t="s">
@@ -19338,7 +19341,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="166" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B33" s="376" t="n">
         <v>1</v>
@@ -19362,7 +19365,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="166" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B34" s="376" t="n">
         <v>2</v>
@@ -19386,7 +19389,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="166" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B35" s="376" t="n">
         <v>3</v>
@@ -19410,10 +19413,10 @@
     </row>
     <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="166" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B36" s="383" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C36" s="386"/>
       <c r="D36" s="14"/>
@@ -19422,7 +19425,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="166" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B37" s="374" t="str">
         <f aca="false">A42</f>
@@ -19435,7 +19438,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="166" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B38" s="374"/>
       <c r="C38" s="374"/>
@@ -19445,7 +19448,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="166" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B39" s="374"/>
       <c r="C39" s="374"/>
@@ -19455,7 +19458,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="166" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B40" s="374"/>
       <c r="C40" s="374"/>
@@ -19465,7 +19468,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="166" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B41" s="374"/>
       <c r="C41" s="374"/>
@@ -19475,7 +19478,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="166" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B42" s="374"/>
       <c r="C42" s="374"/>
@@ -19485,10 +19488,10 @@
     </row>
     <row r="43" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="166" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B43" s="375" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C43" s="375"/>
       <c r="D43" s="375"/>
@@ -19497,7 +19500,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="166" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B44" s="376" t="n">
         <v>1</v>
@@ -19512,7 +19515,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="166" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B45" s="376" t="n">
         <v>2</v>
@@ -19527,7 +19530,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="166" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B46" s="376" t="n">
         <v>3</v>
@@ -19542,25 +19545,25 @@
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="166" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B47" s="385"/>
       <c r="C47" s="379" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D47" s="379" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E47" s="379" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F47" s="380" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="166" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B48" s="385"/>
       <c r="C48" s="120" t="s">
@@ -19578,7 +19581,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="166" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B49" s="376" t="n">
         <v>1</v>
@@ -19602,7 +19605,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="166" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B50" s="376" t="n">
         <v>2</v>
@@ -19626,7 +19629,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="166" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B51" s="376" t="n">
         <v>3</v>
@@ -19650,7 +19653,7 @@
     </row>
     <row r="52" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="367" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B52" s="292" t="str">
         <f aca="false">"Todistustunnus: "&amp;A1&amp;", 6/8"</f>
@@ -19663,48 +19666,48 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="367" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B53" s="387"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="367" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="367" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="367" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="367" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="367" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="367" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="367" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="367" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>
@@ -19908,10 +19911,10 @@
     </row>
     <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="367" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B2" s="371" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C2" s="102"/>
       <c r="D2" s="372"/>
@@ -19920,7 +19923,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="367" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B3" s="374" t="str">
         <f aca="false">A2</f>
@@ -19933,7 +19936,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="367" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B4" s="374"/>
       <c r="C4" s="374"/>
@@ -19943,7 +19946,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="367" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B5" s="374"/>
       <c r="C5" s="374"/>
@@ -19954,7 +19957,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="367" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B6" s="374"/>
       <c r="C6" s="374"/>
@@ -19965,7 +19968,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="367" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B7" s="374"/>
       <c r="C7" s="374"/>
@@ -19975,7 +19978,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="367" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B8" s="374"/>
       <c r="C8" s="374"/>
@@ -19985,7 +19988,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="367" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B9" s="374"/>
       <c r="C9" s="374"/>
@@ -19995,10 +19998,10 @@
     </row>
     <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="166" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B10" s="388" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C10" s="388"/>
       <c r="D10" s="388"/>
@@ -20007,7 +20010,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="166" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B11" s="376" t="n">
         <v>1</v>
@@ -20022,7 +20025,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="166" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B12" s="376" t="n">
         <v>2</v>
@@ -20037,7 +20040,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="166" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B13" s="376" t="n">
         <v>3</v>
@@ -20052,25 +20055,25 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="166" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B14" s="385"/>
       <c r="C14" s="379" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D14" s="379" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E14" s="379" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F14" s="380" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="166" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B15" s="385"/>
       <c r="C15" s="120" t="s">
@@ -20088,7 +20091,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="166" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B16" s="376" t="n">
         <v>1</v>
@@ -20112,7 +20115,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="166" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B17" s="376" t="n">
         <v>2</v>
@@ -20136,7 +20139,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="166" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B18" s="376" t="n">
         <v>3</v>
@@ -20160,10 +20163,10 @@
     </row>
     <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="166" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B19" s="383" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C19" s="386"/>
       <c r="D19" s="14"/>
@@ -20172,7 +20175,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="166" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B20" s="374" t="str">
         <f aca="false">A22</f>
@@ -20185,7 +20188,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="166" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B21" s="374"/>
       <c r="C21" s="374"/>
@@ -20195,7 +20198,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="166" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B22" s="374"/>
       <c r="C22" s="374"/>
@@ -20205,7 +20208,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="166" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B23" s="374"/>
       <c r="C23" s="374"/>
@@ -20215,7 +20218,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="166" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B24" s="374"/>
       <c r="C24" s="374"/>
@@ -20225,7 +20228,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="166" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B25" s="374"/>
       <c r="C25" s="374"/>
@@ -20235,7 +20238,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="166" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B26" s="374"/>
       <c r="C26" s="374"/>
@@ -20245,10 +20248,10 @@
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="166" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B27" s="388" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C27" s="388"/>
       <c r="D27" s="388"/>
@@ -20257,7 +20260,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="166" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B28" s="376" t="n">
         <v>1</v>
@@ -20272,7 +20275,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="166" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B29" s="376" t="n">
         <v>2</v>
@@ -20287,7 +20290,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="166" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B30" s="376" t="n">
         <v>3</v>
@@ -20302,25 +20305,25 @@
     </row>
     <row r="31" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="166" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B31" s="385"/>
       <c r="C31" s="379" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D31" s="379" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E31" s="379" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F31" s="380" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="166" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B32" s="385"/>
       <c r="C32" s="120" t="s">
@@ -20338,7 +20341,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="166" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B33" s="376" t="n">
         <v>1</v>
@@ -20362,7 +20365,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="166" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B34" s="376" t="n">
         <v>2</v>
@@ -20386,7 +20389,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="166" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B35" s="376" t="n">
         <v>3</v>
@@ -20410,10 +20413,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="166" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B36" s="390" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C36" s="390"/>
       <c r="D36" s="390"/>
@@ -20422,7 +20425,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="166" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B37" s="374" t="str">
         <f aca="false">A42</f>
@@ -20435,7 +20438,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="166" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B38" s="374"/>
       <c r="C38" s="374"/>
@@ -20445,7 +20448,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="166" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B39" s="374"/>
       <c r="C39" s="374"/>
@@ -20455,7 +20458,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="166" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B40" s="374"/>
       <c r="C40" s="374"/>
@@ -20465,7 +20468,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="166" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B41" s="374"/>
       <c r="C41" s="374"/>
@@ -20475,7 +20478,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="166" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B42" s="374"/>
       <c r="C42" s="374"/>
@@ -20485,7 +20488,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="166" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B43" s="374"/>
       <c r="C43" s="374"/>
@@ -20495,7 +20498,7 @@
     </row>
     <row r="44" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="166" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B44" s="374"/>
       <c r="C44" s="374"/>
@@ -20505,7 +20508,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="166" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B45" s="374"/>
       <c r="C45" s="374"/>
@@ -20563,7 +20566,7 @@
     </row>
     <row r="52" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="371" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C52" s="102"/>
       <c r="D52" s="372"/>
@@ -20581,7 +20584,7 @@
     <row r="54" customFormat="false" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="166"/>
       <c r="B54" s="333" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C54" s="333"/>
       <c r="D54" s="333"/>
@@ -20752,7 +20755,7 @@
   </sheetPr>
   <dimension ref="A1:Q140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
@@ -20774,11 +20777,11 @@
     </row>
     <row r="2" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="166" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B2" s="393"/>
       <c r="C2" s="394" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D2" s="394"/>
       <c r="E2" s="394"/>
@@ -20793,7 +20796,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="367" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B3" s="358"/>
       <c r="C3" s="395" t="str">
@@ -20813,7 +20816,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="367" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B4" s="358"/>
       <c r="C4" s="395"/>
@@ -20830,7 +20833,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="367" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B5" s="358"/>
       <c r="C5" s="395"/>
@@ -20847,7 +20850,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="367" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B6" s="358"/>
       <c r="C6" s="395"/>
@@ -20865,7 +20868,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="367" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B7" s="358"/>
       <c r="C7" s="395"/>
@@ -20884,7 +20887,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="367" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B8" s="358"/>
       <c r="C8" s="395"/>
@@ -20901,7 +20904,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="367" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B9" s="358"/>
       <c r="C9" s="395"/>
@@ -20919,7 +20922,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="367" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B10" s="358"/>
       <c r="C10" s="395"/>
@@ -20936,7 +20939,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="367" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B11" s="358"/>
       <c r="C11" s="395"/>
@@ -20953,7 +20956,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="367" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B12" s="358"/>
       <c r="C12" s="395"/>
@@ -20970,7 +20973,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="367" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B13" s="358"/>
       <c r="C13" s="395"/>
@@ -20987,7 +20990,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="367" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B14" s="358"/>
       <c r="C14" s="395"/>
@@ -21004,7 +21007,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="367" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B15" s="358"/>
       <c r="C15" s="395"/>
@@ -21021,7 +21024,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="367" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B16" s="358"/>
       <c r="C16" s="395"/>
@@ -21038,7 +21041,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="367" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B17" s="358"/>
       <c r="C17" s="395"/>
@@ -21055,7 +21058,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="367" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B18" s="358"/>
       <c r="C18" s="395"/>
@@ -21072,7 +21075,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="367" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B19" s="358"/>
       <c r="C19" s="395"/>
@@ -21089,7 +21092,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="367" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B20" s="358"/>
       <c r="C20" s="395"/>
@@ -21106,7 +21109,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="367" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B21" s="358"/>
       <c r="C21" s="395"/>
@@ -21123,7 +21126,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="367" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B22" s="358"/>
       <c r="C22" s="395"/>
@@ -21140,7 +21143,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="367" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B23" s="358"/>
       <c r="C23" s="395"/>
@@ -21157,7 +21160,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="367" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B24" s="358"/>
       <c r="C24" s="395"/>
@@ -21174,7 +21177,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="367" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B25" s="358"/>
       <c r="C25" s="395"/>
@@ -21191,7 +21194,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="367" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B26" s="358"/>
       <c r="C26" s="395"/>
@@ -21208,7 +21211,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="367" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B27" s="358"/>
       <c r="C27" s="395"/>
@@ -21226,7 +21229,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="367" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B28" s="358"/>
       <c r="C28" s="395"/>
@@ -21243,7 +21246,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="367" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B29" s="358"/>
       <c r="C29" s="395"/>
@@ -21260,7 +21263,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="367" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B30" s="358"/>
       <c r="C30" s="395"/>
@@ -21277,7 +21280,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="367" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B31" s="358"/>
       <c r="C31" s="395"/>
@@ -21295,7 +21298,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="367" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B32" s="358"/>
       <c r="C32" s="395"/>
@@ -21312,7 +21315,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="367" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B33" s="358"/>
       <c r="C33" s="395"/>
@@ -21329,7 +21332,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="367" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B34" s="358"/>
       <c r="C34" s="395"/>
@@ -21346,7 +21349,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="367" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B35" s="358"/>
       <c r="C35" s="395"/>
@@ -21363,11 +21366,11 @@
     </row>
     <row r="36" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="367" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B36" s="396"/>
       <c r="C36" s="397" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D36" s="398"/>
       <c r="E36" s="398"/>
@@ -21382,100 +21385,100 @@
     </row>
     <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="367" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B37" s="400"/>
       <c r="C37" s="401"/>
       <c r="D37" s="402" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="E37" s="402"/>
       <c r="F37" s="402"/>
       <c r="G37" s="403" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="H37" s="403"/>
       <c r="I37" s="403"/>
       <c r="J37" s="403" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="K37" s="403"/>
       <c r="L37" s="403" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="M37" s="403"/>
     </row>
     <row r="38" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="367" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B38" s="404"/>
       <c r="C38" s="405" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="D38" s="406" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E38" s="406"/>
       <c r="F38" s="406"/>
       <c r="G38" s="407" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="H38" s="407"/>
       <c r="I38" s="407"/>
       <c r="J38" s="407" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="K38" s="407"/>
       <c r="L38" s="407" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="M38" s="407"/>
     </row>
     <row r="39" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="367" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B39" s="408"/>
       <c r="C39" s="409"/>
       <c r="D39" s="410" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="E39" s="411" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F39" s="411" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="G39" s="410" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H39" s="410" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="I39" s="411" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="J39" s="411" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="K39" s="411" t="s">
+        <v>308</v>
+      </c>
+      <c r="L39" s="411" t="s">
         <v>307</v>
       </c>
-      <c r="L39" s="411" t="s">
-        <v>306</v>
-      </c>
       <c r="M39" s="411" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="367" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B40" s="412"/>
       <c r="C40" s="413" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D40" s="414" t="str">
         <f aca="false">A11</f>
@@ -21520,11 +21523,11 @@
     </row>
     <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="367" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B41" s="412"/>
       <c r="C41" s="413" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="D41" s="414" t="str">
         <f aca="false">A21</f>
@@ -21569,11 +21572,11 @@
     </row>
     <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="367" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B42" s="412"/>
       <c r="C42" s="413" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D42" s="414" t="str">
         <f aca="false">A31</f>
@@ -21618,11 +21621,11 @@
     </row>
     <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="367" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B43" s="412"/>
       <c r="C43" s="413" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D43" s="414" t="str">
         <f aca="false">A41</f>
@@ -21667,11 +21670,11 @@
     </row>
     <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="367" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B44" s="412"/>
       <c r="C44" s="413" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D44" s="414" t="str">
         <f aca="false">A51</f>
@@ -21716,11 +21719,11 @@
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="367" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B45" s="412"/>
       <c r="C45" s="413" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D45" s="414" t="str">
         <f aca="false">A61</f>
@@ -21765,11 +21768,11 @@
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="367" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B46" s="412"/>
       <c r="C46" s="413" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="D46" s="414" t="str">
         <f aca="false">A71</f>
@@ -21814,11 +21817,11 @@
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="367" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B47" s="412"/>
       <c r="C47" s="413" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D47" s="414" t="str">
         <f aca="false">A81</f>
@@ -21863,11 +21866,11 @@
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="367" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B48" s="412"/>
       <c r="C48" s="413" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D48" s="414" t="str">
         <f aca="false">A91</f>
@@ -21912,11 +21915,11 @@
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="367" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B49" s="412"/>
       <c r="C49" s="413" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D49" s="414" t="str">
         <f aca="false">A101</f>
@@ -21961,11 +21964,11 @@
     </row>
     <row r="50" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="367" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B50" s="412"/>
       <c r="C50" s="413" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="D50" s="414" t="str">
         <f aca="false">A111</f>
@@ -22010,11 +22013,11 @@
     </row>
     <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="367" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B51" s="412"/>
       <c r="C51" s="413" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D51" s="414" t="str">
         <f aca="false">A121</f>
@@ -22059,11 +22062,11 @@
     </row>
     <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="367" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B52" s="412"/>
       <c r="C52" s="415" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D52" s="416" t="str">
         <f aca="false">A131</f>
@@ -22108,11 +22111,11 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="367" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B53" s="400"/>
       <c r="C53" s="417" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="D53" s="417"/>
       <c r="E53" s="417"/>
@@ -22127,7 +22130,7 @@
     </row>
     <row r="54" customFormat="false" ht="7.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="367" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B54" s="400"/>
       <c r="C54" s="418"/>
@@ -22144,11 +22147,11 @@
     </row>
     <row r="55" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="367" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B55" s="419"/>
       <c r="C55" s="420" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D55" s="420"/>
       <c r="E55" s="420"/>
@@ -22163,11 +22166,11 @@
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="367" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B56" s="421"/>
       <c r="C56" s="422" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D56" s="422"/>
       <c r="E56" s="422"/>
@@ -22185,11 +22188,11 @@
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="367" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B57" s="421"/>
       <c r="C57" s="422" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="D57" s="422"/>
       <c r="E57" s="422"/>
@@ -22207,11 +22210,11 @@
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="367" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B58" s="421"/>
       <c r="C58" s="422" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="D58" s="422"/>
       <c r="E58" s="422"/>
@@ -22229,11 +22232,11 @@
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="367" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B59" s="421"/>
       <c r="C59" s="422" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="D59" s="422"/>
       <c r="E59" s="422"/>
@@ -22251,11 +22254,11 @@
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="367" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B60" s="421"/>
       <c r="C60" s="422" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D60" s="422"/>
       <c r="E60" s="422"/>
@@ -22273,11 +22276,11 @@
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="367" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B61" s="404"/>
       <c r="C61" s="426" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="D61" s="426"/>
       <c r="E61" s="426"/>
@@ -22295,7 +22298,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="367" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B62" s="430" t="str">
         <f aca="false">"Todistustunnus: "&amp;A1&amp;", 8/8"</f>
@@ -22315,7 +22318,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="367" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B63" s="430"/>
       <c r="C63" s="430"/>
@@ -22332,387 +22335,387 @@
     </row>
     <row r="64" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="367" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="367" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="367" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="367" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="367" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="367" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="367" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="367" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="367" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="367" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="367" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="367" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="367" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="367" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="367" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="367" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="367" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="367" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="367" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="367" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="367" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="367" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="367" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="367" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="367" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="367" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="367" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="367" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="367" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="367" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="367" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="367" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="367" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="367" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="367" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="367" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="367" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="367" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="367" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="367" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="367" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="367" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="367" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="367" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="367" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="367" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="367" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="367" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="367" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="367" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="367" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="367" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="367" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="367" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="367" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="367" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="367" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="367" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="367" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="367" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="367" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="367" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="367" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="367" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="367" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="367" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="367" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="367" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="367" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="367" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="367" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="367" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="367" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="367" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="367" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="367" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="367" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AE-578 add missing sum of kuluttajalaitteet and valaistus to käytettävät energiamuodot in 2013 pdf
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,23 +19,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'1) etusivu'!$B$1:$R$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$M$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$B$1:$R$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$66</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$L$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$N$62</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0" vbProcedure="false">'8) lisämerkintöjä'!$B$1:$M$63</definedName>
   </definedNames>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="782">
   <si>
     <t xml:space="preserve">[:id]</t>
   </si>
@@ -223,7 +223,7 @@
     <t xml:space="preserve">Viimeinen voimassaolopäivä:</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55835]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55923]</t>
   </si>
   <si>
     <t xml:space="preserve">YHTEENVETO RAKENNUKSEN ENERGIATEHOKKUUDESTA</t>
@@ -468,67 +468,43 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 1 :nimi]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 1 :ostoenergia]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 1 :ostoenergia-nettoala]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 1 :muotokerroin]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 1 :ostoenergia-nettoala-kertoimella]</t>
+    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :valaistus-kuluttaja-sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :valaistus-kuluttaja-sahko-nettoala]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :e-luokka-rajat :kayttotarkoitus :label-fi]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :e-luokka-rajat :kayttotarkoitus :label-sv]</t>
   </si>
   <si>
     <t xml:space="preserve">TOIMENPIDE-EHDOTUKSIA E-LUVUN PARANTAMISEKSI</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 2 :nimi]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55925]</t>
   </si>
   <si>
     <t xml:space="preserve">Keskeiset suositukset rakennuksen E-lukua parantaviksi toimenpiteiksi (ei koske uusia rakennuksia)</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 2 :ostoenergia]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 2 :ostoenergia-nettoala]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 2 :muotokerroin]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 2 :ostoenergia-nettoala-kertoimella]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :e-luokka-rajat :kayttotarkoitus :label-fi]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :e-luokka-rajat :kayttotarkoitus :label-sv]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55837]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55840]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55843]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55846]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55849]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55852]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55855]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55927]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55930]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55933]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55936]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55939]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--55942]</t>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :e-luokka]</t>
@@ -1662,18 +1638,33 @@
     <t xml:space="preserve">Lämpöpumpun lämmönlähteestä ottama energia</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 1 :nimi]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Muu ympäristöstä otettu energia, sähkö</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 1 :ostoenergia]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Muu ympäristöstä otettu energia, lämpö</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 1 :muotokerroin]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 1 :ostoenergia-kertoimella]</t>
   </si>
   <si>
     <t xml:space="preserve">Rakennuksen teknisten järjestelmien energiankulutus</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 1 :ostoenergia-nettoala-kertoimella]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 2 :nimi]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sähkö</t>
   </si>
   <si>
@@ -1683,7 +1674,16 @@
     <t xml:space="preserve">Kaukojäähdytys</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 2 :ostoenergia]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 2 :muotokerroin]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 2 :ostoenergia-kertoimella]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 2 :ostoenergia-nettoala-kertoimella]</t>
   </si>
   <si>
     <r>
@@ -4803,11 +4803,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4823,31 +4823,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="9" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4859,7 +4859,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4903,8 +4903,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -4929,10 +4933,6 @@
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -8637,9 +8637,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>229680</xdr:colOff>
+      <xdr:colOff>229320</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8653,7 +8653,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4656960"/>
-          <a:ext cx="739800" cy="196560"/>
+          <a:ext cx="739440" cy="196200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8674,9 +8674,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>129240</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8690,7 +8690,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4971240"/>
-          <a:ext cx="1083240" cy="196560"/>
+          <a:ext cx="1082880" cy="196200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8711,9 +8711,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2880</xdr:colOff>
+      <xdr:colOff>2520</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8727,7 +8727,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5285520"/>
-          <a:ext cx="1389960" cy="196560"/>
+          <a:ext cx="1389600" cy="196200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8748,9 +8748,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>326880</xdr:colOff>
+      <xdr:colOff>326520</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8764,7 +8764,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5599800"/>
-          <a:ext cx="1713960" cy="196560"/>
+          <a:ext cx="1713600" cy="196200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8785,9 +8785,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>200160</xdr:colOff>
+      <xdr:colOff>199800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>257040</xdr:rowOff>
+      <xdr:rowOff>256680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8801,7 +8801,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5909760"/>
-          <a:ext cx="2021040" cy="209520"/>
+          <a:ext cx="2020680" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8822,9 +8822,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>143280</xdr:colOff>
+      <xdr:colOff>142920</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8838,7 +8838,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6219720"/>
-          <a:ext cx="2357280" cy="196560"/>
+          <a:ext cx="2356920" cy="196200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8859,9 +8859,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>83520</xdr:colOff>
+      <xdr:colOff>83160</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>245160</xdr:rowOff>
+      <xdr:rowOff>244800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8871,7 +8871,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6531480"/>
-          <a:ext cx="2670120" cy="195480"/>
+          <a:ext cx="2669760" cy="195120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9240,9 +9240,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>282960</xdr:colOff>
+      <xdr:colOff>282600</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
+      <xdr:rowOff>83880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9252,7 +9252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1978200" y="78480"/>
-          <a:ext cx="6969240" cy="10490760"/>
+          <a:ext cx="6968880" cy="10490400"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9381,7 +9381,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -11021,8 +11021,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11171,7 +11171,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="107" t="str">
         <f aca="false">A2</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55835]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55923]</v>
       </c>
       <c r="G5" s="108"/>
       <c r="H5" s="5"/>
@@ -11394,7 +11394,7 @@
       <c r="Z11" s="0"/>
       <c r="AA11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="97" t="s">
         <v>59</v>
       </c>
@@ -11726,7 +11726,7 @@
       <c r="G20" s="133"/>
       <c r="H20" s="133"/>
       <c r="I20" s="134" t="str">
-        <f aca="false">A42</f>
+        <f aca="false">A34</f>
         <v>[:tulokset :e-luku]</v>
       </c>
       <c r="J20" s="134"/>
@@ -11821,7 +11821,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="135" t="str">
-        <f aca="false">A43</f>
+        <f aca="false">A35</f>
         <v>[:tulokset :e-luokka-rajat :kayttotarkoitus :label-fi]</v>
       </c>
       <c r="H23" s="0"/>
@@ -11887,16 +11887,16 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="139" t="str">
-        <f aca="false">A45</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55837]</v>
+        <f aca="false">A37</f>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55925]</v>
       </c>
       <c r="H25" s="140" t="str">
-        <f aca="false">A46</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55840]</v>
+        <f aca="false">A38</f>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55927]</v>
       </c>
       <c r="I25" s="141" t="str">
-        <f aca="false">A47</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55843]</v>
+        <f aca="false">A39</f>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55930]</v>
       </c>
       <c r="J25" s="136"/>
       <c r="L25" s="0"/>
@@ -11926,16 +11926,16 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="142" t="str">
-        <f aca="false">A48</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55846]</v>
+        <f aca="false">A40</f>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55933]</v>
       </c>
       <c r="H26" s="143" t="str">
-        <f aca="false">A49</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55849]</v>
+        <f aca="false">A41</f>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55936]</v>
       </c>
       <c r="I26" s="144" t="str">
-        <f aca="false">A50</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55852]</v>
+        <f aca="false">A42</f>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55939]</v>
       </c>
       <c r="J26" s="136"/>
       <c r="L26" s="0"/>
@@ -11965,8 +11965,8 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="145" t="str">
-        <f aca="false">A51</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55855]</v>
+        <f aca="false">A43</f>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--55942]</v>
       </c>
       <c r="H27" s="146"/>
       <c r="I27" s="146"/>
@@ -12030,7 +12030,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="148" t="str">
-        <f aca="false">A52</f>
+        <f aca="false">A44</f>
         <v>[:tulokset :e-luokka]</v>
       </c>
       <c r="H29" s="149"/>
@@ -12177,7 +12177,7 @@
     </row>
     <row r="34" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="97" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="B34" s="105"/>
       <c r="C34" s="151"/>
@@ -12207,7 +12207,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="97" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B35" s="152"/>
       <c r="C35" s="153"/>
@@ -12237,11 +12237,11 @@
     </row>
     <row r="36" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="97" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" s="155"/>
       <c r="C36" s="156" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D36" s="156"/>
       <c r="E36" s="156"/>
@@ -12269,11 +12269,11 @@
     </row>
     <row r="37" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="97" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B37" s="101"/>
       <c r="C37" s="102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D37" s="102"/>
       <c r="E37" s="103"/>
@@ -12300,12 +12300,12 @@
       <c r="AA37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>102</v>
+      <c r="A38" s="97" t="s">
+        <v>101</v>
       </c>
       <c r="B38" s="158"/>
       <c r="C38" s="159" t="str">
-        <f aca="false">A53</f>
+        <f aca="false">A45</f>
         <v>[:perustiedot :keskeiset-suositukset-fi]</v>
       </c>
       <c r="D38" s="159"/>
@@ -12333,8 +12333,8 @@
       <c r="AA38" s="0"/>
     </row>
     <row r="39" s="3" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>103</v>
+      <c r="A39" s="97" t="s">
+        <v>102</v>
       </c>
       <c r="B39" s="105"/>
       <c r="C39" s="159"/>
@@ -12365,7 +12365,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="97" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B40" s="105"/>
       <c r="C40" s="159"/>
@@ -12395,7 +12395,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="97" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B41" s="105"/>
       <c r="C41" s="159"/>
@@ -12425,7 +12425,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="97" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="B42" s="105"/>
       <c r="C42" s="159"/>
@@ -12454,7 +12454,7 @@
       <c r="AA42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="97" t="s">
+      <c r="A43" s="160" t="s">
         <v>106</v>
       </c>
       <c r="B43" s="105"/>
@@ -12574,9 +12574,6 @@
       <c r="AA46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="97" t="s">
-        <v>110</v>
-      </c>
       <c r="B47" s="105"/>
       <c r="C47" s="159"/>
       <c r="D47" s="159"/>
@@ -12604,9 +12601,6 @@
       <c r="AA47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="97" t="s">
-        <v>111</v>
-      </c>
       <c r="B48" s="105"/>
       <c r="C48" s="159"/>
       <c r="D48" s="159"/>
@@ -12634,9 +12628,6 @@
       <c r="AA48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="97" t="s">
-        <v>112</v>
-      </c>
       <c r="B49" s="105"/>
       <c r="C49" s="159"/>
       <c r="D49" s="159"/>
@@ -12664,9 +12655,6 @@
       <c r="AA49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="97" t="s">
-        <v>113</v>
-      </c>
       <c r="B50" s="105"/>
       <c r="C50" s="159"/>
       <c r="D50" s="159"/>
@@ -12694,9 +12682,6 @@
       <c r="AA50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="97" t="s">
-        <v>114</v>
-      </c>
       <c r="B51" s="105"/>
       <c r="C51" s="159"/>
       <c r="D51" s="159"/>
@@ -12724,9 +12709,6 @@
       <c r="AA51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="97" t="s">
-        <v>115</v>
-      </c>
       <c r="B52" s="105"/>
       <c r="C52" s="159"/>
       <c r="D52" s="159"/>
@@ -12754,9 +12736,6 @@
       <c r="AA52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="97" t="s">
-        <v>116</v>
-      </c>
       <c r="B53" s="105"/>
       <c r="C53" s="159"/>
       <c r="D53" s="159"/>
@@ -12784,9 +12763,6 @@
       <c r="AA53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="97" t="s">
-        <v>117</v>
-      </c>
       <c r="B54" s="105"/>
       <c r="C54" s="159"/>
       <c r="D54" s="159"/>
@@ -12868,17 +12844,17 @@
       <c r="AA56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="160" t="s">
-        <v>118</v>
-      </c>
-      <c r="C57" s="160"/>
-      <c r="D57" s="160"/>
-      <c r="E57" s="160"/>
-      <c r="F57" s="160"/>
-      <c r="G57" s="160"/>
-      <c r="H57" s="160"/>
-      <c r="I57" s="160"/>
-      <c r="J57" s="160"/>
+      <c r="B57" s="161" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="161"/>
+      <c r="D57" s="161"/>
+      <c r="E57" s="161"/>
+      <c r="F57" s="161"/>
+      <c r="G57" s="161"/>
+      <c r="H57" s="161"/>
+      <c r="I57" s="161"/>
+      <c r="J57" s="161"/>
       <c r="L57" s="0"/>
       <c r="M57" s="0"/>
       <c r="N57" s="0"/>
@@ -12897,18 +12873,18 @@
       <c r="AA57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="161"/>
-      <c r="C58" s="162" t="str">
+      <c r="B58" s="162"/>
+      <c r="C58" s="163" t="str">
         <f aca="false">"Todistustunnus: "&amp;A1&amp;", 2/8"</f>
         <v>Todistustunnus: [:id], 2/8</v>
       </c>
-      <c r="D58" s="162"/>
-      <c r="E58" s="162"/>
-      <c r="F58" s="162"/>
-      <c r="G58" s="162"/>
-      <c r="H58" s="162"/>
-      <c r="I58" s="162"/>
-      <c r="J58" s="163"/>
+      <c r="D58" s="163"/>
+      <c r="E58" s="163"/>
+      <c r="F58" s="163"/>
+      <c r="G58" s="163"/>
+      <c r="H58" s="163"/>
+      <c r="I58" s="163"/>
+      <c r="J58" s="164"/>
       <c r="L58" s="0"/>
       <c r="M58" s="0"/>
       <c r="N58" s="0"/>
@@ -12927,7 +12903,7 @@
       <c r="AA58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="164"/>
+      <c r="B59" s="165"/>
       <c r="L59" s="0"/>
       <c r="M59" s="0"/>
       <c r="N59" s="0"/>
@@ -13003,20 +12979,20 @@
       <c r="AA63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O64" s="165"/>
+      <c r="O64" s="166"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N65" s="165"/>
-      <c r="O65" s="165"/>
-      <c r="P65" s="165"/>
-      <c r="Q65" s="165"/>
-      <c r="R65" s="165"/>
-      <c r="S65" s="165"/>
-      <c r="T65" s="165"/>
-      <c r="U65" s="165"/>
-      <c r="V65" s="165"/>
-      <c r="W65" s="165"/>
-      <c r="X65" s="165"/>
+      <c r="N65" s="166"/>
+      <c r="O65" s="166"/>
+      <c r="P65" s="166"/>
+      <c r="Q65" s="166"/>
+      <c r="R65" s="166"/>
+      <c r="S65" s="166"/>
+      <c r="T65" s="166"/>
+      <c r="U65" s="166"/>
+      <c r="V65" s="166"/>
+      <c r="W65" s="166"/>
+      <c r="X65" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="28">
@@ -13234,13 +13210,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D43" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D43" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="166" width="25.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="160" width="25.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="1.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="36.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="3" width="16.57"/>
@@ -13249,7 +13225,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="160" t="s">
         <v>0</v>
       </c>
     </row>
@@ -13258,7 +13234,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="167" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C2" s="167"/>
       <c r="D2" s="167"/>
@@ -13305,12 +13281,12 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="166" t="s">
+      <c r="A3" s="160" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="168"/>
       <c r="C3" s="169" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D3" s="170"/>
       <c r="E3" s="170"/>
@@ -13318,12 +13294,12 @@
       <c r="G3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="166" t="s">
+      <c r="A4" s="160" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="171"/>
       <c r="C4" s="172" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D4" s="173" t="str">
         <f aca="false">A2</f>
@@ -13339,12 +13315,12 @@
       <c r="L4" s="137"/>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="166" t="s">
-        <v>122</v>
+      <c r="A5" s="160" t="s">
+        <v>114</v>
       </c>
       <c r="B5" s="171"/>
       <c r="C5" s="172" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D5" s="0" t="str">
         <f aca="false">A4</f>
@@ -13358,16 +13334,16 @@
         <v>[:lahtotiedot :lammitetty-nettoala]</v>
       </c>
       <c r="G5" s="175" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="166" t="s">
-        <v>125</v>
+      <c r="A6" s="160" t="s">
+        <v>117</v>
       </c>
       <c r="B6" s="176"/>
       <c r="C6" s="177" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D6" s="178"/>
       <c r="E6" s="179"/>
@@ -13375,68 +13351,68 @@
       <c r="G6" s="180"/>
     </row>
     <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="166" t="s">
-        <v>127</v>
+      <c r="A7" s="160" t="s">
+        <v>119</v>
       </c>
       <c r="B7" s="171"/>
       <c r="C7" s="172" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D7" s="181" t="str">
         <f aca="false">A6</f>
         <v>[:lahtotiedot :rakennusvaippa :ilmanvuotoluku]</v>
       </c>
       <c r="E7" s="182" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F7" s="183"/>
       <c r="G7" s="184"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="166" t="s">
-        <v>130</v>
+      <c r="A8" s="160" t="s">
+        <v>122</v>
       </c>
       <c r="B8" s="171"/>
       <c r="C8" s="185"/>
       <c r="D8" s="186" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E8" s="186" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F8" s="186" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G8" s="187" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="166" t="s">
-        <v>135</v>
+      <c r="A9" s="160" t="s">
+        <v>127</v>
       </c>
       <c r="B9" s="171"/>
       <c r="C9" s="185"/>
       <c r="D9" s="188" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E9" s="188" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F9" s="188" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G9" s="188" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="166" t="s">
-        <v>139</v>
+      <c r="A10" s="160" t="s">
+        <v>131</v>
       </c>
       <c r="B10" s="171"/>
       <c r="C10" s="175" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D10" s="174" t="str">
         <f aca="false">A7</f>
@@ -13463,12 +13439,12 @@
       <c r="N10" s="137"/>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="166" t="s">
-        <v>141</v>
+      <c r="A11" s="160" t="s">
+        <v>133</v>
       </c>
       <c r="B11" s="171"/>
       <c r="C11" s="175" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D11" s="174" t="str">
         <f aca="false">A11</f>
@@ -13495,12 +13471,12 @@
       <c r="N11" s="137"/>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="166" t="s">
-        <v>143</v>
+      <c r="A12" s="160" t="s">
+        <v>135</v>
       </c>
       <c r="B12" s="171"/>
       <c r="C12" s="175" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D12" s="192" t="str">
         <f aca="false">A15</f>
@@ -13527,12 +13503,12 @@
       <c r="N12" s="137"/>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="166" t="s">
-        <v>145</v>
+      <c r="A13" s="160" t="s">
+        <v>137</v>
       </c>
       <c r="B13" s="171"/>
       <c r="C13" s="175" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D13" s="174" t="str">
         <f aca="false">A19</f>
@@ -13559,12 +13535,12 @@
       <c r="N13" s="137"/>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="166" t="s">
-        <v>147</v>
+      <c r="A14" s="160" t="s">
+        <v>139</v>
       </c>
       <c r="B14" s="171"/>
       <c r="C14" s="175" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D14" s="174" t="str">
         <f aca="false">A23</f>
@@ -13591,12 +13567,12 @@
       <c r="N14" s="137"/>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="166" t="s">
-        <v>149</v>
+      <c r="A15" s="160" t="s">
+        <v>141</v>
       </c>
       <c r="B15" s="171"/>
       <c r="C15" s="175" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D15" s="194" t="s">
         <v>62</v>
@@ -13621,12 +13597,12 @@
       <c r="N15" s="137"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="166" t="s">
-        <v>151</v>
+      <c r="A16" s="160" t="s">
+        <v>143</v>
       </c>
       <c r="B16" s="176"/>
       <c r="C16" s="177" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D16" s="178"/>
       <c r="E16" s="179"/>
@@ -13634,33 +13610,33 @@
       <c r="G16" s="180"/>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="166" t="s">
-        <v>153</v>
+      <c r="A17" s="160" t="s">
+        <v>145</v>
       </c>
       <c r="B17" s="171"/>
       <c r="C17" s="185"/>
       <c r="D17" s="196" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E17" s="196" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F17" s="197" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G17" s="198"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="166" t="s">
-        <v>155</v>
+      <c r="A18" s="160" t="s">
+        <v>147</v>
       </c>
       <c r="B18" s="171"/>
       <c r="C18" s="185"/>
       <c r="D18" s="188" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E18" s="188" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F18" s="199" t="s">
         <v>62</v>
@@ -13668,12 +13644,12 @@
       <c r="G18" s="198"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="166" t="s">
-        <v>156</v>
+      <c r="A19" s="160" t="s">
+        <v>148</v>
       </c>
       <c r="B19" s="171"/>
       <c r="C19" s="172" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D19" s="190" t="str">
         <f aca="false">A29</f>
@@ -13690,12 +13666,12 @@
       <c r="G19" s="198"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="166" t="s">
-        <v>158</v>
+      <c r="A20" s="160" t="s">
+        <v>150</v>
       </c>
       <c r="B20" s="171"/>
       <c r="C20" s="172" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D20" s="190" t="str">
         <f aca="false">A32</f>
@@ -13712,12 +13688,12 @@
       <c r="G20" s="198"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="166" t="s">
-        <v>160</v>
+      <c r="A21" s="160" t="s">
+        <v>152</v>
       </c>
       <c r="B21" s="171"/>
       <c r="C21" s="172" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D21" s="190" t="str">
         <f aca="false">A35</f>
@@ -13734,12 +13710,12 @@
       <c r="G21" s="198"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="166" t="s">
-        <v>162</v>
+      <c r="A22" s="160" t="s">
+        <v>154</v>
       </c>
       <c r="B22" s="171"/>
       <c r="C22" s="172" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D22" s="190" t="str">
         <f aca="false">A38</f>
@@ -13756,12 +13732,12 @@
       <c r="G22" s="198"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="166" t="s">
-        <v>164</v>
+      <c r="A23" s="160" t="s">
+        <v>156</v>
       </c>
       <c r="B23" s="171"/>
       <c r="C23" s="172" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D23" s="190" t="str">
         <f aca="false">A41</f>
@@ -13778,12 +13754,12 @@
       <c r="G23" s="198"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="166" t="s">
-        <v>166</v>
+      <c r="A24" s="160" t="s">
+        <v>158</v>
       </c>
       <c r="B24" s="171"/>
       <c r="C24" s="172" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D24" s="190" t="str">
         <f aca="false">A44</f>
@@ -13800,12 +13776,12 @@
       <c r="G24" s="198"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="166" t="s">
-        <v>168</v>
+      <c r="A25" s="160" t="s">
+        <v>160</v>
       </c>
       <c r="B25" s="171"/>
       <c r="C25" s="172" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D25" s="190" t="str">
         <f aca="false">A47</f>
@@ -13822,12 +13798,12 @@
       <c r="G25" s="198"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="166" t="s">
-        <v>170</v>
+      <c r="A26" s="160" t="s">
+        <v>162</v>
       </c>
       <c r="B26" s="171"/>
       <c r="C26" s="172" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D26" s="190" t="str">
         <f aca="false">A50</f>
@@ -13844,12 +13820,12 @@
       <c r="G26" s="198"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="166" t="s">
-        <v>172</v>
+      <c r="A27" s="160" t="s">
+        <v>164</v>
       </c>
       <c r="B27" s="168"/>
       <c r="C27" s="169" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D27" s="170"/>
       <c r="E27" s="170"/>
@@ -13857,12 +13833,12 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="166" t="s">
-        <v>174</v>
+      <c r="A28" s="160" t="s">
+        <v>166</v>
       </c>
       <c r="B28" s="171"/>
       <c r="C28" s="175" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D28" s="201" t="str">
         <f aca="false">A53</f>
@@ -13873,8 +13849,8 @@
       <c r="G28" s="201"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="166" t="s">
-        <v>176</v>
+      <c r="A29" s="160" t="s">
+        <v>168</v>
       </c>
       <c r="B29" s="202"/>
       <c r="C29" s="184"/>
@@ -13884,67 +13860,67 @@
       <c r="G29" s="204"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="166" t="s">
-        <v>177</v>
+      <c r="A30" s="160" t="s">
+        <v>169</v>
       </c>
       <c r="B30" s="171"/>
       <c r="C30" s="205"/>
       <c r="D30" s="206" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E30" s="186" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F30" s="186" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G30" s="186" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="166" t="s">
-        <v>182</v>
+      <c r="A31" s="160" t="s">
+        <v>174</v>
       </c>
       <c r="B31" s="171"/>
       <c r="C31" s="205"/>
       <c r="D31" s="207" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E31" s="196" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F31" s="196" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="G31" s="196"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="166" t="s">
-        <v>186</v>
+      <c r="A32" s="160" t="s">
+        <v>178</v>
       </c>
       <c r="B32" s="171"/>
       <c r="C32" s="205"/>
       <c r="D32" s="208" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E32" s="188" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="F32" s="188" t="s">
         <v>62</v>
       </c>
       <c r="G32" s="209" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="166" t="s">
-        <v>190</v>
+      <c r="A33" s="160" t="s">
+        <v>182</v>
       </c>
       <c r="B33" s="171"/>
       <c r="C33" s="175" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D33" s="210" t="str">
         <f aca="false">A55</f>
@@ -13964,12 +13940,12 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="166" t="s">
-        <v>192</v>
+      <c r="A34" s="160" t="s">
+        <v>184</v>
       </c>
       <c r="B34" s="171"/>
       <c r="C34" s="175" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D34" s="210" t="str">
         <f aca="false">A59</f>
@@ -13987,12 +13963,12 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="166" t="s">
-        <v>194</v>
+      <c r="A35" s="160" t="s">
+        <v>186</v>
       </c>
       <c r="B35" s="202"/>
       <c r="C35" s="214" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D35" s="215" t="str">
         <f aca="false">A61</f>
@@ -14010,12 +13986,12 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="166" t="s">
-        <v>195</v>
+      <c r="A36" s="160" t="s">
+        <v>187</v>
       </c>
       <c r="B36" s="171"/>
       <c r="C36" s="218" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D36" s="218"/>
       <c r="E36" s="219" t="str">
@@ -14026,12 +14002,12 @@
       <c r="G36" s="219"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="166" t="s">
-        <v>197</v>
+      <c r="A37" s="160" t="s">
+        <v>189</v>
       </c>
       <c r="B37" s="168"/>
       <c r="C37" s="169" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D37" s="170"/>
       <c r="E37" s="170"/>
@@ -14039,12 +14015,12 @@
       <c r="G37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="166" t="s">
-        <v>199</v>
+      <c r="A38" s="160" t="s">
+        <v>191</v>
       </c>
       <c r="B38" s="171"/>
       <c r="C38" s="172" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D38" s="220" t="str">
         <f aca="false">A64</f>
@@ -14055,8 +14031,8 @@
       <c r="G38" s="220"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="166" t="s">
-        <v>201</v>
+      <c r="A39" s="160" t="s">
+        <v>193</v>
       </c>
       <c r="B39" s="171"/>
       <c r="C39" s="203"/>
@@ -14066,44 +14042,44 @@
       <c r="G39" s="221"/>
     </row>
     <row r="40" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="166" t="s">
-        <v>202</v>
+      <c r="A40" s="160" t="s">
+        <v>194</v>
       </c>
       <c r="B40" s="222"/>
       <c r="C40" s="223"/>
       <c r="D40" s="186" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E40" s="224" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F40" s="186" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="G40" s="186" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="166" t="s">
-        <v>207</v>
+      <c r="A41" s="160" t="s">
+        <v>199</v>
       </c>
       <c r="B41" s="171"/>
       <c r="C41" s="185"/>
       <c r="D41" s="196" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="E41" s="225" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F41" s="196"/>
       <c r="G41" s="196" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="166" t="s">
-        <v>210</v>
+      <c r="A42" s="160" t="s">
+        <v>202</v>
       </c>
       <c r="B42" s="171"/>
       <c r="C42" s="185"/>
@@ -14121,12 +14097,12 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="166" t="s">
-        <v>211</v>
+      <c r="A43" s="160" t="s">
+        <v>203</v>
       </c>
       <c r="B43" s="171"/>
       <c r="C43" s="172" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D43" s="227" t="str">
         <f aca="false">A66</f>
@@ -14146,12 +14122,12 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="166" t="s">
-        <v>213</v>
+      <c r="A44" s="160" t="s">
+        <v>205</v>
       </c>
       <c r="B44" s="171"/>
       <c r="C44" s="172" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D44" s="227" t="str">
         <f aca="false">A70</f>
@@ -14171,12 +14147,12 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="166" t="s">
-        <v>215</v>
+      <c r="A45" s="160" t="s">
+        <v>207</v>
       </c>
       <c r="B45" s="171"/>
       <c r="C45" s="228" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D45" s="229"/>
       <c r="E45" s="229"/>
@@ -14184,12 +14160,12 @@
       <c r="G45" s="229"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="166" t="s">
-        <v>217</v>
+      <c r="A46" s="160" t="s">
+        <v>209</v>
       </c>
       <c r="B46" s="171"/>
       <c r="C46" s="228" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D46" s="172"/>
       <c r="E46" s="172"/>
@@ -14197,8 +14173,8 @@
       <c r="G46" s="175"/>
     </row>
     <row r="47" customFormat="false" ht="6.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="166" t="s">
-        <v>219</v>
+      <c r="A47" s="160" t="s">
+        <v>211</v>
       </c>
       <c r="B47" s="171"/>
       <c r="C47" s="230"/>
@@ -14209,42 +14185,42 @@
       <c r="J47" s="232"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="166" t="s">
-        <v>220</v>
+      <c r="A48" s="160" t="s">
+        <v>212</v>
       </c>
       <c r="B48" s="171"/>
       <c r="C48" s="185"/>
       <c r="D48" s="186" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="E48" s="186" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F48" s="233"/>
       <c r="G48" s="204"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="166" t="s">
-        <v>223</v>
+      <c r="A49" s="160" t="s">
+        <v>215</v>
       </c>
       <c r="B49" s="171"/>
       <c r="C49" s="185"/>
       <c r="D49" s="188" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E49" s="188" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="F49" s="233"/>
       <c r="G49" s="204"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="166" t="s">
-        <v>226</v>
+      <c r="A50" s="160" t="s">
+        <v>218</v>
       </c>
       <c r="B50" s="171"/>
       <c r="C50" s="172" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D50" s="210" t="str">
         <f aca="false">A74</f>
@@ -14258,12 +14234,12 @@
       <c r="G50" s="204"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="166" t="s">
-        <v>228</v>
+      <c r="A51" s="160" t="s">
+        <v>220</v>
       </c>
       <c r="B51" s="171"/>
       <c r="C51" s="172" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D51" s="210" t="str">
         <f aca="false">A76</f>
@@ -14277,12 +14253,12 @@
       <c r="G51" s="204"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="166" t="s">
-        <v>230</v>
+      <c r="A52" s="160" t="s">
+        <v>222</v>
       </c>
       <c r="B52" s="168"/>
       <c r="C52" s="169" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D52" s="170"/>
       <c r="E52" s="170"/>
@@ -14290,20 +14266,20 @@
       <c r="G52" s="11"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="166" t="s">
+      <c r="A53" s="160" t="s">
         <v>45</v>
       </c>
       <c r="B53" s="171"/>
       <c r="C53" s="185"/>
       <c r="D53" s="234" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E53" s="207"/>
       <c r="F53" s="207"/>
       <c r="G53" s="204"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="166" t="s">
+      <c r="A54" s="160" t="s">
         <v>47</v>
       </c>
       <c r="B54" s="171"/>
@@ -14316,12 +14292,12 @@
       <c r="G54" s="204"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="166" t="s">
-        <v>233</v>
+      <c r="A55" s="160" t="s">
+        <v>225</v>
       </c>
       <c r="B55" s="171"/>
       <c r="C55" s="172" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D55" s="200" t="str">
         <f aca="false">A78</f>
@@ -14332,12 +14308,12 @@
       <c r="G55" s="204"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="166" t="s">
-        <v>234</v>
+      <c r="A56" s="160" t="s">
+        <v>226</v>
       </c>
       <c r="B56" s="168"/>
       <c r="C56" s="169" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D56" s="170"/>
       <c r="E56" s="170"/>
@@ -14345,28 +14321,28 @@
       <c r="G56" s="11"/>
     </row>
     <row r="57" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="166" t="s">
-        <v>236</v>
+      <c r="A57" s="160" t="s">
+        <v>228</v>
       </c>
       <c r="B57" s="171"/>
       <c r="C57" s="203"/>
       <c r="D57" s="237" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E57" s="238" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="F57" s="203"/>
       <c r="G57" s="204"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="166" t="s">
-        <v>239</v>
+      <c r="A58" s="160" t="s">
+        <v>231</v>
       </c>
       <c r="B58" s="171"/>
       <c r="C58" s="185"/>
       <c r="D58" s="239" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E58" s="188" t="s">
         <v>61</v>
@@ -14375,12 +14351,12 @@
       <c r="G58" s="204"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="166" t="s">
-        <v>241</v>
+      <c r="A59" s="160" t="s">
+        <v>233</v>
       </c>
       <c r="B59" s="171"/>
       <c r="C59" s="172" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D59" s="240" t="str">
         <f aca="false">A79</f>
@@ -14394,12 +14370,12 @@
       <c r="G59" s="204"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="166" t="s">
-        <v>242</v>
+      <c r="A60" s="160" t="s">
+        <v>234</v>
       </c>
       <c r="B60" s="168"/>
       <c r="C60" s="169" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D60" s="170"/>
       <c r="E60" s="170"/>
@@ -14407,27 +14383,27 @@
       <c r="G60" s="243"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="166" t="s">
-        <v>244</v>
+      <c r="A61" s="160" t="s">
+        <v>236</v>
       </c>
       <c r="B61" s="171"/>
       <c r="C61" s="185"/>
       <c r="D61" s="196" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E61" s="196" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="F61" s="233" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="G61" s="196" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="166" t="s">
-        <v>249</v>
+      <c r="A62" s="160" t="s">
+        <v>241</v>
       </c>
       <c r="B62" s="171"/>
       <c r="C62" s="185"/>
@@ -14435,18 +14411,18 @@
         <v>62</v>
       </c>
       <c r="E62" s="188" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="F62" s="239" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G62" s="188" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="166" t="s">
-        <v>251</v>
+      <c r="A63" s="160" t="s">
+        <v>243</v>
       </c>
       <c r="B63" s="171"/>
       <c r="C63" s="20"/>
@@ -14468,7 +14444,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="166" t="s">
+      <c r="A64" s="160" t="s">
         <v>42</v>
       </c>
       <c r="B64" s="171"/>
@@ -14491,7 +14467,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="166" t="s">
+      <c r="A65" s="160" t="s">
         <v>44</v>
       </c>
       <c r="B65" s="245"/>
@@ -14514,23 +14490,23 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="166" t="s">
-        <v>252</v>
-      </c>
-      <c r="B66" s="162" t="str">
+      <c r="A66" s="160" t="s">
+        <v>244</v>
+      </c>
+      <c r="B66" s="163" t="str">
         <f aca="false">"Todistustunnus: "&amp;A1&amp;", 3/8"</f>
         <v>Todistustunnus: [:id], 3/8</v>
       </c>
-      <c r="C66" s="162"/>
-      <c r="D66" s="162"/>
-      <c r="E66" s="162"/>
-      <c r="F66" s="162"/>
-      <c r="G66" s="162"/>
-      <c r="H66" s="162"/>
+      <c r="C66" s="163"/>
+      <c r="D66" s="163"/>
+      <c r="E66" s="163"/>
+      <c r="F66" s="163"/>
+      <c r="G66" s="163"/>
+      <c r="H66" s="163"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="166" t="s">
-        <v>253</v>
+      <c r="A67" s="160" t="s">
+        <v>245</v>
       </c>
       <c r="B67" s="248"/>
       <c r="C67" s="4"/>
@@ -14540,128 +14516,128 @@
       <c r="G67" s="4"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="166" t="s">
+      <c r="A68" s="160" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="160" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="160" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="160" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="160" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="160" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="160" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="160" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="160" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="166" t="s">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="160" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="166" t="s">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="160" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="166" t="s">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="160" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="166" t="s">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="160" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="166" t="s">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="160" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="166" t="s">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="160" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="166" t="s">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="160" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="166" t="s">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="160" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="166" t="s">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="160" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="166" t="s">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="160" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="166" t="s">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="160" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="166" t="s">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="160" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="166" t="s">
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="160" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="166" t="s">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="160" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="166" t="s">
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="160" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="166" t="s">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="160" t="s">
         <v>270</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="166" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="166" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="166" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="166" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="166" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="166" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="166" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="166" t="s">
-        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -15194,13 +15170,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="166" width="42.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="160" width="42.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="1.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="21.57"/>
@@ -15210,7 +15186,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="160" t="s">
         <v>0</v>
       </c>
     </row>
@@ -15220,7 +15196,7 @@
       </c>
       <c r="B2" s="250"/>
       <c r="C2" s="251" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D2" s="252"/>
       <c r="E2" s="251"/>
@@ -15265,12 +15241,12 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="166" t="s">
+      <c r="A3" s="160" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="254"/>
       <c r="C3" s="255" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D3" s="256"/>
       <c r="E3" s="256"/>
@@ -15278,12 +15254,12 @@
       <c r="G3" s="257"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="166" t="s">
+      <c r="A4" s="160" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="171"/>
       <c r="C4" s="258" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D4" s="259" t="str">
         <f aca="false">A2</f>
@@ -15294,8 +15270,8 @@
       <c r="G4" s="259"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="166" t="s">
-        <v>122</v>
+      <c r="A5" s="160" t="s">
+        <v>114</v>
       </c>
       <c r="B5" s="171"/>
       <c r="C5" s="258"/>
@@ -15305,7 +15281,7 @@
       <c r="G5" s="259"/>
     </row>
     <row r="6" customFormat="false" ht="7.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="166" t="s">
+      <c r="A6" s="160" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="171"/>
@@ -15316,12 +15292,12 @@
       <c r="G6" s="261"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="166" t="s">
+      <c r="A7" s="160" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="171"/>
       <c r="C7" s="262" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D7" s="263" t="str">
         <f aca="false">A4</f>
@@ -15332,12 +15308,12 @@
       <c r="G7" s="175"/>
     </row>
     <row r="8" customFormat="false" ht="18.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="166" t="s">
+      <c r="A8" s="160" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="171"/>
       <c r="C8" s="262" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D8" s="263" t="str">
         <f aca="false">A5</f>
@@ -15348,12 +15324,12 @@
       <c r="G8" s="205"/>
     </row>
     <row r="9" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="166" t="s">
-        <v>281</v>
+      <c r="A9" s="160" t="s">
+        <v>273</v>
       </c>
       <c r="B9" s="171"/>
       <c r="C9" s="234" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D9" s="266" t="str">
         <f aca="false">A6</f>
@@ -15368,7 +15344,7 @@
       <c r="K9" s="137"/>
     </row>
     <row r="10" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="166" t="s">
+      <c r="A10" s="160" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="202"/>
@@ -15379,12 +15355,12 @@
       <c r="G10" s="184"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="166" t="s">
+      <c r="A11" s="160" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="254"/>
       <c r="C11" s="255" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="D11" s="256"/>
       <c r="E11" s="256"/>
@@ -15392,7 +15368,7 @@
       <c r="G11" s="257"/>
     </row>
     <row r="12" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="166" t="s">
+      <c r="A12" s="160" t="s">
         <v>64</v>
       </c>
       <c r="B12" s="171"/>
@@ -15403,43 +15379,43 @@
       <c r="G12" s="204"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="166" t="s">
-        <v>284</v>
+      <c r="A13" s="160" t="s">
+        <v>276</v>
       </c>
       <c r="B13" s="171"/>
       <c r="C13" s="265" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D13" s="196" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="E13" s="196" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="F13" s="197" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="G13" s="197"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="166" t="s">
+      <c r="A14" s="160" t="s">
         <v>65</v>
       </c>
       <c r="B14" s="171"/>
       <c r="C14" s="185"/>
       <c r="D14" s="196" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E14" s="196" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="F14" s="197" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="G14" s="197"/>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="166" t="s">
+      <c r="A15" s="160" t="s">
         <v>75</v>
       </c>
       <c r="B15" s="202"/>
@@ -15451,14 +15427,14 @@
         <v>62</v>
       </c>
       <c r="F15" s="239" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="G15" s="199" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="166" t="s">
+      <c r="A16" s="160" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="171"/>
@@ -15469,8 +15445,8 @@
       <c r="G16" s="197"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="166" t="s">
-        <v>293</v>
+      <c r="A17" s="160" t="s">
+        <v>285</v>
       </c>
       <c r="B17" s="171"/>
       <c r="C17" s="270" t="s">
@@ -15494,7 +15470,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="166" t="s">
+      <c r="A18" s="160" t="s">
         <v>80</v>
       </c>
       <c r="B18" s="171"/>
@@ -15519,7 +15495,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="166" t="s">
+      <c r="A19" s="160" t="s">
         <v>81</v>
       </c>
       <c r="B19" s="171"/>
@@ -15544,7 +15520,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="166" t="s">
+      <c r="A20" s="160" t="s">
         <v>84</v>
       </c>
       <c r="B20" s="171"/>
@@ -15569,8 +15545,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="166" t="s">
-        <v>294</v>
+      <c r="A21" s="160" t="s">
+        <v>286</v>
       </c>
       <c r="B21" s="171"/>
       <c r="C21" s="273" t="s">
@@ -15594,12 +15570,12 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="166" t="s">
+      <c r="A22" s="160" t="s">
         <v>86</v>
       </c>
       <c r="B22" s="171"/>
       <c r="C22" s="265" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="D22" s="274" t="str">
         <f aca="false">A42</f>
@@ -15616,7 +15592,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="166" t="s">
+      <c r="A23" s="160" t="s">
         <v>67</v>
       </c>
       <c r="B23" s="171"/>
@@ -15627,12 +15603,12 @@
       <c r="G23" s="204"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="166" t="s">
+      <c r="A24" s="160" t="s">
         <v>71</v>
       </c>
       <c r="B24" s="254"/>
       <c r="C24" s="255" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="D24" s="170"/>
       <c r="E24" s="256"/>
@@ -15640,8 +15616,8 @@
       <c r="G24" s="257"/>
     </row>
     <row r="25" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="166" t="s">
-        <v>297</v>
+      <c r="A25" s="160" t="s">
+        <v>289</v>
       </c>
       <c r="B25" s="222"/>
       <c r="C25" s="276"/>
@@ -15651,7 +15627,7 @@
       <c r="G25" s="204"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="166" t="s">
+      <c r="A26" s="160" t="s">
         <v>73</v>
       </c>
       <c r="B26" s="171"/>
@@ -15666,7 +15642,7 @@
       <c r="G26" s="204"/>
     </row>
     <row r="27" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="166" t="s">
+      <c r="A27" s="160" t="s">
         <v>87</v>
       </c>
       <c r="B27" s="171"/>
@@ -15677,12 +15653,12 @@
       <c r="G27" s="204"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="166" t="s">
+      <c r="A28" s="160" t="s">
         <v>88</v>
       </c>
       <c r="B28" s="171"/>
       <c r="C28" s="278" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D28" s="278"/>
       <c r="E28" s="241" t="str">
@@ -15696,12 +15672,12 @@
       <c r="G28" s="279"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="166" t="s">
+      <c r="A29" s="160" t="s">
         <v>91</v>
       </c>
       <c r="B29" s="171"/>
       <c r="C29" s="278" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D29" s="278"/>
       <c r="E29" s="241" t="str">
@@ -15715,12 +15691,12 @@
       <c r="G29" s="279"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="166" t="s">
-        <v>300</v>
+      <c r="A30" s="160" t="s">
+        <v>292</v>
       </c>
       <c r="B30" s="171"/>
       <c r="C30" s="280" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="D30" s="280"/>
       <c r="E30" s="241" t="str">
@@ -15734,12 +15710,12 @@
       <c r="G30" s="279"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="166" t="s">
+      <c r="A31" s="160" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="171"/>
       <c r="C31" s="280" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D31" s="280"/>
       <c r="E31" s="241" t="str">
@@ -15753,12 +15729,12 @@
       <c r="G31" s="279"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="166" t="s">
-        <v>94</v>
+      <c r="A32" s="160" t="s">
+        <v>295</v>
       </c>
       <c r="B32" s="171"/>
       <c r="C32" s="280" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="D32" s="280"/>
       <c r="E32" s="241" t="str">
@@ -15772,12 +15748,12 @@
       <c r="G32" s="279"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="166" t="s">
-        <v>95</v>
+      <c r="A33" s="160" t="s">
+        <v>297</v>
       </c>
       <c r="B33" s="171"/>
       <c r="C33" s="280" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D33" s="280"/>
       <c r="E33" s="241" t="str">
@@ -15791,8 +15767,8 @@
       <c r="G33" s="279"/>
     </row>
     <row r="34" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="166" t="s">
-        <v>97</v>
+      <c r="A34" s="160" t="s">
+        <v>299</v>
       </c>
       <c r="B34" s="202"/>
       <c r="C34" s="267"/>
@@ -15802,12 +15778,12 @@
       <c r="G34" s="204"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="166" t="s">
-        <v>305</v>
+      <c r="A35" s="160" t="s">
+        <v>300</v>
       </c>
       <c r="B35" s="254"/>
       <c r="C35" s="255" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D35" s="256"/>
       <c r="E35" s="256"/>
@@ -15815,8 +15791,8 @@
       <c r="G35" s="257"/>
     </row>
     <row r="36" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="166" t="s">
-        <v>98</v>
+      <c r="A36" s="160" t="s">
+        <v>302</v>
       </c>
       <c r="B36" s="171"/>
       <c r="C36" s="203"/>
@@ -15826,25 +15802,25 @@
       <c r="G36" s="268"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="166" t="s">
-        <v>100</v>
+      <c r="A37" s="160" t="s">
+        <v>303</v>
       </c>
       <c r="B37" s="171"/>
       <c r="C37" s="185"/>
       <c r="D37" s="185"/>
       <c r="E37" s="196" t="s">
+        <v>304</v>
+      </c>
+      <c r="F37" s="196" t="s">
+        <v>305</v>
+      </c>
+      <c r="G37" s="196" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="160" t="s">
         <v>307</v>
-      </c>
-      <c r="F37" s="196" t="s">
-        <v>308</v>
-      </c>
-      <c r="G37" s="196" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="166" t="s">
-        <v>102</v>
       </c>
       <c r="B38" s="171"/>
       <c r="C38" s="185"/>
@@ -15860,8 +15836,8 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="6.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="166" t="s">
-        <v>104</v>
+      <c r="A39" s="160" t="s">
+        <v>308</v>
       </c>
       <c r="B39" s="171"/>
       <c r="C39" s="185"/>
@@ -15871,12 +15847,12 @@
       <c r="G39" s="196"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="166" t="s">
-        <v>310</v>
+      <c r="A40" s="160" t="s">
+        <v>309</v>
       </c>
       <c r="B40" s="171"/>
       <c r="C40" s="172" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D40" s="172"/>
       <c r="E40" s="0"/>
@@ -15884,8 +15860,8 @@
       <c r="G40" s="282"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="166" t="s">
-        <v>105</v>
+      <c r="A41" s="160" t="s">
+        <v>310</v>
       </c>
       <c r="B41" s="171"/>
       <c r="C41" s="172" t="s">
@@ -15905,7 +15881,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="166" t="s">
+      <c r="A42" s="160" t="s">
         <v>312</v>
       </c>
       <c r="B42" s="171"/>
@@ -15926,7 +15902,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="166" t="s">
+      <c r="A43" s="160" t="s">
         <v>314</v>
       </c>
       <c r="B43" s="171"/>
@@ -15947,7 +15923,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="166" t="s">
+      <c r="A44" s="160" t="s">
         <v>22</v>
       </c>
       <c r="B44" s="171"/>
@@ -15967,12 +15943,12 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="166" t="s">
+      <c r="A45" s="160" t="s">
         <v>317</v>
       </c>
       <c r="B45" s="171"/>
       <c r="C45" s="172" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D45" s="172"/>
       <c r="E45" s="241" t="str">
@@ -15989,7 +15965,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="166" t="s">
+      <c r="A46" s="160" t="s">
         <v>318</v>
       </c>
       <c r="B46" s="171"/>
@@ -16009,12 +15985,12 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="166" t="s">
+      <c r="A47" s="160" t="s">
         <v>320</v>
       </c>
       <c r="B47" s="171"/>
       <c r="C47" s="265" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="D47" s="265"/>
       <c r="E47" s="283" t="str">
@@ -16031,7 +16007,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="166" t="s">
+      <c r="A48" s="160" t="s">
         <v>321</v>
       </c>
       <c r="B48" s="171"/>
@@ -16044,7 +16020,7 @@
       <c r="G48" s="195"/>
     </row>
     <row r="49" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="166" t="s">
+      <c r="A49" s="160" t="s">
         <v>323</v>
       </c>
       <c r="B49" s="171"/>
@@ -16055,7 +16031,7 @@
       <c r="G49" s="221"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="166" t="s">
+      <c r="A50" s="160" t="s">
         <v>324</v>
       </c>
       <c r="B50" s="254"/>
@@ -16068,7 +16044,7 @@
       <c r="G50" s="257"/>
     </row>
     <row r="51" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="166" t="s">
+      <c r="A51" s="160" t="s">
         <v>326</v>
       </c>
       <c r="B51" s="171"/>
@@ -16079,7 +16055,7 @@
       <c r="G51" s="268"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="166" t="s">
+      <c r="A52" s="160" t="s">
         <v>327</v>
       </c>
       <c r="B52" s="171"/>
@@ -16094,7 +16070,7 @@
       <c r="G52" s="195"/>
     </row>
     <row r="53" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="166" t="s">
+      <c r="A53" s="160" t="s">
         <v>328</v>
       </c>
       <c r="B53" s="171"/>
@@ -16105,7 +16081,7 @@
       <c r="G53" s="196"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="166" t="s">
+      <c r="A54" s="160" t="s">
         <v>329</v>
       </c>
       <c r="B54" s="171"/>
@@ -16124,7 +16100,7 @@
       <c r="G54" s="241"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="166" t="s">
+      <c r="A55" s="160" t="s">
         <v>331</v>
       </c>
       <c r="B55" s="171"/>
@@ -16143,12 +16119,12 @@
       <c r="G55" s="274"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="166" t="s">
+      <c r="A56" s="160" t="s">
         <v>333</v>
       </c>
       <c r="B56" s="171"/>
       <c r="C56" s="172" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D56" s="172"/>
       <c r="E56" s="241" t="str">
@@ -16162,7 +16138,7 @@
       <c r="G56" s="241"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="166" t="s">
+      <c r="A57" s="160" t="s">
         <v>334</v>
       </c>
       <c r="B57" s="171"/>
@@ -16181,7 +16157,7 @@
       <c r="G57" s="274"/>
     </row>
     <row r="58" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="166" t="s">
+      <c r="A58" s="160" t="s">
         <v>336</v>
       </c>
       <c r="B58" s="171"/>
@@ -16192,7 +16168,7 @@
       <c r="G58" s="285"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="166" t="s">
+      <c r="A59" s="160" t="s">
         <v>337</v>
       </c>
       <c r="B59" s="171"/>
@@ -16205,7 +16181,7 @@
       <c r="G59" s="285"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="166" t="s">
+      <c r="A60" s="160" t="s">
         <v>339</v>
       </c>
       <c r="B60" s="171"/>
@@ -16218,7 +16194,7 @@
       <c r="G60" s="289"/>
     </row>
     <row r="61" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="166" t="s">
+      <c r="A61" s="160" t="s">
         <v>341</v>
       </c>
       <c r="B61" s="171"/>
@@ -16229,7 +16205,7 @@
       <c r="G61" s="221"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="166" t="s">
+      <c r="A62" s="160" t="s">
         <v>342</v>
       </c>
       <c r="B62" s="254"/>
@@ -16242,7 +16218,7 @@
       <c r="G62" s="257"/>
     </row>
     <row r="63" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="166" t="s">
+      <c r="A63" s="160" t="s">
         <v>344</v>
       </c>
       <c r="B63" s="171"/>
@@ -16253,7 +16229,7 @@
       <c r="G63" s="268"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="166" t="s">
+      <c r="A64" s="160" t="s">
         <v>345</v>
       </c>
       <c r="B64" s="171"/>
@@ -16268,7 +16244,7 @@
       <c r="G64" s="196"/>
     </row>
     <row r="65" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="166" t="s">
+      <c r="A65" s="160" t="s">
         <v>346</v>
       </c>
       <c r="B65" s="171"/>
@@ -16279,7 +16255,7 @@
       <c r="G65" s="196"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="166" t="s">
+      <c r="A66" s="160" t="s">
         <v>347</v>
       </c>
       <c r="B66" s="171"/>
@@ -16298,12 +16274,12 @@
       <c r="G66" s="274"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="166" t="s">
+      <c r="A67" s="160" t="s">
         <v>349</v>
       </c>
       <c r="B67" s="171"/>
       <c r="C67" s="172" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="D67" s="172"/>
       <c r="E67" s="241" t="str">
@@ -16317,12 +16293,12 @@
       <c r="G67" s="274"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="166" t="s">
+      <c r="A68" s="160" t="s">
         <v>350</v>
       </c>
       <c r="B68" s="171"/>
       <c r="C68" s="172" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D68" s="172"/>
       <c r="E68" s="241" t="str">
@@ -16336,12 +16312,12 @@
       <c r="G68" s="274"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="166" t="s">
+      <c r="A69" s="160" t="s">
         <v>351</v>
       </c>
       <c r="B69" s="171"/>
       <c r="C69" s="172" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D69" s="172"/>
       <c r="E69" s="241" t="str">
@@ -16355,7 +16331,7 @@
       <c r="G69" s="274"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="166" t="s">
+      <c r="A70" s="160" t="s">
         <v>352</v>
       </c>
       <c r="B70" s="171"/>
@@ -16374,7 +16350,7 @@
       <c r="G70" s="274"/>
     </row>
     <row r="71" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="166" t="s">
+      <c r="A71" s="160" t="s">
         <v>354</v>
       </c>
       <c r="B71" s="171"/>
@@ -16385,7 +16361,7 @@
       <c r="G71" s="221"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="166" t="s">
+      <c r="A72" s="160" t="s">
         <v>355</v>
       </c>
       <c r="B72" s="254"/>
@@ -16398,7 +16374,7 @@
       <c r="G72" s="257"/>
     </row>
     <row r="73" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="166" t="s">
+      <c r="A73" s="160" t="s">
         <v>357</v>
       </c>
       <c r="B73" s="171"/>
@@ -16409,7 +16385,7 @@
       <c r="G73" s="277"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="166" t="s">
+      <c r="A74" s="160" t="s">
         <v>358</v>
       </c>
       <c r="B74" s="171"/>
@@ -16425,7 +16401,7 @@
       <c r="G74" s="290"/>
     </row>
     <row r="75" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="166" t="s">
+      <c r="A75" s="160" t="s">
         <v>359</v>
       </c>
       <c r="B75" s="245"/>
@@ -16436,12 +16412,12 @@
       <c r="G75" s="291"/>
     </row>
     <row r="76" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="166" t="s">
+      <c r="A76" s="160" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="166" t="s">
+      <c r="A77" s="160" t="s">
         <v>361</v>
       </c>
       <c r="B77" s="292" t="str">
@@ -16455,182 +16431,182 @@
       <c r="G77" s="292"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="166" t="s">
+      <c r="A78" s="160" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="166" t="s">
+      <c r="A79" s="160" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="166" t="s">
+      <c r="A80" s="160" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="166" t="s">
+      <c r="A81" s="160" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="166" t="s">
+      <c r="A82" s="160" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="166" t="s">
+      <c r="A83" s="160" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="166" t="s">
+      <c r="A84" s="160" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="166" t="s">
+      <c r="A85" s="160" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="166" t="s">
+      <c r="A86" s="160" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="166" t="s">
+      <c r="A87" s="160" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="166" t="s">
+      <c r="A88" s="160" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="166" t="s">
+      <c r="A89" s="160" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="166" t="s">
+      <c r="A90" s="160" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="166" t="s">
+      <c r="A91" s="160" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="166" t="s">
+      <c r="A92" s="160" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="166" t="s">
+      <c r="A93" s="160" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="166" t="s">
+      <c r="A94" s="160" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="166" t="s">
+      <c r="A95" s="160" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="166" t="s">
+      <c r="A96" s="160" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="166" t="s">
+      <c r="A97" s="160" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="166" t="s">
+      <c r="A98" s="160" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="166" t="s">
+      <c r="A99" s="160" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="166" t="s">
+      <c r="A100" s="160" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="166" t="s">
+      <c r="A101" s="160" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="166" t="s">
+      <c r="A102" s="160" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="166" t="s">
+      <c r="A103" s="160" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="166" t="s">
+      <c r="A104" s="160" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="166" t="s">
+      <c r="A105" s="160" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="166" t="s">
+      <c r="A106" s="160" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="166" t="s">
+      <c r="A107" s="160" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="166" t="s">
+      <c r="A108" s="160" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="166" t="s">
+      <c r="A109" s="160" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="166" t="s">
+      <c r="A110" s="160" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="166" t="s">
+      <c r="A111" s="160" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="166" t="s">
+      <c r="A112" s="160" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="166" t="s">
+      <c r="A113" s="160" t="s">
         <v>397</v>
       </c>
     </row>
@@ -17119,7 +17095,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -17144,7 +17120,7 @@
     </row>
     <row r="2" s="298" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="293" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B2" s="294"/>
       <c r="C2" s="295" t="s">
@@ -17207,7 +17183,7 @@
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="97" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B3" s="105"/>
       <c r="C3" s="299" t="s">
@@ -17548,7 +17524,7 @@
       </c>
       <c r="B19" s="105"/>
       <c r="C19" s="108" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D19" s="108"/>
       <c r="E19" s="108"/>
@@ -18117,7 +18093,7 @@
       </c>
       <c r="B44" s="105"/>
       <c r="C44" s="32" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D44" s="32"/>
       <c r="E44" s="32"/>
@@ -18155,7 +18131,7 @@
       </c>
       <c r="B46" s="105"/>
       <c r="C46" s="16" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -18857,7 +18833,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -18872,7 +18848,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="160" t="s">
         <v>0</v>
       </c>
     </row>
@@ -18919,7 +18895,7 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="166" t="s">
+      <c r="A3" s="160" t="s">
         <v>490</v>
       </c>
       <c r="B3" s="370" t="s">
@@ -19007,7 +18983,7 @@
       <c r="F10" s="374"/>
     </row>
     <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="166" t="s">
+      <c r="A11" s="160" t="s">
         <v>500</v>
       </c>
       <c r="B11" s="375" t="s">
@@ -19019,7 +18995,7 @@
       <c r="F11" s="375"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="166" t="s">
+      <c r="A12" s="160" t="s">
         <v>502</v>
       </c>
       <c r="B12" s="376" t="n">
@@ -19034,7 +19010,7 @@
       <c r="F12" s="377"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="166" t="s">
+      <c r="A13" s="160" t="s">
         <v>503</v>
       </c>
       <c r="B13" s="376" t="n">
@@ -19049,7 +19025,7 @@
       <c r="F13" s="377"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="166" t="s">
+      <c r="A14" s="160" t="s">
         <v>504</v>
       </c>
       <c r="B14" s="376" t="n">
@@ -19064,7 +19040,7 @@
       <c r="F14" s="377"/>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="166" t="s">
+      <c r="A15" s="160" t="s">
         <v>505</v>
       </c>
       <c r="B15" s="378"/>
@@ -19082,7 +19058,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="166" t="s">
+      <c r="A16" s="160" t="s">
         <v>510</v>
       </c>
       <c r="B16" s="381"/>
@@ -19100,7 +19076,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="166" t="s">
+      <c r="A17" s="160" t="s">
         <v>511</v>
       </c>
       <c r="B17" s="376" t="n">
@@ -19124,7 +19100,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="166" t="s">
+      <c r="A18" s="160" t="s">
         <v>512</v>
       </c>
       <c r="B18" s="376" t="n">
@@ -19148,7 +19124,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="166" t="s">
+      <c r="A19" s="160" t="s">
         <v>513</v>
       </c>
       <c r="B19" s="376" t="n">
@@ -19172,7 +19148,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="166" t="s">
+      <c r="A20" s="160" t="s">
         <v>514</v>
       </c>
       <c r="B20" s="383" t="s">
@@ -19184,7 +19160,7 @@
       <c r="F20" s="384"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="166" t="s">
+      <c r="A21" s="160" t="s">
         <v>516</v>
       </c>
       <c r="B21" s="374" t="str">
@@ -19197,7 +19173,7 @@
       <c r="F21" s="374"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="166" t="s">
+      <c r="A22" s="160" t="s">
         <v>517</v>
       </c>
       <c r="B22" s="374"/>
@@ -19207,7 +19183,7 @@
       <c r="F22" s="374"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="166" t="s">
+      <c r="A23" s="160" t="s">
         <v>518</v>
       </c>
       <c r="B23" s="374"/>
@@ -19217,7 +19193,7 @@
       <c r="F23" s="374"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="166" t="s">
+      <c r="A24" s="160" t="s">
         <v>519</v>
       </c>
       <c r="B24" s="374"/>
@@ -19227,7 +19203,7 @@
       <c r="F24" s="374"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="166" t="s">
+      <c r="A25" s="160" t="s">
         <v>520</v>
       </c>
       <c r="B25" s="374"/>
@@ -19237,7 +19213,7 @@
       <c r="F25" s="374"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="166" t="s">
+      <c r="A26" s="160" t="s">
         <v>521</v>
       </c>
       <c r="B26" s="374"/>
@@ -19247,7 +19223,7 @@
       <c r="F26" s="374"/>
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="166" t="s">
+      <c r="A27" s="160" t="s">
         <v>522</v>
       </c>
       <c r="B27" s="375" t="s">
@@ -19259,7 +19235,7 @@
       <c r="F27" s="375"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="166" t="s">
+      <c r="A28" s="160" t="s">
         <v>523</v>
       </c>
       <c r="B28" s="376" t="n">
@@ -19274,7 +19250,7 @@
       <c r="F28" s="377"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="166" t="s">
+      <c r="A29" s="160" t="s">
         <v>524</v>
       </c>
       <c r="B29" s="376" t="n">
@@ -19289,7 +19265,7 @@
       <c r="F29" s="377"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="166" t="s">
+      <c r="A30" s="160" t="s">
         <v>525</v>
       </c>
       <c r="B30" s="376" t="n">
@@ -19304,7 +19280,7 @@
       <c r="F30" s="377"/>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="166" t="s">
+      <c r="A31" s="160" t="s">
         <v>526</v>
       </c>
       <c r="B31" s="385"/>
@@ -19322,7 +19298,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="166" t="s">
+      <c r="A32" s="160" t="s">
         <v>529</v>
       </c>
       <c r="B32" s="385"/>
@@ -19340,7 +19316,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="166" t="s">
+      <c r="A33" s="160" t="s">
         <v>530</v>
       </c>
       <c r="B33" s="376" t="n">
@@ -19364,7 +19340,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="166" t="s">
+      <c r="A34" s="160" t="s">
         <v>531</v>
       </c>
       <c r="B34" s="376" t="n">
@@ -19388,7 +19364,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="166" t="s">
+      <c r="A35" s="160" t="s">
         <v>532</v>
       </c>
       <c r="B35" s="376" t="n">
@@ -19412,7 +19388,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="166" t="s">
+      <c r="A36" s="160" t="s">
         <v>533</v>
       </c>
       <c r="B36" s="383" t="s">
@@ -19424,7 +19400,7 @@
       <c r="F36" s="384"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="166" t="s">
+      <c r="A37" s="160" t="s">
         <v>535</v>
       </c>
       <c r="B37" s="374" t="str">
@@ -19437,7 +19413,7 @@
       <c r="F37" s="374"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="166" t="s">
+      <c r="A38" s="160" t="s">
         <v>536</v>
       </c>
       <c r="B38" s="374"/>
@@ -19447,7 +19423,7 @@
       <c r="F38" s="374"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="166" t="s">
+      <c r="A39" s="160" t="s">
         <v>537</v>
       </c>
       <c r="B39" s="374"/>
@@ -19457,7 +19433,7 @@
       <c r="F39" s="374"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="166" t="s">
+      <c r="A40" s="160" t="s">
         <v>538</v>
       </c>
       <c r="B40" s="374"/>
@@ -19467,7 +19443,7 @@
       <c r="F40" s="374"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="166" t="s">
+      <c r="A41" s="160" t="s">
         <v>539</v>
       </c>
       <c r="B41" s="374"/>
@@ -19477,7 +19453,7 @@
       <c r="F41" s="374"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="166" t="s">
+      <c r="A42" s="160" t="s">
         <v>540</v>
       </c>
       <c r="B42" s="374"/>
@@ -19487,7 +19463,7 @@
       <c r="F42" s="374"/>
     </row>
     <row r="43" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="166" t="s">
+      <c r="A43" s="160" t="s">
         <v>541</v>
       </c>
       <c r="B43" s="375" t="s">
@@ -19499,7 +19475,7 @@
       <c r="F43" s="375"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="166" t="s">
+      <c r="A44" s="160" t="s">
         <v>542</v>
       </c>
       <c r="B44" s="376" t="n">
@@ -19514,7 +19490,7 @@
       <c r="F44" s="377"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="166" t="s">
+      <c r="A45" s="160" t="s">
         <v>543</v>
       </c>
       <c r="B45" s="376" t="n">
@@ -19529,7 +19505,7 @@
       <c r="F45" s="377"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="166" t="s">
+      <c r="A46" s="160" t="s">
         <v>544</v>
       </c>
       <c r="B46" s="376" t="n">
@@ -19544,7 +19520,7 @@
       <c r="F46" s="377"/>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="166" t="s">
+      <c r="A47" s="160" t="s">
         <v>545</v>
       </c>
       <c r="B47" s="385"/>
@@ -19562,7 +19538,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="166" t="s">
+      <c r="A48" s="160" t="s">
         <v>547</v>
       </c>
       <c r="B48" s="385"/>
@@ -19580,7 +19556,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="166" t="s">
+      <c r="A49" s="160" t="s">
         <v>548</v>
       </c>
       <c r="B49" s="376" t="n">
@@ -19604,7 +19580,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="166" t="s">
+      <c r="A50" s="160" t="s">
         <v>549</v>
       </c>
       <c r="B50" s="376" t="n">
@@ -19628,7 +19604,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="166" t="s">
+      <c r="A51" s="160" t="s">
         <v>550</v>
       </c>
       <c r="B51" s="376" t="n">
@@ -19890,7 +19866,7 @@
   </sheetPr>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
     </sheetView>
   </sheetViews>
@@ -19905,7 +19881,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="160" t="s">
         <v>0</v>
       </c>
     </row>
@@ -19997,7 +19973,7 @@
       <c r="F9" s="374"/>
     </row>
     <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="166" t="s">
+      <c r="A10" s="160" t="s">
         <v>570</v>
       </c>
       <c r="B10" s="388" t="s">
@@ -20009,7 +19985,7 @@
       <c r="F10" s="388"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="166" t="s">
+      <c r="A11" s="160" t="s">
         <v>571</v>
       </c>
       <c r="B11" s="376" t="n">
@@ -20024,7 +20000,7 @@
       <c r="F11" s="389"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="166" t="s">
+      <c r="A12" s="160" t="s">
         <v>572</v>
       </c>
       <c r="B12" s="376" t="n">
@@ -20039,7 +20015,7 @@
       <c r="F12" s="389"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="166" t="s">
+      <c r="A13" s="160" t="s">
         <v>573</v>
       </c>
       <c r="B13" s="376" t="n">
@@ -20054,7 +20030,7 @@
       <c r="F13" s="389"/>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="166" t="s">
+      <c r="A14" s="160" t="s">
         <v>574</v>
       </c>
       <c r="B14" s="385"/>
@@ -20072,7 +20048,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="166" t="s">
+      <c r="A15" s="160" t="s">
         <v>575</v>
       </c>
       <c r="B15" s="385"/>
@@ -20090,7 +20066,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="166" t="s">
+      <c r="A16" s="160" t="s">
         <v>576</v>
       </c>
       <c r="B16" s="376" t="n">
@@ -20114,7 +20090,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="166" t="s">
+      <c r="A17" s="160" t="s">
         <v>577</v>
       </c>
       <c r="B17" s="376" t="n">
@@ -20138,7 +20114,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="166" t="s">
+      <c r="A18" s="160" t="s">
         <v>578</v>
       </c>
       <c r="B18" s="376" t="n">
@@ -20162,7 +20138,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="166" t="s">
+      <c r="A19" s="160" t="s">
         <v>579</v>
       </c>
       <c r="B19" s="383" t="s">
@@ -20174,7 +20150,7 @@
       <c r="F19" s="384"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="166" t="s">
+      <c r="A20" s="160" t="s">
         <v>581</v>
       </c>
       <c r="B20" s="374" t="str">
@@ -20187,7 +20163,7 @@
       <c r="F20" s="374"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="166" t="s">
+      <c r="A21" s="160" t="s">
         <v>582</v>
       </c>
       <c r="B21" s="374"/>
@@ -20197,7 +20173,7 @@
       <c r="F21" s="374"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="166" t="s">
+      <c r="A22" s="160" t="s">
         <v>583</v>
       </c>
       <c r="B22" s="374"/>
@@ -20207,7 +20183,7 @@
       <c r="F22" s="374"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="166" t="s">
+      <c r="A23" s="160" t="s">
         <v>584</v>
       </c>
       <c r="B23" s="374"/>
@@ -20217,7 +20193,7 @@
       <c r="F23" s="374"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="166" t="s">
+      <c r="A24" s="160" t="s">
         <v>585</v>
       </c>
       <c r="B24" s="374"/>
@@ -20227,7 +20203,7 @@
       <c r="F24" s="374"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="166" t="s">
+      <c r="A25" s="160" t="s">
         <v>586</v>
       </c>
       <c r="B25" s="374"/>
@@ -20237,7 +20213,7 @@
       <c r="F25" s="374"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="166" t="s">
+      <c r="A26" s="160" t="s">
         <v>587</v>
       </c>
       <c r="B26" s="374"/>
@@ -20247,7 +20223,7 @@
       <c r="F26" s="374"/>
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="166" t="s">
+      <c r="A27" s="160" t="s">
         <v>588</v>
       </c>
       <c r="B27" s="388" t="s">
@@ -20259,7 +20235,7 @@
       <c r="F27" s="388"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="166" t="s">
+      <c r="A28" s="160" t="s">
         <v>589</v>
       </c>
       <c r="B28" s="376" t="n">
@@ -20274,7 +20250,7 @@
       <c r="F28" s="389"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="166" t="s">
+      <c r="A29" s="160" t="s">
         <v>590</v>
       </c>
       <c r="B29" s="376" t="n">
@@ -20289,7 +20265,7 @@
       <c r="F29" s="389"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="166" t="s">
+      <c r="A30" s="160" t="s">
         <v>591</v>
       </c>
       <c r="B30" s="376" t="n">
@@ -20304,7 +20280,7 @@
       <c r="F30" s="389"/>
     </row>
     <row r="31" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="166" t="s">
+      <c r="A31" s="160" t="s">
         <v>592</v>
       </c>
       <c r="B31" s="385"/>
@@ -20322,7 +20298,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="166" t="s">
+      <c r="A32" s="160" t="s">
         <v>593</v>
       </c>
       <c r="B32" s="385"/>
@@ -20340,7 +20316,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="166" t="s">
+      <c r="A33" s="160" t="s">
         <v>594</v>
       </c>
       <c r="B33" s="376" t="n">
@@ -20364,7 +20340,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="166" t="s">
+      <c r="A34" s="160" t="s">
         <v>595</v>
       </c>
       <c r="B34" s="376" t="n">
@@ -20388,7 +20364,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="166" t="s">
+      <c r="A35" s="160" t="s">
         <v>596</v>
       </c>
       <c r="B35" s="376" t="n">
@@ -20412,7 +20388,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="166" t="s">
+      <c r="A36" s="160" t="s">
         <v>597</v>
       </c>
       <c r="B36" s="390" t="s">
@@ -20424,7 +20400,7 @@
       <c r="F36" s="390"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="166" t="s">
+      <c r="A37" s="160" t="s">
         <v>599</v>
       </c>
       <c r="B37" s="374" t="str">
@@ -20437,7 +20413,7 @@
       <c r="F37" s="374"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="166" t="s">
+      <c r="A38" s="160" t="s">
         <v>600</v>
       </c>
       <c r="B38" s="374"/>
@@ -20447,7 +20423,7 @@
       <c r="F38" s="374"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="166" t="s">
+      <c r="A39" s="160" t="s">
         <v>601</v>
       </c>
       <c r="B39" s="374"/>
@@ -20457,7 +20433,7 @@
       <c r="F39" s="374"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="166" t="s">
+      <c r="A40" s="160" t="s">
         <v>602</v>
       </c>
       <c r="B40" s="374"/>
@@ -20467,7 +20443,7 @@
       <c r="F40" s="374"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="166" t="s">
+      <c r="A41" s="160" t="s">
         <v>603</v>
       </c>
       <c r="B41" s="374"/>
@@ -20477,7 +20453,7 @@
       <c r="F41" s="374"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="166" t="s">
+      <c r="A42" s="160" t="s">
         <v>604</v>
       </c>
       <c r="B42" s="374"/>
@@ -20487,7 +20463,7 @@
       <c r="F42" s="374"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="166" t="s">
+      <c r="A43" s="160" t="s">
         <v>605</v>
       </c>
       <c r="B43" s="374"/>
@@ -20497,7 +20473,7 @@
       <c r="F43" s="374"/>
     </row>
     <row r="44" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="166" t="s">
+      <c r="A44" s="160" t="s">
         <v>606</v>
       </c>
       <c r="B44" s="374"/>
@@ -20507,7 +20483,7 @@
       <c r="F44" s="374"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="166" t="s">
+      <c r="A45" s="160" t="s">
         <v>607</v>
       </c>
       <c r="B45" s="374"/>
@@ -20517,7 +20493,7 @@
       <c r="F45" s="374"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="166"/>
+      <c r="A46" s="160"/>
       <c r="B46" s="374"/>
       <c r="C46" s="374"/>
       <c r="D46" s="374"/>
@@ -20525,7 +20501,7 @@
       <c r="F46" s="374"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="166"/>
+      <c r="A47" s="160"/>
       <c r="B47" s="374"/>
       <c r="C47" s="374"/>
       <c r="D47" s="374"/>
@@ -20533,7 +20509,7 @@
       <c r="F47" s="374"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="166"/>
+      <c r="A48" s="160"/>
       <c r="B48" s="374"/>
       <c r="C48" s="374"/>
       <c r="D48" s="374"/>
@@ -20541,7 +20517,7 @@
       <c r="F48" s="374"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="166"/>
+      <c r="A49" s="160"/>
       <c r="B49" s="374"/>
       <c r="C49" s="374"/>
       <c r="D49" s="374"/>
@@ -20549,7 +20525,7 @@
       <c r="F49" s="374"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="166"/>
+      <c r="A50" s="160"/>
       <c r="B50" s="374"/>
       <c r="C50" s="374"/>
       <c r="D50" s="374"/>
@@ -20557,7 +20533,7 @@
       <c r="F50" s="374"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="166"/>
+      <c r="A51" s="160"/>
       <c r="B51" s="374"/>
       <c r="C51" s="374"/>
       <c r="D51" s="374"/>
@@ -20574,7 +20550,7 @@
       <c r="F52" s="373"/>
     </row>
     <row r="53" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="166"/>
+      <c r="A53" s="160"/>
       <c r="B53" s="158"/>
       <c r="C53" s="5"/>
       <c r="D53" s="4"/>
@@ -20582,7 +20558,7 @@
       <c r="F53" s="391"/>
     </row>
     <row r="54" customFormat="false" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="166"/>
+      <c r="A54" s="160"/>
       <c r="B54" s="333" t="s">
         <v>609</v>
       </c>
@@ -20592,7 +20568,7 @@
       <c r="F54" s="333"/>
     </row>
     <row r="55" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="166"/>
+      <c r="A55" s="160"/>
       <c r="B55" s="392" t="str">
         <f aca="false">A44</f>
         <v>[:huomiot :lisatietoja-fi]</v>
@@ -20603,7 +20579,7 @@
       <c r="F55" s="392"/>
     </row>
     <row r="56" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="166"/>
+      <c r="A56" s="160"/>
       <c r="B56" s="392"/>
       <c r="C56" s="392"/>
       <c r="D56" s="392"/>
@@ -20611,7 +20587,7 @@
       <c r="F56" s="392"/>
     </row>
     <row r="57" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="166"/>
+      <c r="A57" s="160"/>
       <c r="B57" s="392"/>
       <c r="C57" s="392"/>
       <c r="D57" s="392"/>
@@ -20755,7 +20731,7 @@
   </sheetPr>
   <dimension ref="A1:Q140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
@@ -20771,12 +20747,12 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="7.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="160" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="166" t="s">
+      <c r="A2" s="160" t="s">
         <v>610</v>
       </c>
       <c r="B2" s="393"/>
@@ -21445,7 +21421,7 @@
         <v>656</v>
       </c>
       <c r="E39" s="411" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="F39" s="411" t="s">
         <v>657</v>
@@ -21460,16 +21436,16 @@
         <v>660</v>
       </c>
       <c r="J39" s="411" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="K39" s="411" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="L39" s="411" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M39" s="411" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
AE-825 remove kuukausierittely from last page in 2018 xlsx templates
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,23 +19,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'1) etusivu'!$B$1:$R$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$M$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$B$1:$R$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$66</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$L$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$N$62</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0" vbProcedure="false">'8) lisämerkintöjä'!$B$1:$M$63</definedName>
   </definedNames>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="761">
   <si>
     <t xml:space="preserve">[:id]</t>
   </si>
@@ -2935,175 +2935,55 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">Kuukausitason erittely ympäristöstä olevasta energiasta otetun energian määrästä</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 2 :kulutus :sahko]</t>
   </si>
   <si>
-    <t xml:space="preserve">Sähköenergiantuotto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lämpöenergiantuotto</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF009EE0"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Energiankulutus</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF009EE0"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Hyödynnetty osuus</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 2 :kulutus :lampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">Kuukausi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kWh/kk</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 2 :hyoty :sahko]</t>
   </si>
   <si>
-    <t xml:space="preserve">Aurinko-sähkö</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muu sähkö</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aurinko-lämpö</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lämpö-pumppu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muu lämpö</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 2 :hyoty :lampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">Tammikuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :aurinkosahko]</t>
   </si>
   <si>
-    <t xml:space="preserve">Helmikuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :tuulisahko]</t>
   </si>
   <si>
-    <t xml:space="preserve">Maaliskuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :muusahko]</t>
   </si>
   <si>
-    <t xml:space="preserve">Huhtikuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :aurinkolampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">Toukokuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :lampopumppu]</t>
   </si>
   <si>
-    <t xml:space="preserve">Kesäkuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">Heinäkuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :kulutus :sahko]</t>
   </si>
   <si>
-    <t xml:space="preserve">Elokuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :kulutus :lampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">Syyskuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :hyoty :sahko]</t>
   </si>
   <si>
-    <t xml:space="preserve">Lokakuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :hyoty :lampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">Marraskuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :aurinkosahko]</t>
   </si>
   <si>
-    <t xml:space="preserve">Joulukuu</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :tuulisahko]</t>
   </si>
   <si>
-    <t xml:space="preserve">Yhteensä</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :muusahko]</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="7.5"/>
-        <color rgb="FF009EE0"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7.5"/>
-        <color rgb="FF009EE0"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Energiankulutukseen merkitään se osuus rakennuksen energiankulutuksesta, jonka määrää voidaan vähentää ympäristössä olevasta energiasta otetulla energialla.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :aurinkolampo]</t>
@@ -3574,9 +3454,9 @@
   <numFmts count="11">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="00000"/>
-    <numFmt numFmtId="166" formatCode="#,##0"/>
-    <numFmt numFmtId="167" formatCode="[$-409]m/d/yyyy"/>
-    <numFmt numFmtId="168" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="[$-409]m/d/yyyy"/>
     <numFmt numFmtId="169" formatCode="[$-40B]0"/>
     <numFmt numFmtId="170" formatCode="[$-40B]0.00"/>
     <numFmt numFmtId="171" formatCode="[$-40B]General"/>
@@ -3584,7 +3464,7 @@
     <numFmt numFmtId="173" formatCode="0%"/>
     <numFmt numFmtId="174" formatCode="0"/>
   </numFmts>
-  <fonts count="55">
+  <fonts count="48">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3925,60 +3805,6 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="7.5"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="7.5"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -4281,7 +4107,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="429">
+  <cellXfs count="409">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4398,7 +4224,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -4426,7 +4252,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -4550,11 +4376,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4602,7 +4428,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4662,11 +4488,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4718,7 +4544,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4726,7 +4552,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4734,7 +4560,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4826,11 +4652,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4838,7 +4664,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -4846,31 +4672,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="23" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="23" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="23" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="23" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="23" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="23" fillId="9" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="9" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="13" fillId="10" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4882,7 +4708,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4926,7 +4752,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4942,7 +4768,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4982,11 +4808,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5014,7 +4840,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5058,11 +4884,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5094,7 +4920,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="4" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5130,302 +4956,302 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="13" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="13" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="13" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="17" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="13" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="13" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="13" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="17" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -5450,7 +5276,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5458,7 +5284,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5490,7 +5316,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5546,7 +5372,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5554,7 +5380,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5650,7 +5476,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5670,7 +5496,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5678,7 +5504,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5698,7 +5524,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5754,7 +5580,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5786,7 +5612,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5794,15 +5620,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5818,7 +5644,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5846,7 +5672,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5858,7 +5684,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="44" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="44" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5870,131 +5696,51 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="45" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="45" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="46" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="47" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="48" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="48" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="46" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="48" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="50" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="50" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="50" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="50" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="50" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="50" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="48" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="51" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="53" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="54" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="47" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8644,9 +8390,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>228240</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>243000</xdr:rowOff>
+      <xdr:rowOff>242640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8660,7 +8406,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4656960"/>
-          <a:ext cx="738720" cy="195480"/>
+          <a:ext cx="738360" cy="195120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8681,9 +8427,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>128520</xdr:colOff>
+      <xdr:colOff>128160</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>243000</xdr:rowOff>
+      <xdr:rowOff>242640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8697,7 +8443,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4971240"/>
-          <a:ext cx="1082160" cy="195480"/>
+          <a:ext cx="1081800" cy="195120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8718,9 +8464,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1800</xdr:colOff>
+      <xdr:colOff>1440</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>243000</xdr:rowOff>
+      <xdr:rowOff>242640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8734,7 +8480,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5285520"/>
-          <a:ext cx="1388880" cy="195480"/>
+          <a:ext cx="1388520" cy="195120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8755,9 +8501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>325800</xdr:colOff>
+      <xdr:colOff>325440</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>243000</xdr:rowOff>
+      <xdr:rowOff>242640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8771,7 +8517,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5599800"/>
-          <a:ext cx="1712880" cy="195480"/>
+          <a:ext cx="1712520" cy="195120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8792,9 +8538,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>199080</xdr:colOff>
+      <xdr:colOff>198720</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>255960</xdr:rowOff>
+      <xdr:rowOff>255600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8808,7 +8554,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5909760"/>
-          <a:ext cx="2019960" cy="208440"/>
+          <a:ext cx="2019600" cy="208080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8829,9 +8575,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>142200</xdr:colOff>
+      <xdr:colOff>141840</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>243000</xdr:rowOff>
+      <xdr:rowOff>242640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8845,7 +8591,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6219720"/>
-          <a:ext cx="2356200" cy="195480"/>
+          <a:ext cx="2355840" cy="195120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8866,9 +8612,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>82440</xdr:colOff>
+      <xdr:colOff>82080</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8878,7 +8624,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6531480"/>
-          <a:ext cx="2669040" cy="194400"/>
+          <a:ext cx="2668680" cy="194040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9247,9 +8993,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>281880</xdr:colOff>
+      <xdr:colOff>281520</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>83160</xdr:rowOff>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9259,7 +9005,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1978200" y="78480"/>
-          <a:ext cx="6968160" cy="10489680"/>
+          <a:ext cx="6967800" cy="10489320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9388,7 +9134,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
@@ -20761,8 +20507,8 @@
   </sheetPr>
   <dimension ref="A1:Q140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21374,1369 +21120,902 @@
       <c r="A36" s="369" t="s">
         <v>650</v>
       </c>
-      <c r="B36" s="398"/>
-      <c r="C36" s="399" t="s">
-        <v>651</v>
-      </c>
-      <c r="D36" s="400"/>
-      <c r="E36" s="400"/>
-      <c r="F36" s="400"/>
-      <c r="G36" s="400"/>
-      <c r="H36" s="400"/>
-      <c r="I36" s="400"/>
-      <c r="J36" s="400"/>
-      <c r="K36" s="400"/>
-      <c r="L36" s="400"/>
-      <c r="M36" s="401"/>
+      <c r="B36" s="360"/>
+      <c r="C36" s="397"/>
+      <c r="D36" s="397"/>
+      <c r="E36" s="397"/>
+      <c r="F36" s="397"/>
+      <c r="G36" s="397"/>
+      <c r="H36" s="397"/>
+      <c r="I36" s="397"/>
+      <c r="J36" s="397"/>
+      <c r="K36" s="397"/>
+      <c r="L36" s="397"/>
+      <c r="M36" s="397"/>
     </row>
     <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="369" t="s">
-        <v>652</v>
-      </c>
-      <c r="B37" s="402"/>
-      <c r="C37" s="403"/>
-      <c r="D37" s="404" t="s">
-        <v>653</v>
-      </c>
-      <c r="E37" s="404"/>
-      <c r="F37" s="404"/>
-      <c r="G37" s="405" t="s">
-        <v>654</v>
-      </c>
-      <c r="H37" s="405"/>
-      <c r="I37" s="405"/>
-      <c r="J37" s="405" t="s">
-        <v>655</v>
-      </c>
-      <c r="K37" s="405"/>
-      <c r="L37" s="405" t="s">
-        <v>656</v>
-      </c>
-      <c r="M37" s="405"/>
+        <v>651</v>
+      </c>
+      <c r="B37" s="360"/>
+      <c r="C37" s="397"/>
+      <c r="D37" s="397"/>
+      <c r="E37" s="397"/>
+      <c r="F37" s="397"/>
+      <c r="G37" s="397"/>
+      <c r="H37" s="397"/>
+      <c r="I37" s="397"/>
+      <c r="J37" s="397"/>
+      <c r="K37" s="397"/>
+      <c r="L37" s="397"/>
+      <c r="M37" s="397"/>
     </row>
     <row r="38" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="369" t="s">
-        <v>657</v>
-      </c>
-      <c r="B38" s="406"/>
-      <c r="C38" s="407" t="s">
-        <v>658</v>
-      </c>
-      <c r="D38" s="408" t="s">
-        <v>659</v>
-      </c>
-      <c r="E38" s="408"/>
-      <c r="F38" s="408"/>
-      <c r="G38" s="409" t="s">
-        <v>659</v>
-      </c>
-      <c r="H38" s="409"/>
-      <c r="I38" s="409"/>
-      <c r="J38" s="409" t="s">
-        <v>659</v>
-      </c>
-      <c r="K38" s="409"/>
-      <c r="L38" s="409" t="s">
-        <v>659</v>
-      </c>
-      <c r="M38" s="409"/>
+        <v>652</v>
+      </c>
+      <c r="B38" s="360"/>
+      <c r="C38" s="397"/>
+      <c r="D38" s="397"/>
+      <c r="E38" s="397"/>
+      <c r="F38" s="397"/>
+      <c r="G38" s="397"/>
+      <c r="H38" s="397"/>
+      <c r="I38" s="397"/>
+      <c r="J38" s="397"/>
+      <c r="K38" s="397"/>
+      <c r="L38" s="397"/>
+      <c r="M38" s="397"/>
     </row>
     <row r="39" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="369" t="s">
-        <v>660</v>
-      </c>
-      <c r="B39" s="410"/>
-      <c r="C39" s="411"/>
-      <c r="D39" s="412" t="s">
-        <v>661</v>
-      </c>
-      <c r="E39" s="413" t="s">
-        <v>298</v>
-      </c>
-      <c r="F39" s="413" t="s">
-        <v>662</v>
-      </c>
-      <c r="G39" s="412" t="s">
-        <v>663</v>
-      </c>
-      <c r="H39" s="412" t="s">
-        <v>664</v>
-      </c>
-      <c r="I39" s="413" t="s">
-        <v>665</v>
-      </c>
-      <c r="J39" s="413" t="s">
-        <v>309</v>
-      </c>
-      <c r="K39" s="413" t="s">
-        <v>310</v>
-      </c>
-      <c r="L39" s="413" t="s">
-        <v>309</v>
-      </c>
-      <c r="M39" s="413" t="s">
-        <v>310</v>
-      </c>
+        <v>653</v>
+      </c>
+      <c r="B39" s="360"/>
+      <c r="C39" s="397"/>
+      <c r="D39" s="397"/>
+      <c r="E39" s="397"/>
+      <c r="F39" s="397"/>
+      <c r="G39" s="397"/>
+      <c r="H39" s="397"/>
+      <c r="I39" s="397"/>
+      <c r="J39" s="397"/>
+      <c r="K39" s="397"/>
+      <c r="L39" s="397"/>
+      <c r="M39" s="397"/>
     </row>
     <row r="40" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="369" t="s">
-        <v>666</v>
-      </c>
-      <c r="B40" s="414"/>
-      <c r="C40" s="415" t="s">
-        <v>667</v>
-      </c>
-      <c r="D40" s="416" t="str">
-        <f aca="false">A11</f>
-        <v>[:tulokset :kuukausierittely 0 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E40" s="416" t="str">
-        <f aca="false">A12</f>
-        <v>[:tulokset :kuukausierittely 0 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F40" s="416" t="str">
-        <f aca="false">A13</f>
-        <v>[:tulokset :kuukausierittely 0 :tuotto :muusahko]</v>
-      </c>
-      <c r="G40" s="416" t="str">
-        <f aca="false">A14</f>
-        <v>[:tulokset :kuukausierittely 0 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H40" s="416" t="str">
-        <f aca="false">A15</f>
-        <v>[:tulokset :kuukausierittely 0 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I40" s="416" t="str">
-        <f aca="false">A16</f>
-        <v>[:tulokset :kuukausierittely 0 :tuotto :muulampo]</v>
-      </c>
-      <c r="J40" s="416" t="str">
-        <f aca="false">A17</f>
-        <v>[:tulokset :kuukausierittely 0 :kulutus :sahko]</v>
-      </c>
-      <c r="K40" s="416" t="str">
-        <f aca="false">A18</f>
-        <v>[:tulokset :kuukausierittely 0 :kulutus :lampo]</v>
-      </c>
-      <c r="L40" s="416" t="str">
-        <f aca="false">A19</f>
-        <v>[:tulokset :kuukausierittely 0 :hyoty :sahko]</v>
-      </c>
-      <c r="M40" s="416" t="str">
-        <f aca="false">A20</f>
-        <v>[:tulokset :kuukausierittely 0 :hyoty :lampo]</v>
-      </c>
+        <v>654</v>
+      </c>
+      <c r="B40" s="360"/>
+      <c r="C40" s="397"/>
+      <c r="D40" s="397"/>
+      <c r="E40" s="397"/>
+      <c r="F40" s="397"/>
+      <c r="G40" s="397"/>
+      <c r="H40" s="397"/>
+      <c r="I40" s="397"/>
+      <c r="J40" s="397"/>
+      <c r="K40" s="397"/>
+      <c r="L40" s="397"/>
+      <c r="M40" s="397"/>
     </row>
     <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="369" t="s">
-        <v>668</v>
-      </c>
-      <c r="B41" s="414"/>
-      <c r="C41" s="415" t="s">
-        <v>669</v>
-      </c>
-      <c r="D41" s="416" t="str">
-        <f aca="false">A21</f>
-        <v>[:tulokset :kuukausierittely 1 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E41" s="416" t="str">
-        <f aca="false">A22</f>
-        <v>[:tulokset :kuukausierittely 1 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F41" s="416" t="str">
-        <f aca="false">A23</f>
-        <v>[:tulokset :kuukausierittely 1 :tuotto :muusahko]</v>
-      </c>
-      <c r="G41" s="416" t="str">
-        <f aca="false">A24</f>
-        <v>[:tulokset :kuukausierittely 1 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H41" s="416" t="str">
-        <f aca="false">A25</f>
-        <v>[:tulokset :kuukausierittely 1 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I41" s="416" t="str">
-        <f aca="false">A26</f>
-        <v>[:tulokset :kuukausierittely 1 :tuotto :muulampo]</v>
-      </c>
-      <c r="J41" s="416" t="str">
-        <f aca="false">A27</f>
-        <v>[:tulokset :kuukausierittely 1 :kulutus :sahko]</v>
-      </c>
-      <c r="K41" s="416" t="str">
-        <f aca="false">A28</f>
-        <v>[:tulokset :kuukausierittely 1 :kulutus :lampo]</v>
-      </c>
-      <c r="L41" s="416" t="str">
-        <f aca="false">A29</f>
-        <v>[:tulokset :kuukausierittely 1 :hyoty :sahko]</v>
-      </c>
-      <c r="M41" s="416" t="str">
-        <f aca="false">A30</f>
-        <v>[:tulokset :kuukausierittely 1 :hyoty :lampo]</v>
-      </c>
+        <v>655</v>
+      </c>
+      <c r="B41" s="360"/>
+      <c r="C41" s="397"/>
+      <c r="D41" s="397"/>
+      <c r="E41" s="397"/>
+      <c r="F41" s="397"/>
+      <c r="G41" s="397"/>
+      <c r="H41" s="397"/>
+      <c r="I41" s="397"/>
+      <c r="J41" s="397"/>
+      <c r="K41" s="397"/>
+      <c r="L41" s="397"/>
+      <c r="M41" s="397"/>
     </row>
     <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="369" t="s">
-        <v>670</v>
-      </c>
-      <c r="B42" s="414"/>
-      <c r="C42" s="415" t="s">
-        <v>671</v>
-      </c>
-      <c r="D42" s="416" t="str">
-        <f aca="false">A31</f>
-        <v>[:tulokset :kuukausierittely 2 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E42" s="416" t="str">
-        <f aca="false">A32</f>
-        <v>[:tulokset :kuukausierittely 2 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F42" s="416" t="str">
-        <f aca="false">A33</f>
-        <v>[:tulokset :kuukausierittely 2 :tuotto :muusahko]</v>
-      </c>
-      <c r="G42" s="416" t="str">
-        <f aca="false">A34</f>
-        <v>[:tulokset :kuukausierittely 2 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H42" s="416" t="str">
-        <f aca="false">A35</f>
-        <v>[:tulokset :kuukausierittely 2 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I42" s="416" t="str">
-        <f aca="false">A36</f>
-        <v>[:tulokset :kuukausierittely 2 :tuotto :muulampo]</v>
-      </c>
-      <c r="J42" s="416" t="str">
-        <f aca="false">A37</f>
-        <v>[:tulokset :kuukausierittely 2 :kulutus :sahko]</v>
-      </c>
-      <c r="K42" s="416" t="str">
-        <f aca="false">A38</f>
-        <v>[:tulokset :kuukausierittely 2 :kulutus :lampo]</v>
-      </c>
-      <c r="L42" s="416" t="str">
-        <f aca="false">A39</f>
-        <v>[:tulokset :kuukausierittely 2 :hyoty :sahko]</v>
-      </c>
-      <c r="M42" s="416" t="str">
-        <f aca="false">A40</f>
-        <v>[:tulokset :kuukausierittely 2 :hyoty :lampo]</v>
-      </c>
+        <v>656</v>
+      </c>
+      <c r="B42" s="360"/>
+      <c r="C42" s="397"/>
+      <c r="D42" s="397"/>
+      <c r="E42" s="397"/>
+      <c r="F42" s="397"/>
+      <c r="G42" s="397"/>
+      <c r="H42" s="397"/>
+      <c r="I42" s="397"/>
+      <c r="J42" s="397"/>
+      <c r="K42" s="397"/>
+      <c r="L42" s="397"/>
+      <c r="M42" s="397"/>
     </row>
     <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="369" t="s">
-        <v>672</v>
-      </c>
-      <c r="B43" s="414"/>
-      <c r="C43" s="415" t="s">
-        <v>673</v>
-      </c>
-      <c r="D43" s="416" t="str">
-        <f aca="false">A41</f>
-        <v>[:tulokset :kuukausierittely 3 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E43" s="416" t="str">
-        <f aca="false">A42</f>
-        <v>[:tulokset :kuukausierittely 3 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F43" s="416" t="str">
-        <f aca="false">A43</f>
-        <v>[:tulokset :kuukausierittely 3 :tuotto :muusahko]</v>
-      </c>
-      <c r="G43" s="416" t="str">
-        <f aca="false">A44</f>
-        <v>[:tulokset :kuukausierittely 3 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H43" s="416" t="str">
-        <f aca="false">A45</f>
-        <v>[:tulokset :kuukausierittely 3 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I43" s="416" t="str">
-        <f aca="false">A46</f>
-        <v>[:tulokset :kuukausierittely 3 :tuotto :muulampo]</v>
-      </c>
-      <c r="J43" s="416" t="str">
-        <f aca="false">A47</f>
-        <v>[:tulokset :kuukausierittely 3 :kulutus :sahko]</v>
-      </c>
-      <c r="K43" s="416" t="str">
-        <f aca="false">A48</f>
-        <v>[:tulokset :kuukausierittely 3 :kulutus :lampo]</v>
-      </c>
-      <c r="L43" s="416" t="str">
-        <f aca="false">A49</f>
-        <v>[:tulokset :kuukausierittely 3 :hyoty :sahko]</v>
-      </c>
-      <c r="M43" s="416" t="str">
-        <f aca="false">A50</f>
-        <v>[:tulokset :kuukausierittely 3 :hyoty :lampo]</v>
-      </c>
+        <v>657</v>
+      </c>
+      <c r="B43" s="360"/>
+      <c r="C43" s="397"/>
+      <c r="D43" s="397"/>
+      <c r="E43" s="397"/>
+      <c r="F43" s="397"/>
+      <c r="G43" s="397"/>
+      <c r="H43" s="397"/>
+      <c r="I43" s="397"/>
+      <c r="J43" s="397"/>
+      <c r="K43" s="397"/>
+      <c r="L43" s="397"/>
+      <c r="M43" s="397"/>
     </row>
     <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="369" t="s">
-        <v>674</v>
-      </c>
-      <c r="B44" s="414"/>
-      <c r="C44" s="415" t="s">
-        <v>675</v>
-      </c>
-      <c r="D44" s="416" t="str">
-        <f aca="false">A51</f>
-        <v>[:tulokset :kuukausierittely 4 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E44" s="416" t="str">
-        <f aca="false">A52</f>
-        <v>[:tulokset :kuukausierittely 4 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F44" s="416" t="str">
-        <f aca="false">A53</f>
-        <v>[:tulokset :kuukausierittely 4 :tuotto :muusahko]</v>
-      </c>
-      <c r="G44" s="416" t="str">
-        <f aca="false">A54</f>
-        <v>[:tulokset :kuukausierittely 4 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H44" s="416" t="str">
-        <f aca="false">A55</f>
-        <v>[:tulokset :kuukausierittely 4 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I44" s="416" t="str">
-        <f aca="false">A56</f>
-        <v>[:tulokset :kuukausierittely 4 :tuotto :muulampo]</v>
-      </c>
-      <c r="J44" s="416" t="str">
-        <f aca="false">A57</f>
-        <v>[:tulokset :kuukausierittely 4 :kulutus :sahko]</v>
-      </c>
-      <c r="K44" s="416" t="str">
-        <f aca="false">A58</f>
-        <v>[:tulokset :kuukausierittely 4 :kulutus :lampo]</v>
-      </c>
-      <c r="L44" s="416" t="str">
-        <f aca="false">A59</f>
-        <v>[:tulokset :kuukausierittely 4 :hyoty :sahko]</v>
-      </c>
-      <c r="M44" s="416" t="str">
-        <f aca="false">A60</f>
-        <v>[:tulokset :kuukausierittely 4 :hyoty :lampo]</v>
-      </c>
+        <v>658</v>
+      </c>
+      <c r="B44" s="360"/>
+      <c r="C44" s="397"/>
+      <c r="D44" s="397"/>
+      <c r="E44" s="397"/>
+      <c r="F44" s="397"/>
+      <c r="G44" s="397"/>
+      <c r="H44" s="397"/>
+      <c r="I44" s="397"/>
+      <c r="J44" s="397"/>
+      <c r="K44" s="397"/>
+      <c r="L44" s="397"/>
+      <c r="M44" s="397"/>
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="369" t="s">
-        <v>676</v>
-      </c>
-      <c r="B45" s="414"/>
-      <c r="C45" s="415" t="s">
-        <v>677</v>
-      </c>
-      <c r="D45" s="416" t="str">
-        <f aca="false">A61</f>
-        <v>[:tulokset :kuukausierittely 5 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E45" s="416" t="str">
-        <f aca="false">A62</f>
-        <v>[:tulokset :kuukausierittely 5 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F45" s="416" t="str">
-        <f aca="false">A63</f>
-        <v>[:tulokset :kuukausierittely 5 :tuotto :muusahko]</v>
-      </c>
-      <c r="G45" s="416" t="str">
-        <f aca="false">A64</f>
-        <v>[:tulokset :kuukausierittely 5 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H45" s="416" t="str">
-        <f aca="false">A65</f>
-        <v>[:tulokset :kuukausierittely 5 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I45" s="416" t="str">
-        <f aca="false">A66</f>
-        <v>[:tulokset :kuukausierittely 5 :tuotto :muulampo]</v>
-      </c>
-      <c r="J45" s="416" t="str">
-        <f aca="false">A67</f>
-        <v>[:tulokset :kuukausierittely 5 :kulutus :sahko]</v>
-      </c>
-      <c r="K45" s="416" t="str">
-        <f aca="false">A68</f>
-        <v>[:tulokset :kuukausierittely 5 :kulutus :lampo]</v>
-      </c>
-      <c r="L45" s="416" t="str">
-        <f aca="false">A69</f>
-        <v>[:tulokset :kuukausierittely 5 :hyoty :sahko]</v>
-      </c>
-      <c r="M45" s="416" t="str">
-        <f aca="false">A70</f>
-        <v>[:tulokset :kuukausierittely 5 :hyoty :lampo]</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="B45" s="360"/>
+      <c r="C45" s="397"/>
+      <c r="D45" s="397"/>
+      <c r="E45" s="397"/>
+      <c r="F45" s="397"/>
+      <c r="G45" s="397"/>
+      <c r="H45" s="397"/>
+      <c r="I45" s="397"/>
+      <c r="J45" s="397"/>
+      <c r="K45" s="397"/>
+      <c r="L45" s="397"/>
+      <c r="M45" s="397"/>
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="369" t="s">
-        <v>678</v>
-      </c>
-      <c r="B46" s="414"/>
-      <c r="C46" s="415" t="s">
-        <v>679</v>
-      </c>
-      <c r="D46" s="416" t="str">
-        <f aca="false">A71</f>
-        <v>[:tulokset :kuukausierittely 6 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E46" s="416" t="str">
-        <f aca="false">A72</f>
-        <v>[:tulokset :kuukausierittely 6 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F46" s="416" t="str">
-        <f aca="false">A73</f>
-        <v>[:tulokset :kuukausierittely 6 :tuotto :muusahko]</v>
-      </c>
-      <c r="G46" s="416" t="str">
-        <f aca="false">A74</f>
-        <v>[:tulokset :kuukausierittely 6 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H46" s="416" t="str">
-        <f aca="false">A75</f>
-        <v>[:tulokset :kuukausierittely 6 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I46" s="416" t="str">
-        <f aca="false">A76</f>
-        <v>[:tulokset :kuukausierittely 6 :tuotto :muulampo]</v>
-      </c>
-      <c r="J46" s="416" t="str">
-        <f aca="false">A77</f>
-        <v>[:tulokset :kuukausierittely 6 :kulutus :sahko]</v>
-      </c>
-      <c r="K46" s="416" t="str">
-        <f aca="false">A78</f>
-        <v>[:tulokset :kuukausierittely 6 :kulutus :lampo]</v>
-      </c>
-      <c r="L46" s="416" t="str">
-        <f aca="false">A79</f>
-        <v>[:tulokset :kuukausierittely 6 :hyoty :sahko]</v>
-      </c>
-      <c r="M46" s="416" t="str">
-        <f aca="false">A80</f>
-        <v>[:tulokset :kuukausierittely 6 :hyoty :lampo]</v>
-      </c>
+        <v>660</v>
+      </c>
+      <c r="B46" s="360"/>
+      <c r="C46" s="397"/>
+      <c r="D46" s="397"/>
+      <c r="E46" s="397"/>
+      <c r="F46" s="397"/>
+      <c r="G46" s="397"/>
+      <c r="H46" s="397"/>
+      <c r="I46" s="397"/>
+      <c r="J46" s="397"/>
+      <c r="K46" s="397"/>
+      <c r="L46" s="397"/>
+      <c r="M46" s="397"/>
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="369" t="s">
-        <v>680</v>
-      </c>
-      <c r="B47" s="414"/>
-      <c r="C47" s="415" t="s">
-        <v>681</v>
-      </c>
-      <c r="D47" s="416" t="str">
-        <f aca="false">A81</f>
-        <v>[:tulokset :kuukausierittely 7 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E47" s="416" t="str">
-        <f aca="false">A82</f>
-        <v>[:tulokset :kuukausierittely 7 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F47" s="416" t="str">
-        <f aca="false">A83</f>
-        <v>[:tulokset :kuukausierittely 7 :tuotto :muusahko]</v>
-      </c>
-      <c r="G47" s="416" t="str">
-        <f aca="false">A84</f>
-        <v>[:tulokset :kuukausierittely 7 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H47" s="416" t="str">
-        <f aca="false">A85</f>
-        <v>[:tulokset :kuukausierittely 7 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I47" s="416" t="str">
-        <f aca="false">A86</f>
-        <v>[:tulokset :kuukausierittely 7 :tuotto :muulampo]</v>
-      </c>
-      <c r="J47" s="416" t="str">
-        <f aca="false">A87</f>
-        <v>[:tulokset :kuukausierittely 7 :kulutus :sahko]</v>
-      </c>
-      <c r="K47" s="416" t="str">
-        <f aca="false">A88</f>
-        <v>[:tulokset :kuukausierittely 7 :kulutus :lampo]</v>
-      </c>
-      <c r="L47" s="416" t="str">
-        <f aca="false">A89</f>
-        <v>[:tulokset :kuukausierittely 7 :hyoty :sahko]</v>
-      </c>
-      <c r="M47" s="416" t="str">
-        <f aca="false">A90</f>
-        <v>[:tulokset :kuukausierittely 7 :hyoty :lampo]</v>
-      </c>
+        <v>661</v>
+      </c>
+      <c r="B47" s="360"/>
+      <c r="C47" s="397"/>
+      <c r="D47" s="397"/>
+      <c r="E47" s="397"/>
+      <c r="F47" s="397"/>
+      <c r="G47" s="397"/>
+      <c r="H47" s="397"/>
+      <c r="I47" s="397"/>
+      <c r="J47" s="397"/>
+      <c r="K47" s="397"/>
+      <c r="L47" s="397"/>
+      <c r="M47" s="397"/>
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="369" t="s">
-        <v>682</v>
-      </c>
-      <c r="B48" s="414"/>
-      <c r="C48" s="415" t="s">
-        <v>683</v>
-      </c>
-      <c r="D48" s="416" t="str">
-        <f aca="false">A91</f>
-        <v>[:tulokset :kuukausierittely 8 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E48" s="416" t="str">
-        <f aca="false">A92</f>
-        <v>[:tulokset :kuukausierittely 8 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F48" s="416" t="str">
-        <f aca="false">A93</f>
-        <v>[:tulokset :kuukausierittely 8 :tuotto :muusahko]</v>
-      </c>
-      <c r="G48" s="416" t="str">
-        <f aca="false">A94</f>
-        <v>[:tulokset :kuukausierittely 8 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H48" s="416" t="str">
-        <f aca="false">A95</f>
-        <v>[:tulokset :kuukausierittely 8 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I48" s="416" t="str">
-        <f aca="false">A96</f>
-        <v>[:tulokset :kuukausierittely 8 :tuotto :muulampo]</v>
-      </c>
-      <c r="J48" s="416" t="str">
-        <f aca="false">A97</f>
-        <v>[:tulokset :kuukausierittely 8 :kulutus :sahko]</v>
-      </c>
-      <c r="K48" s="416" t="str">
-        <f aca="false">A98</f>
-        <v>[:tulokset :kuukausierittely 8 :kulutus :lampo]</v>
-      </c>
-      <c r="L48" s="416" t="str">
-        <f aca="false">A99</f>
-        <v>[:tulokset :kuukausierittely 8 :hyoty :sahko]</v>
-      </c>
-      <c r="M48" s="416" t="str">
-        <f aca="false">A100</f>
-        <v>[:tulokset :kuukausierittely 8 :hyoty :lampo]</v>
-      </c>
+        <v>662</v>
+      </c>
+      <c r="B48" s="360"/>
+      <c r="C48" s="397"/>
+      <c r="D48" s="397"/>
+      <c r="E48" s="397"/>
+      <c r="F48" s="397"/>
+      <c r="G48" s="397"/>
+      <c r="H48" s="397"/>
+      <c r="I48" s="397"/>
+      <c r="J48" s="397"/>
+      <c r="K48" s="397"/>
+      <c r="L48" s="397"/>
+      <c r="M48" s="397"/>
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="369" t="s">
-        <v>684</v>
-      </c>
-      <c r="B49" s="414"/>
-      <c r="C49" s="415" t="s">
-        <v>685</v>
-      </c>
-      <c r="D49" s="416" t="str">
-        <f aca="false">A101</f>
-        <v>[:tulokset :kuukausierittely 9 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E49" s="416" t="str">
-        <f aca="false">A102</f>
-        <v>[:tulokset :kuukausierittely 9 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F49" s="416" t="str">
-        <f aca="false">A103</f>
-        <v>[:tulokset :kuukausierittely 9 :tuotto :muusahko]</v>
-      </c>
-      <c r="G49" s="416" t="str">
-        <f aca="false">A104</f>
-        <v>[:tulokset :kuukausierittely 9 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H49" s="416" t="str">
-        <f aca="false">A105</f>
-        <v>[:tulokset :kuukausierittely 9 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I49" s="416" t="str">
-        <f aca="false">A106</f>
-        <v>[:tulokset :kuukausierittely 9 :tuotto :muulampo]</v>
-      </c>
-      <c r="J49" s="416" t="str">
-        <f aca="false">A107</f>
-        <v>[:tulokset :kuukausierittely 9 :kulutus :sahko]</v>
-      </c>
-      <c r="K49" s="416" t="str">
-        <f aca="false">A108</f>
-        <v>[:tulokset :kuukausierittely 9 :kulutus :lampo]</v>
-      </c>
-      <c r="L49" s="416" t="str">
-        <f aca="false">A109</f>
-        <v>[:tulokset :kuukausierittely 9 :hyoty :sahko]</v>
-      </c>
-      <c r="M49" s="416" t="str">
-        <f aca="false">A110</f>
-        <v>[:tulokset :kuukausierittely 9 :hyoty :lampo]</v>
-      </c>
+        <v>663</v>
+      </c>
+      <c r="B49" s="360"/>
+      <c r="C49" s="397"/>
+      <c r="D49" s="397"/>
+      <c r="E49" s="397"/>
+      <c r="F49" s="397"/>
+      <c r="G49" s="397"/>
+      <c r="H49" s="397"/>
+      <c r="I49" s="397"/>
+      <c r="J49" s="397"/>
+      <c r="K49" s="397"/>
+      <c r="L49" s="397"/>
+      <c r="M49" s="397"/>
     </row>
     <row r="50" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="369" t="s">
-        <v>686</v>
-      </c>
-      <c r="B50" s="414"/>
-      <c r="C50" s="415" t="s">
-        <v>687</v>
-      </c>
-      <c r="D50" s="416" t="str">
-        <f aca="false">A111</f>
-        <v>[:tulokset :kuukausierittely 10 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E50" s="416" t="str">
-        <f aca="false">A112</f>
-        <v>[:tulokset :kuukausierittely 10 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F50" s="416" t="str">
-        <f aca="false">A113</f>
-        <v>[:tulokset :kuukausierittely 10 :tuotto :muusahko]</v>
-      </c>
-      <c r="G50" s="416" t="str">
-        <f aca="false">A114</f>
-        <v>[:tulokset :kuukausierittely 10 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H50" s="416" t="str">
-        <f aca="false">A115</f>
-        <v>[:tulokset :kuukausierittely 10 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I50" s="416" t="str">
-        <f aca="false">A116</f>
-        <v>[:tulokset :kuukausierittely 10 :tuotto :muulampo]</v>
-      </c>
-      <c r="J50" s="416" t="str">
-        <f aca="false">A117</f>
-        <v>[:tulokset :kuukausierittely 10 :kulutus :sahko]</v>
-      </c>
-      <c r="K50" s="416" t="str">
-        <f aca="false">A118</f>
-        <v>[:tulokset :kuukausierittely 10 :kulutus :lampo]</v>
-      </c>
-      <c r="L50" s="416" t="str">
-        <f aca="false">A119</f>
-        <v>[:tulokset :kuukausierittely 10 :hyoty :sahko]</v>
-      </c>
-      <c r="M50" s="416" t="str">
-        <f aca="false">A120</f>
-        <v>[:tulokset :kuukausierittely 10 :hyoty :lampo]</v>
-      </c>
+        <v>664</v>
+      </c>
+      <c r="B50" s="360"/>
+      <c r="C50" s="397"/>
+      <c r="D50" s="397"/>
+      <c r="E50" s="397"/>
+      <c r="F50" s="397"/>
+      <c r="G50" s="397"/>
+      <c r="H50" s="397"/>
+      <c r="I50" s="397"/>
+      <c r="J50" s="397"/>
+      <c r="K50" s="397"/>
+      <c r="L50" s="397"/>
+      <c r="M50" s="397"/>
     </row>
     <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="369" t="s">
-        <v>688</v>
-      </c>
-      <c r="B51" s="414"/>
-      <c r="C51" s="415" t="s">
-        <v>689</v>
-      </c>
-      <c r="D51" s="416" t="str">
-        <f aca="false">A121</f>
-        <v>[:tulokset :kuukausierittely 11 :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E51" s="416" t="str">
-        <f aca="false">A122</f>
-        <v>[:tulokset :kuukausierittely 11 :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F51" s="416" t="str">
-        <f aca="false">A123</f>
-        <v>[:tulokset :kuukausierittely 11 :tuotto :muusahko]</v>
-      </c>
-      <c r="G51" s="416" t="str">
-        <f aca="false">A124</f>
-        <v>[:tulokset :kuukausierittely 11 :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H51" s="416" t="str">
-        <f aca="false">A125</f>
-        <v>[:tulokset :kuukausierittely 11 :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I51" s="416" t="str">
-        <f aca="false">A126</f>
-        <v>[:tulokset :kuukausierittely 11 :tuotto :muulampo]</v>
-      </c>
-      <c r="J51" s="416" t="str">
-        <f aca="false">A127</f>
-        <v>[:tulokset :kuukausierittely 11 :kulutus :sahko]</v>
-      </c>
-      <c r="K51" s="416" t="str">
-        <f aca="false">A128</f>
-        <v>[:tulokset :kuukausierittely 11 :kulutus :lampo]</v>
-      </c>
-      <c r="L51" s="416" t="str">
-        <f aca="false">A129</f>
-        <v>[:tulokset :kuukausierittely 11 :hyoty :sahko]</v>
-      </c>
-      <c r="M51" s="416" t="str">
-        <f aca="false">A130</f>
-        <v>[:tulokset :kuukausierittely 11 :hyoty :lampo]</v>
-      </c>
+        <v>665</v>
+      </c>
+      <c r="B51" s="360"/>
+      <c r="C51" s="397"/>
+      <c r="D51" s="397"/>
+      <c r="E51" s="397"/>
+      <c r="F51" s="397"/>
+      <c r="G51" s="397"/>
+      <c r="H51" s="397"/>
+      <c r="I51" s="397"/>
+      <c r="J51" s="397"/>
+      <c r="K51" s="397"/>
+      <c r="L51" s="397"/>
+      <c r="M51" s="397"/>
     </row>
     <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="369" t="s">
-        <v>690</v>
-      </c>
-      <c r="B52" s="414"/>
-      <c r="C52" s="417" t="s">
-        <v>691</v>
-      </c>
-      <c r="D52" s="418" t="str">
-        <f aca="false">A131</f>
-        <v>[:tulokset :kuukausierittely-summat :tuotto :aurinkosahko]</v>
-      </c>
-      <c r="E52" s="418" t="str">
-        <f aca="false">A132</f>
-        <v>[:tulokset :kuukausierittely-summat :tuotto :tuulisahko]</v>
-      </c>
-      <c r="F52" s="418" t="str">
-        <f aca="false">A133</f>
-        <v>[:tulokset :kuukausierittely-summat :tuotto :muulampo]</v>
-      </c>
-      <c r="G52" s="418" t="str">
-        <f aca="false">A134</f>
-        <v>[:tulokset :kuukausierittely-summat :tuotto :aurinkolampo]</v>
-      </c>
-      <c r="H52" s="418" t="str">
-        <f aca="false">A135</f>
-        <v>[:tulokset :kuukausierittely-summat :tuotto :lampopumppu]</v>
-      </c>
-      <c r="I52" s="418" t="str">
-        <f aca="false">A136</f>
-        <v>[:tulokset :kuukausierittely-summat :tuotto :muulampo]</v>
-      </c>
-      <c r="J52" s="418" t="str">
-        <f aca="false">A137</f>
-        <v>[:tulokset :kuukausierittely-summat :kulutus :sahko]</v>
-      </c>
-      <c r="K52" s="418" t="str">
-        <f aca="false">A138</f>
-        <v>[:tulokset :kuukausierittely-summat :kulutus :lampo]</v>
-      </c>
-      <c r="L52" s="418" t="str">
-        <f aca="false">A139</f>
-        <v>[:tulokset :kuukausierittely-summat :hyoty :sahko]</v>
-      </c>
-      <c r="M52" s="418" t="str">
-        <f aca="false">A140</f>
-        <v>[:tulokset :kuukausierittely-summat :hyoty :lampo]</v>
-      </c>
+        <v>666</v>
+      </c>
+      <c r="B52" s="360"/>
+      <c r="C52" s="397"/>
+      <c r="D52" s="397"/>
+      <c r="E52" s="397"/>
+      <c r="F52" s="397"/>
+      <c r="G52" s="397"/>
+      <c r="H52" s="397"/>
+      <c r="I52" s="397"/>
+      <c r="J52" s="397"/>
+      <c r="K52" s="397"/>
+      <c r="L52" s="397"/>
+      <c r="M52" s="397"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="369" t="s">
-        <v>692</v>
-      </c>
-      <c r="B53" s="402"/>
-      <c r="C53" s="419" t="s">
-        <v>693</v>
-      </c>
-      <c r="D53" s="419"/>
-      <c r="E53" s="419"/>
-      <c r="F53" s="419"/>
-      <c r="G53" s="419"/>
-      <c r="H53" s="419"/>
-      <c r="I53" s="419"/>
-      <c r="J53" s="419"/>
-      <c r="K53" s="419"/>
-      <c r="L53" s="419"/>
-      <c r="M53" s="419"/>
+        <v>667</v>
+      </c>
+      <c r="B53" s="360"/>
+      <c r="C53" s="397"/>
+      <c r="D53" s="397"/>
+      <c r="E53" s="397"/>
+      <c r="F53" s="397"/>
+      <c r="G53" s="397"/>
+      <c r="H53" s="397"/>
+      <c r="I53" s="397"/>
+      <c r="J53" s="397"/>
+      <c r="K53" s="397"/>
+      <c r="L53" s="397"/>
+      <c r="M53" s="397"/>
     </row>
     <row r="54" customFormat="false" ht="7.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="369" t="s">
-        <v>694</v>
-      </c>
-      <c r="B54" s="402"/>
-      <c r="C54" s="420"/>
-      <c r="D54" s="420"/>
-      <c r="E54" s="420"/>
-      <c r="F54" s="420"/>
-      <c r="G54" s="420"/>
-      <c r="H54" s="420"/>
-      <c r="I54" s="420"/>
-      <c r="J54" s="420"/>
-      <c r="K54" s="420"/>
-      <c r="L54" s="420"/>
-      <c r="M54" s="403"/>
+        <v>668</v>
+      </c>
+      <c r="B54" s="360"/>
+      <c r="C54" s="398"/>
+      <c r="D54" s="398"/>
+      <c r="E54" s="398"/>
+      <c r="F54" s="398"/>
+      <c r="G54" s="398"/>
+      <c r="H54" s="398"/>
+      <c r="I54" s="398"/>
+      <c r="J54" s="398"/>
+      <c r="K54" s="398"/>
+      <c r="L54" s="398"/>
+      <c r="M54" s="399"/>
     </row>
     <row r="55" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="369" t="s">
-        <v>695</v>
-      </c>
-      <c r="B55" s="421"/>
-      <c r="C55" s="422" t="s">
-        <v>696</v>
-      </c>
-      <c r="D55" s="422"/>
-      <c r="E55" s="422"/>
-      <c r="F55" s="422"/>
-      <c r="G55" s="422"/>
-      <c r="H55" s="422"/>
-      <c r="I55" s="422"/>
-      <c r="J55" s="422"/>
-      <c r="K55" s="422"/>
-      <c r="L55" s="422"/>
-      <c r="M55" s="422"/>
+        <v>669</v>
+      </c>
+      <c r="B55" s="400"/>
+      <c r="C55" s="401" t="s">
+        <v>670</v>
+      </c>
+      <c r="D55" s="401"/>
+      <c r="E55" s="401"/>
+      <c r="F55" s="401"/>
+      <c r="G55" s="401"/>
+      <c r="H55" s="401"/>
+      <c r="I55" s="401"/>
+      <c r="J55" s="401"/>
+      <c r="K55" s="401"/>
+      <c r="L55" s="401"/>
+      <c r="M55" s="401"/>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="369" t="s">
-        <v>697</v>
-      </c>
-      <c r="B56" s="423"/>
-      <c r="C56" s="424" t="s">
-        <v>698</v>
-      </c>
-      <c r="D56" s="424"/>
-      <c r="E56" s="424"/>
-      <c r="F56" s="424"/>
-      <c r="G56" s="424"/>
-      <c r="H56" s="424"/>
-      <c r="I56" s="424"/>
-      <c r="J56" s="424"/>
-      <c r="K56" s="424"/>
-      <c r="L56" s="424"/>
-      <c r="M56" s="425" t="str">
+        <v>671</v>
+      </c>
+      <c r="B56" s="402"/>
+      <c r="C56" s="403" t="s">
+        <v>672</v>
+      </c>
+      <c r="D56" s="403"/>
+      <c r="E56" s="403"/>
+      <c r="F56" s="403"/>
+      <c r="G56" s="403"/>
+      <c r="H56" s="403"/>
+      <c r="I56" s="403"/>
+      <c r="J56" s="403"/>
+      <c r="K56" s="403"/>
+      <c r="L56" s="403"/>
+      <c r="M56" s="404" t="str">
         <f aca="false">A4</f>
         <v>[:lahtotiedot :rakennusvaippa :lampokapasiteetti]</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="369" t="s">
-        <v>699</v>
-      </c>
-      <c r="B57" s="423"/>
-      <c r="C57" s="424" t="s">
-        <v>700</v>
-      </c>
-      <c r="D57" s="424"/>
-      <c r="E57" s="424"/>
-      <c r="F57" s="424"/>
-      <c r="G57" s="424"/>
-      <c r="H57" s="424"/>
-      <c r="I57" s="424"/>
-      <c r="J57" s="424"/>
-      <c r="K57" s="424"/>
-      <c r="L57" s="424"/>
-      <c r="M57" s="425" t="str">
+        <v>673</v>
+      </c>
+      <c r="B57" s="402"/>
+      <c r="C57" s="403" t="s">
+        <v>674</v>
+      </c>
+      <c r="D57" s="403"/>
+      <c r="E57" s="403"/>
+      <c r="F57" s="403"/>
+      <c r="G57" s="403"/>
+      <c r="H57" s="403"/>
+      <c r="I57" s="403"/>
+      <c r="J57" s="403"/>
+      <c r="K57" s="403"/>
+      <c r="L57" s="403"/>
+      <c r="M57" s="404" t="str">
         <f aca="false">A5</f>
         <v>[:lahtotiedot :rakennusvaippa :ilmatilavuus]</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="369" t="s">
-        <v>701</v>
-      </c>
-      <c r="B58" s="423"/>
-      <c r="C58" s="424" t="s">
-        <v>702</v>
-      </c>
-      <c r="D58" s="424"/>
-      <c r="E58" s="424"/>
-      <c r="F58" s="424"/>
-      <c r="G58" s="424"/>
-      <c r="H58" s="424"/>
-      <c r="I58" s="424"/>
-      <c r="J58" s="424"/>
-      <c r="K58" s="424"/>
-      <c r="L58" s="424"/>
-      <c r="M58" s="425" t="str">
+        <v>675</v>
+      </c>
+      <c r="B58" s="402"/>
+      <c r="C58" s="403" t="s">
+        <v>676</v>
+      </c>
+      <c r="D58" s="403"/>
+      <c r="E58" s="403"/>
+      <c r="F58" s="403"/>
+      <c r="G58" s="403"/>
+      <c r="H58" s="403"/>
+      <c r="I58" s="403"/>
+      <c r="J58" s="403"/>
+      <c r="K58" s="403"/>
+      <c r="L58" s="403"/>
+      <c r="M58" s="404" t="str">
         <f aca="false">A6</f>
         <v>[:lahtotiedot :ilmanvaihto :tuloilma-lampotila]</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="369" t="s">
-        <v>703</v>
-      </c>
-      <c r="B59" s="423"/>
-      <c r="C59" s="424" t="s">
-        <v>704</v>
-      </c>
-      <c r="D59" s="424"/>
-      <c r="E59" s="424"/>
-      <c r="F59" s="424"/>
-      <c r="G59" s="424"/>
-      <c r="H59" s="424"/>
-      <c r="I59" s="424"/>
-      <c r="J59" s="424"/>
-      <c r="K59" s="424"/>
-      <c r="L59" s="424"/>
-      <c r="M59" s="425" t="str">
+        <v>677</v>
+      </c>
+      <c r="B59" s="402"/>
+      <c r="C59" s="403" t="s">
+        <v>678</v>
+      </c>
+      <c r="D59" s="403"/>
+      <c r="E59" s="403"/>
+      <c r="F59" s="403"/>
+      <c r="G59" s="403"/>
+      <c r="H59" s="403"/>
+      <c r="I59" s="403"/>
+      <c r="J59" s="403"/>
+      <c r="K59" s="403"/>
+      <c r="L59" s="403"/>
+      <c r="M59" s="404" t="str">
         <f aca="false">A7</f>
         <v>[:lahtotiedot :lammitys :tilat-ja-iv :lampopumppu-tuotto-osuus]</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="369" t="s">
-        <v>705</v>
-      </c>
-      <c r="B60" s="423"/>
-      <c r="C60" s="424" t="s">
-        <v>706</v>
-      </c>
-      <c r="D60" s="424"/>
-      <c r="E60" s="424"/>
-      <c r="F60" s="424"/>
-      <c r="G60" s="424"/>
-      <c r="H60" s="424"/>
-      <c r="I60" s="424"/>
-      <c r="J60" s="424"/>
-      <c r="K60" s="424"/>
-      <c r="L60" s="424"/>
-      <c r="M60" s="425" t="str">
+        <v>679</v>
+      </c>
+      <c r="B60" s="402"/>
+      <c r="C60" s="403" t="s">
+        <v>680</v>
+      </c>
+      <c r="D60" s="403"/>
+      <c r="E60" s="403"/>
+      <c r="F60" s="403"/>
+      <c r="G60" s="403"/>
+      <c r="H60" s="403"/>
+      <c r="I60" s="403"/>
+      <c r="J60" s="403"/>
+      <c r="K60" s="403"/>
+      <c r="L60" s="403"/>
+      <c r="M60" s="404" t="str">
         <f aca="false">A8</f>
         <v>[:lahtotiedot :lammitys :lammin-kayttovesi :lampopumppu-tuotto-osuus]</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="369" t="s">
-        <v>707</v>
-      </c>
-      <c r="B61" s="406"/>
-      <c r="C61" s="426" t="s">
-        <v>708</v>
-      </c>
-      <c r="D61" s="426"/>
-      <c r="E61" s="426"/>
-      <c r="F61" s="426"/>
-      <c r="G61" s="426"/>
-      <c r="H61" s="426"/>
-      <c r="I61" s="426"/>
-      <c r="J61" s="426"/>
-      <c r="K61" s="426"/>
-      <c r="L61" s="426"/>
-      <c r="M61" s="427" t="str">
+        <v>681</v>
+      </c>
+      <c r="B61" s="405"/>
+      <c r="C61" s="406" t="s">
+        <v>682</v>
+      </c>
+      <c r="D61" s="406"/>
+      <c r="E61" s="406"/>
+      <c r="F61" s="406"/>
+      <c r="G61" s="406"/>
+      <c r="H61" s="406"/>
+      <c r="I61" s="406"/>
+      <c r="J61" s="406"/>
+      <c r="K61" s="406"/>
+      <c r="L61" s="406"/>
+      <c r="M61" s="407" t="str">
         <f aca="false">A9</f>
         <v>[:lahtotiedot :lammitys :tilat-ja-iv :lampohavio-lammittamaton-tila]</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="369" t="s">
-        <v>709</v>
-      </c>
-      <c r="B62" s="428" t="str">
+        <v>683</v>
+      </c>
+      <c r="B62" s="408" t="str">
         <f aca="false">"Todistustunnus: "&amp;A1&amp;", 8/8"</f>
         <v>Todistustunnus: [:id], 8/8</v>
       </c>
-      <c r="C62" s="428"/>
-      <c r="D62" s="428"/>
-      <c r="E62" s="428"/>
-      <c r="F62" s="428"/>
-      <c r="G62" s="428"/>
-      <c r="H62" s="428"/>
-      <c r="I62" s="428"/>
-      <c r="J62" s="428"/>
-      <c r="K62" s="428"/>
-      <c r="L62" s="428"/>
-      <c r="M62" s="428"/>
+      <c r="C62" s="408"/>
+      <c r="D62" s="408"/>
+      <c r="E62" s="408"/>
+      <c r="F62" s="408"/>
+      <c r="G62" s="408"/>
+      <c r="H62" s="408"/>
+      <c r="I62" s="408"/>
+      <c r="J62" s="408"/>
+      <c r="K62" s="408"/>
+      <c r="L62" s="408"/>
+      <c r="M62" s="408"/>
     </row>
     <row r="63" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="369" t="s">
-        <v>710</v>
-      </c>
-      <c r="B63" s="428"/>
-      <c r="C63" s="428"/>
-      <c r="D63" s="428"/>
-      <c r="E63" s="428"/>
-      <c r="F63" s="428"/>
-      <c r="G63" s="428"/>
-      <c r="H63" s="428"/>
-      <c r="I63" s="428"/>
-      <c r="J63" s="428"/>
-      <c r="K63" s="428"/>
-      <c r="L63" s="428"/>
-      <c r="M63" s="428"/>
+        <v>684</v>
+      </c>
+      <c r="B63" s="408"/>
+      <c r="C63" s="408"/>
+      <c r="D63" s="408"/>
+      <c r="E63" s="408"/>
+      <c r="F63" s="408"/>
+      <c r="G63" s="408"/>
+      <c r="H63" s="408"/>
+      <c r="I63" s="408"/>
+      <c r="J63" s="408"/>
+      <c r="K63" s="408"/>
+      <c r="L63" s="408"/>
+      <c r="M63" s="408"/>
     </row>
     <row r="64" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="369" t="s">
-        <v>711</v>
+        <v>685</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="369" t="s">
-        <v>712</v>
+        <v>686</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="369" t="s">
-        <v>713</v>
+        <v>687</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="369" t="s">
-        <v>714</v>
+        <v>688</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="369" t="s">
-        <v>715</v>
+        <v>689</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="369" t="s">
-        <v>716</v>
+        <v>690</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="369" t="s">
-        <v>717</v>
+        <v>691</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="369" t="s">
-        <v>718</v>
+        <v>692</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="369" t="s">
-        <v>719</v>
+        <v>693</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="369" t="s">
-        <v>720</v>
+        <v>694</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="369" t="s">
-        <v>721</v>
+        <v>695</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="369" t="s">
-        <v>722</v>
+        <v>696</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="369" t="s">
-        <v>723</v>
+        <v>697</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="369" t="s">
-        <v>724</v>
+        <v>698</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="369" t="s">
-        <v>725</v>
+        <v>699</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="369" t="s">
-        <v>726</v>
+        <v>700</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="369" t="s">
-        <v>727</v>
+        <v>701</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="369" t="s">
-        <v>728</v>
+        <v>702</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="369" t="s">
-        <v>729</v>
+        <v>703</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="369" t="s">
-        <v>730</v>
+        <v>704</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="369" t="s">
-        <v>731</v>
+        <v>705</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="369" t="s">
-        <v>732</v>
+        <v>706</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="369" t="s">
-        <v>733</v>
+        <v>707</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="369" t="s">
-        <v>734</v>
+        <v>708</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="369" t="s">
-        <v>735</v>
+        <v>709</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="369" t="s">
-        <v>736</v>
+        <v>710</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="369" t="s">
-        <v>737</v>
+        <v>711</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="369" t="s">
-        <v>738</v>
+        <v>712</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="369" t="s">
-        <v>739</v>
+        <v>713</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="369" t="s">
-        <v>740</v>
+        <v>714</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="369" t="s">
-        <v>741</v>
+        <v>715</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="369" t="s">
-        <v>742</v>
+        <v>716</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="369" t="s">
-        <v>743</v>
+        <v>717</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="369" t="s">
-        <v>744</v>
+        <v>718</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="369" t="s">
-        <v>745</v>
+        <v>719</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="369" t="s">
-        <v>746</v>
+        <v>720</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="369" t="s">
-        <v>747</v>
+        <v>721</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="369" t="s">
-        <v>748</v>
+        <v>722</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="369" t="s">
-        <v>749</v>
+        <v>723</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="369" t="s">
-        <v>750</v>
+        <v>724</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="369" t="s">
-        <v>751</v>
+        <v>725</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="369" t="s">
-        <v>752</v>
+        <v>726</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="369" t="s">
-        <v>753</v>
+        <v>727</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="369" t="s">
-        <v>754</v>
+        <v>728</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="369" t="s">
-        <v>755</v>
+        <v>729</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="369" t="s">
-        <v>756</v>
+        <v>730</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="369" t="s">
-        <v>757</v>
+        <v>731</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="369" t="s">
-        <v>758</v>
+        <v>732</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="369" t="s">
-        <v>759</v>
+        <v>733</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="369" t="s">
-        <v>760</v>
+        <v>734</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="369" t="s">
-        <v>761</v>
+        <v>735</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="369" t="s">
-        <v>762</v>
+        <v>736</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="369" t="s">
-        <v>763</v>
+        <v>737</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="369" t="s">
-        <v>764</v>
+        <v>738</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="369" t="s">
-        <v>765</v>
+        <v>739</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="369" t="s">
-        <v>766</v>
+        <v>740</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="369" t="s">
-        <v>767</v>
+        <v>741</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="369" t="s">
-        <v>768</v>
+        <v>742</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="369" t="s">
-        <v>769</v>
+        <v>743</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="369" t="s">
-        <v>770</v>
+        <v>744</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="369" t="s">
-        <v>771</v>
+        <v>745</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="369" t="s">
-        <v>772</v>
+        <v>746</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="369" t="s">
-        <v>773</v>
+        <v>747</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="369" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="369" t="s">
-        <v>775</v>
+        <v>749</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="369" t="s">
-        <v>776</v>
+        <v>750</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="369" t="s">
-        <v>777</v>
+        <v>751</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="369" t="s">
-        <v>778</v>
+        <v>752</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="369" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="369" t="s">
-        <v>780</v>
+        <v>754</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="369" t="s">
-        <v>781</v>
+        <v>755</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="369" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="369" t="s">
-        <v>780</v>
+        <v>754</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="369" t="s">
-        <v>783</v>
+        <v>757</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="369" t="s">
-        <v>784</v>
+        <v>758</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="369" t="s">
-        <v>785</v>
+        <v>759</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="369" t="s">
-        <v>786</v>
+        <v>760</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="10">
     <mergeCell ref="C2:M2"/>
-    <mergeCell ref="C3:M35"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="C53:M53"/>
+    <mergeCell ref="C3:M53"/>
     <mergeCell ref="C55:M55"/>
     <mergeCell ref="C56:L56"/>
     <mergeCell ref="C57:L57"/>
@@ -22746,7 +22025,7 @@
     <mergeCell ref="C61:L61"/>
     <mergeCell ref="B62:M63"/>
   </mergeCells>
-  <conditionalFormatting sqref="B62:AMJ1048576 B2:C2 N2:AMJ61 B55:M55 D40:M51 B38:B39 B36 A3:A1048576 B56:I61 K56:K61 M56:M61">
+  <conditionalFormatting sqref="B62:AMJ1048576 B2:C2 N2:AMJ61 B55:M55 A3:A1048576 B56:I61 K56:K61 M56:M61">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="356">
       <formula>"*"</formula>
     </cfRule>

</xml_diff>

<commit_message>
AE-505 Reorder energy sources on ET page 4
ET 2018
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,23 +19,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'1) etusivu'!$B$1:$R$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$M$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$B$1:$R$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$66</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$L$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$N$62</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0" vbProcedure="false">'8) lisämerkintöjä'!$B$1:$M$63</definedName>
   </definedNames>
@@ -5198,11 +5198,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -7011,13 +7011,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
@@ -7155,13 +7148,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
@@ -7252,6 +7238,20 @@
       <font>
         <color rgb="FFFF0000"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -8388,9 +8388,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>227160</xdr:colOff>
+      <xdr:colOff>226800</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>241560</xdr:rowOff>
+      <xdr:rowOff>241200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8404,12 +8404,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4656960"/>
-          <a:ext cx="737280" cy="194040"/>
+          <a:ext cx="736920" cy="193680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8425,9 +8425,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>127080</xdr:colOff>
+      <xdr:colOff>126720</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>241560</xdr:rowOff>
+      <xdr:rowOff>241200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8441,12 +8441,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4971240"/>
-          <a:ext cx="1080720" cy="194040"/>
+          <a:ext cx="1080360" cy="193680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8462,9 +8462,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>433800</xdr:colOff>
+      <xdr:colOff>433440</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>241560</xdr:rowOff>
+      <xdr:rowOff>241200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8478,12 +8478,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5285520"/>
-          <a:ext cx="1387440" cy="194040"/>
+          <a:ext cx="1387080" cy="193680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8499,9 +8499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>324360</xdr:colOff>
+      <xdr:colOff>324000</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>241560</xdr:rowOff>
+      <xdr:rowOff>241200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8515,12 +8515,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5599800"/>
-          <a:ext cx="1711440" cy="194040"/>
+          <a:ext cx="1711080" cy="193680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8536,9 +8536,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>197640</xdr:colOff>
+      <xdr:colOff>197280</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>254520</xdr:rowOff>
+      <xdr:rowOff>254160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8552,12 +8552,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5909760"/>
-          <a:ext cx="2018520" cy="207000"/>
+          <a:ext cx="2018160" cy="206640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8573,9 +8573,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>140760</xdr:colOff>
+      <xdr:colOff>140400</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>241560</xdr:rowOff>
+      <xdr:rowOff>241200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8589,12 +8589,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6219720"/>
-          <a:ext cx="2354760" cy="194040"/>
+          <a:ext cx="2354400" cy="193680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8610,9 +8610,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>80640</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>242640</xdr:rowOff>
+      <xdr:rowOff>242280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8622,18 +8622,17 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6531480"/>
-          <a:ext cx="2667600" cy="192960"/>
+          <a:ext cx="2667240" cy="192600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:blipFill rotWithShape="0">
           <a:blip r:embed="rId7"/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
+          <a:srcRect/>
+          <a:stretch/>
         </a:blipFill>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8991,9 +8990,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>280440</xdr:colOff>
+      <xdr:colOff>280080</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9003,7 +9002,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1978200" y="78480"/>
-          <a:ext cx="6966720" cy="10488240"/>
+          <a:ext cx="6966360" cy="10487880"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9132,8 +9131,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10758,14 +10757,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A9:A11" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A9:A11" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -10781,8 +10780,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12968,8 +12967,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -12984,8 +12983,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14879,70 +14878,70 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4" type="custom">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4" type="custom">
       <formula1>OR(ISNUMBER(C52),C52="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E10" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E10" type="none">
       <formula1>OR(ISNUMBER(F12),F12="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E11 E13:E14" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E11 E13:E14" type="none">
       <formula1>OR(ISNUMBER(F13),F13="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F15" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F15" type="none">
       <formula1>OR(ISNUMBER(G17),G17="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G15" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G15" type="none">
       <formula1>OR(ISNUMBER(H17),H17="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D19:D21 E20 D22:D26" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D19:D21 E20 D22:D26" type="none">
       <formula1>OR(ISNUMBER(E12),E12="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E19:F19 F20:F26 E21:E26" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E19:F19 F20:F26 E21:E26" type="none">
       <formula1>OR(ISNUMBER(F12),F12="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D33:F33" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D33:F33" type="none">
       <formula1>OR(ISNUMBER(F48),F48="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D34:E34" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D34:E34" type="none">
       <formula1>OR(ISNUMBER(F49),F49="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D35:E35" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D35:E35" type="none">
       <formula1>OR(ISNUMBER(F50),F50="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G33" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G33" type="none">
       <formula1>OR(ISNUMBER(H48),H48="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E36" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E36" type="none">
       <formula1>OR(ISNUMBER(F39),F39="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D43:G44" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D43:G44" type="none">
       <formula1>OR(ISNUMBER(E7),E7="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D50:E51" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D50:E51" type="none">
       <formula1>OR(ISNUMBER(E14),E14="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D55:E55 D59:E59 D63:G65" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D55:E55 D59:E59 D63:G65" type="none">
       <formula1>OR(ISNUMBER(E40),E40="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="0" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="0" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14957,8 +14956,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15287,23 +15286,23 @@
       </c>
       <c r="B19" s="173"/>
       <c r="C19" s="274" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D19" s="243" t="str">
-        <f aca="false">A15</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine]</v>
+        <f aca="false">A23</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine]</v>
       </c>
       <c r="E19" s="273" t="str">
-        <f aca="false">A16</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-kerroin]</v>
+        <f aca="false">A24</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-kerroin]</v>
       </c>
       <c r="F19" s="243" t="str">
-        <f aca="false">A17</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-kertoimella]</v>
+        <f aca="false">A25</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-kertoimella]</v>
       </c>
       <c r="G19" s="243" t="str">
-        <f aca="false">A18</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-nettoala-kertoimella]</v>
+        <f aca="false">A26</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-nettoala-kertoimella]</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15311,24 +15310,24 @@
         <v>88</v>
       </c>
       <c r="B20" s="173"/>
-      <c r="C20" s="274" t="s">
-        <v>75</v>
+      <c r="C20" s="275" t="s">
+        <v>73</v>
       </c>
       <c r="D20" s="243" t="str">
-        <f aca="false">A19</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys]</v>
+        <f aca="false">A15</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine]</v>
       </c>
       <c r="E20" s="273" t="str">
-        <f aca="false">A20</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-kerroin]</v>
+        <f aca="false">A16</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-kerroin]</v>
       </c>
       <c r="F20" s="243" t="str">
-        <f aca="false">A21</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-kertoimella]</v>
+        <f aca="false">A17</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-kertoimella]</v>
       </c>
       <c r="G20" s="243" t="str">
-        <f aca="false">A22</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-nettoala-kertoimella]</v>
+        <f aca="false">A18</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-nettoala-kertoimella]</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15337,23 +15336,23 @@
       </c>
       <c r="B21" s="173"/>
       <c r="C21" s="275" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D21" s="243" t="str">
-        <f aca="false">A23</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine]</v>
+        <f aca="false">A19</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys]</v>
       </c>
       <c r="E21" s="273" t="str">
-        <f aca="false">A24</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-kerroin]</v>
+        <f aca="false">A20</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-kerroin]</v>
       </c>
       <c r="F21" s="243" t="str">
-        <f aca="false">A25</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-kertoimella]</v>
+        <f aca="false">A21</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-kertoimella]</v>
       </c>
       <c r="G21" s="243" t="str">
-        <f aca="false">A26</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-nettoala-kertoimella]</v>
+        <f aca="false">A22</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-nettoala-kertoimella]</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16438,7 +16437,7 @@
       <formula>"Täytä lähtötietoihin!"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:D4 E7 C7 C9 E18:F22 D21:G21 E17:F21 G17:G20 G22 D18:D20 D22 F28:F33 F54:F57 F66:F70">
+  <conditionalFormatting sqref="C4:D4 E7 C7 C9 E22:F22 E17:F18 G17:G18 G22 D18 D22 F28:F33 F54:F57 F66:F70 D19:G21">
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139">
       <formula>"*"</formula>
     </cfRule>
@@ -16511,42 +16510,42 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154">
-      <formula>LEFT(C21,1)="*"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155">
+    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C33">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156">
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155">
       <formula>LEFT(C32,1)="*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
+    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38">
     <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
+  <conditionalFormatting sqref="C47:C48">
     <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47:C48">
+  <conditionalFormatting sqref="C40:C46">
     <cfRule type="cellIs" priority="23" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:C46">
+  <conditionalFormatting sqref="F47:F48">
     <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F47:F48">
+  <conditionalFormatting sqref="G47:G48">
     <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
       <formula>"*"</formula>
     </cfRule>
@@ -16556,112 +16555,112 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47:G48">
+  <conditionalFormatting sqref="F40">
     <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
+  <conditionalFormatting sqref="G40">
     <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
+  <conditionalFormatting sqref="G41">
     <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
+  <conditionalFormatting sqref="G44">
     <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G44">
+  <conditionalFormatting sqref="F44">
     <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F44">
+  <conditionalFormatting sqref="F46">
     <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F46">
+  <conditionalFormatting sqref="G46">
     <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
+  <conditionalFormatting sqref="G42:G43">
     <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G42:G43">
+  <conditionalFormatting sqref="G58:G59">
     <cfRule type="cellIs" priority="35" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G58:G59">
+      <formula>"Täytä lähtötietoihin!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53 F58">
     <cfRule type="cellIs" priority="36" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F53 E52">
+    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="cellIs" priority="39" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F65">
+    <cfRule type="cellIs" priority="40" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F52">
+    <cfRule type="cellIs" priority="41" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C58">
+    <cfRule type="cellIs" priority="42" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:C60">
+    <cfRule type="cellIs" priority="43" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62:G63 D71:G71">
+    <cfRule type="cellIs" priority="44" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180">
       <formula>"Täytä lähtötietoihin!"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E53 F58">
-    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
-    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F53 E52">
-    <cfRule type="cellIs" priority="39" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
-    <cfRule type="cellIs" priority="40" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F65">
-    <cfRule type="cellIs" priority="41" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F52">
-    <cfRule type="cellIs" priority="42" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C58">
-    <cfRule type="cellIs" priority="43" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59:C60">
-    <cfRule type="cellIs" priority="44" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B62:G63 D71:G71">
+  <conditionalFormatting sqref="C71">
     <cfRule type="cellIs" priority="45" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181">
-      <formula>"Täytä lähtötietoihin!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
     <cfRule type="cellIs" priority="46" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
+  <conditionalFormatting sqref="C66:C68 C70">
     <cfRule type="cellIs" priority="47" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C66:C68 C70">
+  <conditionalFormatting sqref="E74">
     <cfRule type="cellIs" priority="48" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184">
       <formula>"*"</formula>
     </cfRule>
@@ -16671,203 +16670,203 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
+  <conditionalFormatting sqref="C74">
     <cfRule type="cellIs" priority="50" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C74">
+  <conditionalFormatting sqref="C17:C18">
     <cfRule type="cellIs" priority="51" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17:C18">
-    <cfRule type="cellIs" priority="52" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188">
       <formula>"- Valitse -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:C20">
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188">
+      <formula>LEFT(C30,1)="*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
     <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189">
-      <formula>LEFT(C19,1)="*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190">
-      <formula>LEFT(C30,1)="*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191">
       <formula>LEFT(C31,1)="*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:C29">
+    <cfRule type="cellIs" priority="54" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190">
+      <formula>"tyhjä"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="55" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191">
+      <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C29">
     <cfRule type="cellIs" priority="56" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192">
-      <formula>"tyhjä"</formula>
-    </cfRule>
+      <formula>"- Valitse -"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
     <cfRule type="cellIs" priority="57" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C29">
+  <conditionalFormatting sqref="D16">
     <cfRule type="cellIs" priority="58" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194">
-      <formula>"- Valitse -"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
     <cfRule type="cellIs" priority="59" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
+  <conditionalFormatting sqref="G28:G33">
     <cfRule type="cellIs" priority="60" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
+  <conditionalFormatting sqref="G28:G33">
     <cfRule type="cellIs" priority="61" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28:G33">
+  <conditionalFormatting sqref="G64:G65">
     <cfRule type="cellIs" priority="62" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28:G33">
+  <conditionalFormatting sqref="G66:G70">
     <cfRule type="cellIs" priority="63" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G64:G65">
+  <conditionalFormatting sqref="G53 G55 G57">
     <cfRule type="cellIs" priority="64" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G66:G70">
+  <conditionalFormatting sqref="G52 G54 G56">
     <cfRule type="cellIs" priority="65" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G53 G55 G57">
+  <conditionalFormatting sqref="D7">
     <cfRule type="cellIs" priority="66" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G52 G54 G56">
+  <conditionalFormatting sqref="D4 D7">
     <cfRule type="cellIs" priority="67" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
+      <formula>"Täytä etusivulle!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C69">
     <cfRule type="cellIs" priority="68" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4 D7">
+  <conditionalFormatting sqref="F47:G47">
     <cfRule type="cellIs" priority="69" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205">
-      <formula>"Täytä etusivulle!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C69">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66:E70">
     <cfRule type="cellIs" priority="70" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F47:G47">
+  <conditionalFormatting sqref="D17">
     <cfRule type="cellIs" priority="71" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E66:E70">
+  <conditionalFormatting sqref="E28">
     <cfRule type="cellIs" priority="72" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
+  <conditionalFormatting sqref="E29:E33">
     <cfRule type="cellIs" priority="73" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
+  <conditionalFormatting sqref="E42:E46">
     <cfRule type="cellIs" priority="74" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29:E33">
+  <conditionalFormatting sqref="F41:F43">
     <cfRule type="cellIs" priority="75" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42:E46">
+  <conditionalFormatting sqref="F45">
     <cfRule type="cellIs" priority="76" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41:F43">
+  <conditionalFormatting sqref="G45">
     <cfRule type="cellIs" priority="77" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
+  <conditionalFormatting sqref="E54:E57">
     <cfRule type="cellIs" priority="78" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
+  <conditionalFormatting sqref="C8">
     <cfRule type="cellIs" priority="79" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E54:E57">
+  <conditionalFormatting sqref="F38">
     <cfRule type="cellIs" priority="80" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
+  <conditionalFormatting sqref="G38">
     <cfRule type="cellIs" priority="81" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38">
+  <conditionalFormatting sqref="E64">
     <cfRule type="cellIs" priority="82" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G38">
+  <conditionalFormatting sqref="F64">
     <cfRule type="cellIs" priority="83" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E64">
-    <cfRule type="cellIs" priority="84" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F64">
-    <cfRule type="cellIs" priority="85" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" priority="86" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="84" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" priority="87" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222">
-      <formula>"*"</formula>
+    <cfRule type="cellIs" priority="85" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:C21">
+    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221">
+      <formula>LEFT(C21,1)="*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222">
+      <formula>LEFT(C19,1)="*"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A40:D49 F40:AMJ40 E41:AMJ49" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A40:D49 F40:AMJ40 E41:AMJ49" type="none">
       <formula1>OR(ISNUMBER(#ref!),#ref!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -16882,7 +16881,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -18598,14 +18597,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A6:B55 D6:AMJ6 D7 F7:AMJ7 C8:AMJ38 C39:H47 K39:AMJ39 I40:AMJ47 C48:AMJ55" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A6:B55 D6:AMJ6 D7 F7:AMJ7 C8:AMJ38 C39:H47 K39:AMJ39 I40:AMJ47 C48:AMJ55" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -18620,7 +18619,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -19637,8 +19636,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -19653,7 +19652,7 @@
   </sheetPr>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
     </sheetView>
   </sheetViews>
@@ -20502,8 +20501,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -20518,7 +20517,7 @@
   </sheetPr>
   <dimension ref="A1:Q140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -22042,8 +22041,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>